<commit_message>
Development of the dog endpoints
</commit_message>
<xml_diff>
--- a/documentation/planning/planning_effectif_travail_de_diplome.xlsx
+++ b/documentation/planning/planning_effectif_travail_de_diplome.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bj-travail-diplome-2021\documentation\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C78ECCA-5964-4A4B-829C-6082E00CCD6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -279,7 +278,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\.m"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -1136,7 +1135,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1144,7 +1143,7 @@
   <dimension ref="A1:BT41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1587,7 +1586,9 @@
       <c r="G5" s="56">
         <v>2</v>
       </c>
-      <c r="H5" s="56"/>
+      <c r="H5" s="56">
+        <v>4</v>
+      </c>
       <c r="I5" s="56"/>
       <c r="J5" s="56"/>
       <c r="K5" s="56"/>
@@ -1624,7 +1625,7 @@
       <c r="AP5" s="60"/>
       <c r="AQ5" s="20">
         <f t="shared" ref="AQ5:AQ12" si="0">SUM(C5:AP5)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AR5" s="73"/>
       <c r="AS5" s="69"/>
@@ -1645,7 +1646,9 @@
       <c r="G6" s="57">
         <v>1</v>
       </c>
-      <c r="H6" s="57"/>
+      <c r="H6" s="57">
+        <v>2</v>
+      </c>
       <c r="I6" s="56"/>
       <c r="J6" s="56"/>
       <c r="K6" s="56"/>
@@ -1682,7 +1685,7 @@
       <c r="AP6" s="60"/>
       <c r="AQ6" s="20">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AR6" s="74" t="s">
         <v>64</v>
@@ -3823,7 +3826,7 @@
     </row>
     <row r="41" spans="1:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="22">
-        <f t="shared" ref="B41:AQ41" si="4">SUM(B4:B40)</f>
+        <f t="shared" ref="B41:AP41" si="4">SUM(B4:B40)</f>
         <v>300</v>
       </c>
       <c r="C41">
@@ -3848,7 +3851,7 @@
       </c>
       <c r="H41" s="22">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I41" s="22">
         <f t="shared" si="4"/>
@@ -3988,7 +3991,7 @@
       </c>
       <c r="AQ41" s="22">
         <f>SUM(AQ4:AQ40)</f>
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="AR41" s="49"/>
       <c r="AS41" s="49"/>

</xml_diff>

<commit_message>
Start of development of the appoitment endpoint
</commit_message>
<xml_diff>
--- a/documentation/planning/planning_effectif_travail_de_diplome.xlsx
+++ b/documentation/planning/planning_effectif_travail_de_diplome.xlsx
@@ -1855,7 +1855,9 @@
       <c r="J9" s="56"/>
       <c r="K9" s="56"/>
       <c r="L9" s="56"/>
-      <c r="M9" s="56"/>
+      <c r="M9" s="56">
+        <v>2</v>
+      </c>
       <c r="N9" s="56"/>
       <c r="O9" s="58"/>
       <c r="P9" s="58"/>
@@ -1887,7 +1889,7 @@
       <c r="AP9" s="60"/>
       <c r="AQ9" s="20">
         <f>SUM(C9:AP9)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AR9" s="67"/>
       <c r="AS9" s="67"/>
@@ -1915,7 +1917,9 @@
       <c r="J10" s="56"/>
       <c r="K10" s="56"/>
       <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
+      <c r="M10" s="56">
+        <v>1</v>
+      </c>
       <c r="N10" s="56"/>
       <c r="O10" s="58"/>
       <c r="P10" s="58"/>
@@ -1947,7 +1951,7 @@
       <c r="AP10" s="60"/>
       <c r="AQ10" s="20">
         <f>SUM(C10:AP10)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AR10" s="67"/>
       <c r="AS10" s="67"/>
@@ -1975,7 +1979,9 @@
       <c r="J11" s="56"/>
       <c r="K11" s="56"/>
       <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
+      <c r="M11" s="56">
+        <v>2</v>
+      </c>
       <c r="N11" s="56"/>
       <c r="O11" s="58"/>
       <c r="P11" s="58"/>
@@ -2007,7 +2013,7 @@
       <c r="AP11" s="60"/>
       <c r="AQ11" s="20">
         <f t="shared" ref="AQ11" si="1">SUM(C11:AP11)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AR11" s="67"/>
       <c r="AS11" s="67"/>
@@ -2035,7 +2041,9 @@
       <c r="J12" s="56"/>
       <c r="K12" s="56"/>
       <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
+      <c r="M12" s="56">
+        <v>1</v>
+      </c>
       <c r="N12" s="56"/>
       <c r="O12" s="58"/>
       <c r="P12" s="58"/>
@@ -2067,7 +2075,7 @@
       <c r="AP12" s="60"/>
       <c r="AQ12" s="20">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AR12" s="67"/>
       <c r="AS12" s="67"/>
@@ -3951,7 +3959,7 @@
       </c>
       <c r="M42" s="22">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N42">
         <f t="shared" si="4"/>
@@ -4071,7 +4079,7 @@
       </c>
       <c r="AQ42" s="22">
         <f>SUM(AQ4:AQ41)</f>
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="AR42" s="49"/>
       <c r="AS42" s="49"/>

</xml_diff>

<commit_message>
Development of about, home and agenda views
</commit_message>
<xml_diff>
--- a/documentation/planning/planning_effectif_travail_de_diplome.xlsx
+++ b/documentation/planning/planning_effectif_travail_de_diplome.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bj-travail-diplome-2021\documentation\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAD3924-31F7-49FA-8FF9-C744BECA2009}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -276,12 +277,24 @@
   </si>
   <si>
     <t>Documentation technique</t>
+  </si>
+  <si>
+    <t>Invité</t>
+  </si>
+  <si>
+    <t>Onglet à propos</t>
+  </si>
+  <si>
+    <t>Onglet accueil</t>
+  </si>
+  <si>
+    <t>Onglet agenda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\.m"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -824,7 +837,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1145,15 +1193,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BT42"/>
+  <dimension ref="A1:BT46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2164,7 +2212,7 @@
     </row>
     <row r="14" spans="1:72" s="40" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="45" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="B14" s="41"/>
       <c r="C14" s="64"/>
@@ -2240,7 +2288,7 @@
     </row>
     <row r="15" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="B15" s="20">
         <v>4</v>
@@ -2260,7 +2308,9 @@
       <c r="O15" s="58"/>
       <c r="P15" s="58"/>
       <c r="Q15" s="58"/>
-      <c r="R15" s="58"/>
+      <c r="R15" s="58">
+        <v>2</v>
+      </c>
       <c r="S15" s="58"/>
       <c r="T15" s="58"/>
       <c r="U15" s="59"/>
@@ -2287,14 +2337,14 @@
       <c r="AP15" s="60"/>
       <c r="AQ15" s="20">
         <f>SUM(C15:AP15)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR15" s="49"/>
       <c r="AS15" s="49"/>
     </row>
     <row r="16" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="B16" s="20">
         <v>4</v>
@@ -2314,7 +2364,9 @@
       <c r="O16" s="58"/>
       <c r="P16" s="58"/>
       <c r="Q16" s="58"/>
-      <c r="R16" s="58"/>
+      <c r="R16" s="58">
+        <v>2</v>
+      </c>
       <c r="S16" s="58"/>
       <c r="T16" s="58"/>
       <c r="U16" s="59"/>
@@ -2341,17 +2393,17 @@
       <c r="AP16" s="60"/>
       <c r="AQ16" s="20">
         <f>SUM(C16:AP16)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR16" s="49"/>
       <c r="AS16" s="49"/>
     </row>
     <row r="17" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>47</v>
+      <c r="A17" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="B17" s="20">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C17" s="65"/>
       <c r="D17" s="58"/>
@@ -2369,7 +2421,9 @@
       <c r="P17" s="58"/>
       <c r="Q17" s="58"/>
       <c r="R17" s="58"/>
-      <c r="S17" s="58"/>
+      <c r="S17" s="58">
+        <v>6</v>
+      </c>
       <c r="T17" s="58"/>
       <c r="U17" s="59"/>
       <c r="V17" s="58"/>
@@ -2395,144 +2449,144 @@
       <c r="AP17" s="60"/>
       <c r="AQ17" s="20">
         <f>SUM(C17:AP17)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AR17" s="49"/>
       <c r="AS17" s="49"/>
     </row>
-    <row r="18" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="20">
-        <v>8</v>
-      </c>
-      <c r="C18" s="65"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="58"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="58"/>
-      <c r="O18" s="58"/>
-      <c r="P18" s="58"/>
-      <c r="Q18" s="58"/>
-      <c r="R18" s="58"/>
-      <c r="S18" s="58"/>
-      <c r="T18" s="58"/>
+    <row r="18" spans="1:72" s="40" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="41"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="59"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="59"/>
+      <c r="R18" s="59"/>
+      <c r="S18" s="59"/>
+      <c r="T18" s="59"/>
       <c r="U18" s="59"/>
-      <c r="V18" s="58"/>
-      <c r="W18" s="58"/>
-      <c r="X18" s="58"/>
-      <c r="Y18" s="58"/>
-      <c r="Z18" s="58"/>
-      <c r="AA18" s="58"/>
+      <c r="V18" s="59"/>
+      <c r="W18" s="59"/>
+      <c r="X18" s="59"/>
+      <c r="Y18" s="59"/>
+      <c r="Z18" s="59"/>
+      <c r="AA18" s="59"/>
       <c r="AB18" s="59"/>
-      <c r="AC18" s="58"/>
-      <c r="AD18" s="58"/>
-      <c r="AE18" s="58"/>
-      <c r="AF18" s="58"/>
-      <c r="AG18" s="58"/>
-      <c r="AH18" s="58"/>
-      <c r="AI18" s="58"/>
-      <c r="AJ18" s="58"/>
-      <c r="AK18" s="58"/>
-      <c r="AL18" s="58"/>
-      <c r="AM18" s="58"/>
-      <c r="AN18" s="58"/>
-      <c r="AO18" s="58"/>
-      <c r="AP18" s="60"/>
-      <c r="AQ18" s="20">
-        <f>SUM(C18:AP18)</f>
-        <v>0</v>
-      </c>
+      <c r="AC18" s="59"/>
+      <c r="AD18" s="59"/>
+      <c r="AE18" s="59"/>
+      <c r="AF18" s="59"/>
+      <c r="AG18" s="59"/>
+      <c r="AH18" s="59"/>
+      <c r="AI18" s="59"/>
+      <c r="AJ18" s="59"/>
+      <c r="AK18" s="59"/>
+      <c r="AL18" s="59"/>
+      <c r="AM18" s="59"/>
+      <c r="AN18" s="59"/>
+      <c r="AO18" s="59"/>
+      <c r="AP18" s="63"/>
+      <c r="AQ18" s="41"/>
       <c r="AR18" s="49"/>
       <c r="AS18" s="49"/>
+      <c r="AT18" s="2"/>
+      <c r="AU18" s="2"/>
+      <c r="AV18" s="2"/>
+      <c r="AW18" s="2"/>
+      <c r="AX18" s="2"/>
+      <c r="AY18"/>
+      <c r="AZ18"/>
+      <c r="BA18"/>
+      <c r="BB18"/>
+      <c r="BC18"/>
+      <c r="BD18"/>
+      <c r="BE18"/>
+      <c r="BF18"/>
+      <c r="BG18"/>
+      <c r="BH18"/>
+      <c r="BI18"/>
+      <c r="BJ18"/>
+      <c r="BK18"/>
+      <c r="BL18"/>
+      <c r="BM18"/>
+      <c r="BN18"/>
+      <c r="BO18"/>
+      <c r="BP18"/>
+      <c r="BQ18"/>
+      <c r="BR18"/>
+      <c r="BS18"/>
+      <c r="BT18"/>
     </row>
-    <row r="19" spans="1:72" s="40" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="59"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="59"/>
-      <c r="Q19" s="59"/>
-      <c r="R19" s="59"/>
-      <c r="S19" s="59"/>
-      <c r="T19" s="59"/>
+    <row r="19" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="20">
+        <v>4</v>
+      </c>
+      <c r="C19" s="65"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="58"/>
+      <c r="Q19" s="58"/>
+      <c r="R19" s="58"/>
+      <c r="S19" s="58"/>
+      <c r="T19" s="58"/>
       <c r="U19" s="59"/>
-      <c r="V19" s="59"/>
-      <c r="W19" s="59"/>
-      <c r="X19" s="59"/>
-      <c r="Y19" s="59"/>
-      <c r="Z19" s="59"/>
-      <c r="AA19" s="59"/>
+      <c r="V19" s="58"/>
+      <c r="W19" s="58"/>
+      <c r="X19" s="58"/>
+      <c r="Y19" s="58"/>
+      <c r="Z19" s="58"/>
+      <c r="AA19" s="58"/>
       <c r="AB19" s="59"/>
-      <c r="AC19" s="59"/>
-      <c r="AD19" s="59"/>
-      <c r="AE19" s="59"/>
-      <c r="AF19" s="59"/>
-      <c r="AG19" s="59"/>
-      <c r="AH19" s="59"/>
-      <c r="AI19" s="59"/>
-      <c r="AJ19" s="59"/>
-      <c r="AK19" s="59"/>
-      <c r="AL19" s="59"/>
-      <c r="AM19" s="59"/>
-      <c r="AN19" s="59"/>
-      <c r="AO19" s="59"/>
-      <c r="AP19" s="63"/>
-      <c r="AQ19" s="41"/>
+      <c r="AC19" s="58"/>
+      <c r="AD19" s="58"/>
+      <c r="AE19" s="58"/>
+      <c r="AF19" s="58"/>
+      <c r="AG19" s="58"/>
+      <c r="AH19" s="58"/>
+      <c r="AI19" s="58"/>
+      <c r="AJ19" s="58"/>
+      <c r="AK19" s="58"/>
+      <c r="AL19" s="58"/>
+      <c r="AM19" s="58"/>
+      <c r="AN19" s="58"/>
+      <c r="AO19" s="58"/>
+      <c r="AP19" s="60"/>
+      <c r="AQ19" s="20">
+        <f>SUM(C19:AP19)</f>
+        <v>0</v>
+      </c>
       <c r="AR19" s="49"/>
       <c r="AS19" s="49"/>
-      <c r="AT19" s="2"/>
-      <c r="AU19" s="2"/>
-      <c r="AV19" s="2"/>
-      <c r="AW19" s="2"/>
-      <c r="AX19" s="2"/>
-      <c r="AY19"/>
-      <c r="AZ19"/>
-      <c r="BA19"/>
-      <c r="BB19"/>
-      <c r="BC19"/>
-      <c r="BD19"/>
-      <c r="BE19"/>
-      <c r="BF19"/>
-      <c r="BG19"/>
-      <c r="BH19"/>
-      <c r="BI19"/>
-      <c r="BJ19"/>
-      <c r="BK19"/>
-      <c r="BL19"/>
-      <c r="BM19"/>
-      <c r="BN19"/>
-      <c r="BO19"/>
-      <c r="BP19"/>
-      <c r="BQ19"/>
-      <c r="BR19"/>
-      <c r="BS19"/>
-      <c r="BT19"/>
     </row>
     <row r="20" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>75</v>
+      <c r="A20" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="B20" s="20">
         <v>4</v>
@@ -2585,11 +2639,11 @@
       <c r="AS20" s="49"/>
     </row>
     <row r="21" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="20">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C21" s="65"/>
       <c r="D21" s="58"/>
@@ -2639,11 +2693,11 @@
       <c r="AS21" s="49"/>
     </row>
     <row r="22" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
-        <v>49</v>
+      <c r="A22" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="B22" s="20">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C22" s="65"/>
       <c r="D22" s="58"/>
@@ -2692,63 +2746,85 @@
       <c r="AR22" s="49"/>
       <c r="AS22" s="49"/>
     </row>
-    <row r="23" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="20">
-        <v>4</v>
-      </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="58"/>
-      <c r="K23" s="58"/>
-      <c r="L23" s="58"/>
-      <c r="M23" s="58"/>
-      <c r="N23" s="58"/>
-      <c r="O23" s="58"/>
-      <c r="P23" s="58"/>
-      <c r="Q23" s="58"/>
-      <c r="R23" s="58"/>
-      <c r="S23" s="58"/>
-      <c r="T23" s="58"/>
+    <row r="23" spans="1:72" s="40" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="41"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="59"/>
+      <c r="P23" s="59"/>
+      <c r="Q23" s="59"/>
+      <c r="R23" s="59"/>
+      <c r="S23" s="59"/>
+      <c r="T23" s="59"/>
       <c r="U23" s="59"/>
-      <c r="V23" s="58"/>
-      <c r="W23" s="58"/>
-      <c r="X23" s="58"/>
-      <c r="Y23" s="58"/>
-      <c r="Z23" s="58"/>
-      <c r="AA23" s="58"/>
+      <c r="V23" s="59"/>
+      <c r="W23" s="59"/>
+      <c r="X23" s="59"/>
+      <c r="Y23" s="59"/>
+      <c r="Z23" s="59"/>
+      <c r="AA23" s="59"/>
       <c r="AB23" s="59"/>
-      <c r="AC23" s="58"/>
-      <c r="AD23" s="58"/>
-      <c r="AE23" s="58"/>
-      <c r="AF23" s="58"/>
-      <c r="AG23" s="58"/>
-      <c r="AH23" s="58"/>
-      <c r="AI23" s="58"/>
-      <c r="AJ23" s="58"/>
-      <c r="AK23" s="58"/>
-      <c r="AL23" s="58"/>
-      <c r="AM23" s="58"/>
-      <c r="AN23" s="58"/>
-      <c r="AO23" s="58"/>
-      <c r="AP23" s="60"/>
-      <c r="AQ23" s="20">
-        <f>SUM(C23:AP23)</f>
-        <v>0</v>
-      </c>
+      <c r="AC23" s="59"/>
+      <c r="AD23" s="59"/>
+      <c r="AE23" s="59"/>
+      <c r="AF23" s="59"/>
+      <c r="AG23" s="59"/>
+      <c r="AH23" s="59"/>
+      <c r="AI23" s="59"/>
+      <c r="AJ23" s="59"/>
+      <c r="AK23" s="59"/>
+      <c r="AL23" s="59"/>
+      <c r="AM23" s="59"/>
+      <c r="AN23" s="59"/>
+      <c r="AO23" s="59"/>
+      <c r="AP23" s="63"/>
+      <c r="AQ23" s="41"/>
       <c r="AR23" s="49"/>
       <c r="AS23" s="49"/>
+      <c r="AT23" s="2"/>
+      <c r="AU23" s="2"/>
+      <c r="AV23" s="2"/>
+      <c r="AW23" s="2"/>
+      <c r="AX23" s="2"/>
+      <c r="AY23"/>
+      <c r="AZ23"/>
+      <c r="BA23"/>
+      <c r="BB23"/>
+      <c r="BC23"/>
+      <c r="BD23"/>
+      <c r="BE23"/>
+      <c r="BF23"/>
+      <c r="BG23"/>
+      <c r="BH23"/>
+      <c r="BI23"/>
+      <c r="BJ23"/>
+      <c r="BK23"/>
+      <c r="BL23"/>
+      <c r="BM23"/>
+      <c r="BN23"/>
+      <c r="BO23"/>
+      <c r="BP23"/>
+      <c r="BQ23"/>
+      <c r="BR23"/>
+      <c r="BS23"/>
+      <c r="BT23"/>
     </row>
     <row r="24" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B24" s="20">
         <v>4</v>
@@ -2802,7 +2878,7 @@
     </row>
     <row r="25" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="B25" s="20">
         <v>4</v>
@@ -2848,15 +2924,15 @@
       <c r="AO25" s="58"/>
       <c r="AP25" s="60"/>
       <c r="AQ25" s="20">
-        <f t="shared" ref="AQ25" si="2">SUM(C25:AP25)</f>
+        <f>SUM(C25:AP25)</f>
         <v>0</v>
       </c>
       <c r="AR25" s="49"/>
       <c r="AS25" s="49"/>
     </row>
-    <row r="26" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>77</v>
+    <row r="26" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="B26" s="20">
         <v>4</v>
@@ -2908,88 +2984,66 @@
       <c r="AR26" s="49"/>
       <c r="AS26" s="49"/>
     </row>
-    <row r="27" spans="1:72" s="40" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="41"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="59"/>
-      <c r="K27" s="59"/>
-      <c r="L27" s="59"/>
-      <c r="M27" s="59"/>
-      <c r="N27" s="59"/>
-      <c r="O27" s="59"/>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="59"/>
-      <c r="R27" s="59"/>
-      <c r="S27" s="59"/>
-      <c r="T27" s="59"/>
+    <row r="27" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="20">
+        <v>4</v>
+      </c>
+      <c r="C27" s="65"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="58"/>
+      <c r="J27" s="58"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="58"/>
+      <c r="N27" s="58"/>
+      <c r="O27" s="58"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="58"/>
+      <c r="R27" s="58"/>
+      <c r="S27" s="58"/>
+      <c r="T27" s="58"/>
       <c r="U27" s="59"/>
-      <c r="V27" s="59"/>
-      <c r="W27" s="59"/>
-      <c r="X27" s="59"/>
-      <c r="Y27" s="59"/>
-      <c r="Z27" s="59"/>
-      <c r="AA27" s="59"/>
+      <c r="V27" s="58"/>
+      <c r="W27" s="58"/>
+      <c r="X27" s="58"/>
+      <c r="Y27" s="58"/>
+      <c r="Z27" s="58"/>
+      <c r="AA27" s="58"/>
       <c r="AB27" s="59"/>
-      <c r="AC27" s="59"/>
-      <c r="AD27" s="59"/>
-      <c r="AE27" s="59"/>
-      <c r="AF27" s="59"/>
-      <c r="AG27" s="59"/>
-      <c r="AH27" s="59"/>
-      <c r="AI27" s="59"/>
-      <c r="AJ27" s="59"/>
-      <c r="AK27" s="59"/>
-      <c r="AL27" s="59"/>
-      <c r="AM27" s="59"/>
-      <c r="AN27" s="59"/>
-      <c r="AO27" s="59"/>
-      <c r="AP27" s="63"/>
-      <c r="AQ27" s="41"/>
+      <c r="AC27" s="58"/>
+      <c r="AD27" s="58"/>
+      <c r="AE27" s="58"/>
+      <c r="AF27" s="58"/>
+      <c r="AG27" s="58"/>
+      <c r="AH27" s="58"/>
+      <c r="AI27" s="58"/>
+      <c r="AJ27" s="58"/>
+      <c r="AK27" s="58"/>
+      <c r="AL27" s="58"/>
+      <c r="AM27" s="58"/>
+      <c r="AN27" s="58"/>
+      <c r="AO27" s="58"/>
+      <c r="AP27" s="60"/>
+      <c r="AQ27" s="20">
+        <f>SUM(C27:AP27)</f>
+        <v>0</v>
+      </c>
       <c r="AR27" s="49"/>
       <c r="AS27" s="49"/>
-      <c r="AT27" s="2"/>
-      <c r="AU27" s="2"/>
-      <c r="AV27" s="2"/>
-      <c r="AW27" s="2"/>
-      <c r="AX27" s="2"/>
-      <c r="AY27"/>
-      <c r="AZ27"/>
-      <c r="BA27"/>
-      <c r="BB27"/>
-      <c r="BC27"/>
-      <c r="BD27"/>
-      <c r="BE27"/>
-      <c r="BF27"/>
-      <c r="BG27"/>
-      <c r="BH27"/>
-      <c r="BI27"/>
-      <c r="BJ27"/>
-      <c r="BK27"/>
-      <c r="BL27"/>
-      <c r="BM27"/>
-      <c r="BN27"/>
-      <c r="BO27"/>
-      <c r="BP27"/>
-      <c r="BQ27"/>
-      <c r="BR27"/>
-      <c r="BS27"/>
-      <c r="BT27"/>
     </row>
     <row r="28" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B28" s="20">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C28" s="65"/>
       <c r="D28" s="58"/>
@@ -3032,7 +3086,7 @@
       <c r="AO28" s="58"/>
       <c r="AP28" s="60"/>
       <c r="AQ28" s="20">
-        <f t="shared" ref="AQ28:AQ37" si="3">SUM(C28:AP28)</f>
+        <f>SUM(C28:AP28)</f>
         <v>0</v>
       </c>
       <c r="AR28" s="49"/>
@@ -3040,10 +3094,10 @@
     </row>
     <row r="29" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="B29" s="20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C29" s="65"/>
       <c r="D29" s="58"/>
@@ -3086,18 +3140,18 @@
       <c r="AO29" s="58"/>
       <c r="AP29" s="60"/>
       <c r="AQ29" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AQ29" si="2">SUM(C29:AP29)</f>
         <v>0</v>
       </c>
       <c r="AR29" s="49"/>
       <c r="AS29" s="49"/>
     </row>
-    <row r="30" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>72</v>
+    <row r="30" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>77</v>
       </c>
       <c r="B30" s="20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C30" s="65"/>
       <c r="D30" s="58"/>
@@ -3140,72 +3194,94 @@
       <c r="AO30" s="58"/>
       <c r="AP30" s="60"/>
       <c r="AQ30" s="20">
-        <f t="shared" si="3"/>
+        <f>SUM(C30:AP30)</f>
         <v>0</v>
       </c>
       <c r="AR30" s="49"/>
       <c r="AS30" s="49"/>
     </row>
-    <row r="31" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="20">
-        <v>8</v>
-      </c>
-      <c r="C31" s="65"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
-      <c r="K31" s="58"/>
-      <c r="L31" s="58"/>
-      <c r="M31" s="58"/>
-      <c r="N31" s="58"/>
-      <c r="O31" s="58"/>
-      <c r="P31" s="58"/>
-      <c r="Q31" s="58"/>
-      <c r="R31" s="58"/>
-      <c r="S31" s="58"/>
-      <c r="T31" s="58"/>
+    <row r="31" spans="1:72" s="40" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="41"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="59"/>
+      <c r="J31" s="59"/>
+      <c r="K31" s="59"/>
+      <c r="L31" s="59"/>
+      <c r="M31" s="59"/>
+      <c r="N31" s="59"/>
+      <c r="O31" s="59"/>
+      <c r="P31" s="59"/>
+      <c r="Q31" s="59"/>
+      <c r="R31" s="59"/>
+      <c r="S31" s="59"/>
+      <c r="T31" s="59"/>
       <c r="U31" s="59"/>
-      <c r="V31" s="58"/>
-      <c r="W31" s="58"/>
-      <c r="X31" s="58"/>
-      <c r="Y31" s="58"/>
-      <c r="Z31" s="58"/>
-      <c r="AA31" s="58"/>
+      <c r="V31" s="59"/>
+      <c r="W31" s="59"/>
+      <c r="X31" s="59"/>
+      <c r="Y31" s="59"/>
+      <c r="Z31" s="59"/>
+      <c r="AA31" s="59"/>
       <c r="AB31" s="59"/>
-      <c r="AC31" s="58"/>
-      <c r="AD31" s="58"/>
-      <c r="AE31" s="58"/>
-      <c r="AF31" s="58"/>
-      <c r="AG31" s="58"/>
-      <c r="AH31" s="58"/>
-      <c r="AI31" s="58"/>
-      <c r="AJ31" s="58"/>
-      <c r="AK31" s="58"/>
-      <c r="AL31" s="58"/>
-      <c r="AM31" s="58"/>
-      <c r="AN31" s="58"/>
-      <c r="AO31" s="58"/>
-      <c r="AP31" s="60"/>
-      <c r="AQ31" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="AC31" s="59"/>
+      <c r="AD31" s="59"/>
+      <c r="AE31" s="59"/>
+      <c r="AF31" s="59"/>
+      <c r="AG31" s="59"/>
+      <c r="AH31" s="59"/>
+      <c r="AI31" s="59"/>
+      <c r="AJ31" s="59"/>
+      <c r="AK31" s="59"/>
+      <c r="AL31" s="59"/>
+      <c r="AM31" s="59"/>
+      <c r="AN31" s="59"/>
+      <c r="AO31" s="59"/>
+      <c r="AP31" s="63"/>
+      <c r="AQ31" s="41"/>
       <c r="AR31" s="49"/>
       <c r="AS31" s="49"/>
+      <c r="AT31" s="2"/>
+      <c r="AU31" s="2"/>
+      <c r="AV31" s="2"/>
+      <c r="AW31" s="2"/>
+      <c r="AX31" s="2"/>
+      <c r="AY31"/>
+      <c r="AZ31"/>
+      <c r="BA31"/>
+      <c r="BB31"/>
+      <c r="BC31"/>
+      <c r="BD31"/>
+      <c r="BE31"/>
+      <c r="BF31"/>
+      <c r="BG31"/>
+      <c r="BH31"/>
+      <c r="BI31"/>
+      <c r="BJ31"/>
+      <c r="BK31"/>
+      <c r="BL31"/>
+      <c r="BM31"/>
+      <c r="BN31"/>
+      <c r="BO31"/>
+      <c r="BP31"/>
+      <c r="BQ31"/>
+      <c r="BR31"/>
+      <c r="BS31"/>
+      <c r="BT31"/>
     </row>
     <row r="32" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B32" s="20">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C32" s="65"/>
       <c r="D32" s="58"/>
@@ -3248,7 +3324,7 @@
       <c r="AO32" s="58"/>
       <c r="AP32" s="60"/>
       <c r="AQ32" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AQ32:AQ41" si="3">SUM(C32:AP32)</f>
         <v>0</v>
       </c>
       <c r="AR32" s="49"/>
@@ -3256,10 +3332,10 @@
     </row>
     <row r="33" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B33" s="20">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C33" s="65"/>
       <c r="D33" s="58"/>
@@ -3310,10 +3386,10 @@
     </row>
     <row r="34" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="B34" s="20">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C34" s="65"/>
       <c r="D34" s="58"/>
@@ -3363,8 +3439,8 @@
       <c r="AS34" s="49"/>
     </row>
     <row r="35" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
-        <v>59</v>
+      <c r="A35" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="B35" s="20">
         <v>8</v>
@@ -3382,8 +3458,12 @@
       <c r="M35" s="58"/>
       <c r="N35" s="58"/>
       <c r="O35" s="58"/>
-      <c r="P35" s="58"/>
-      <c r="Q35" s="58"/>
+      <c r="P35" s="58">
+        <v>2</v>
+      </c>
+      <c r="Q35" s="58">
+        <v>4</v>
+      </c>
       <c r="R35" s="58"/>
       <c r="S35" s="58"/>
       <c r="T35" s="58"/>
@@ -3411,14 +3491,14 @@
       <c r="AP35" s="60"/>
       <c r="AQ35" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AR35" s="49"/>
       <c r="AS35" s="49"/>
     </row>
     <row r="36" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="B36" s="20">
         <v>16</v>
@@ -3470,12 +3550,12 @@
       <c r="AR36" s="49"/>
       <c r="AS36" s="49"/>
     </row>
-    <row r="37" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B37" s="20">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C37" s="65"/>
       <c r="D37" s="58"/>
@@ -3524,573 +3604,793 @@
       <c r="AR37" s="49"/>
       <c r="AS37" s="49"/>
     </row>
-    <row r="38" spans="1:72" s="40" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="41"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="39"/>
-      <c r="M38" s="39"/>
-      <c r="N38" s="39"/>
-      <c r="O38" s="39"/>
-      <c r="P38" s="39"/>
-      <c r="Q38" s="39"/>
-      <c r="R38" s="39"/>
-      <c r="S38" s="39"/>
-      <c r="T38" s="39"/>
-      <c r="U38" s="39"/>
-      <c r="V38" s="39"/>
-      <c r="W38" s="39"/>
-      <c r="X38" s="39"/>
-      <c r="Y38" s="39"/>
-      <c r="Z38" s="39"/>
-      <c r="AA38" s="39"/>
-      <c r="AB38" s="39"/>
-      <c r="AC38" s="39"/>
-      <c r="AD38" s="39"/>
-      <c r="AE38" s="39"/>
-      <c r="AF38" s="39"/>
-      <c r="AG38" s="39"/>
-      <c r="AH38" s="39"/>
-      <c r="AI38" s="39"/>
-      <c r="AJ38" s="39"/>
-      <c r="AK38" s="39"/>
-      <c r="AL38" s="39"/>
-      <c r="AM38" s="39"/>
-      <c r="AN38" s="39"/>
-      <c r="AO38" s="39"/>
-      <c r="AP38" s="52"/>
-      <c r="AQ38" s="54"/>
+    <row r="38" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="20">
+        <v>8</v>
+      </c>
+      <c r="C38" s="65"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="58"/>
+      <c r="J38" s="58"/>
+      <c r="K38" s="58"/>
+      <c r="L38" s="58"/>
+      <c r="M38" s="58"/>
+      <c r="N38" s="58"/>
+      <c r="O38" s="58"/>
+      <c r="P38" s="58"/>
+      <c r="Q38" s="58"/>
+      <c r="R38" s="58"/>
+      <c r="S38" s="58"/>
+      <c r="T38" s="58"/>
+      <c r="U38" s="59"/>
+      <c r="V38" s="58"/>
+      <c r="W38" s="58"/>
+      <c r="X38" s="58"/>
+      <c r="Y38" s="58"/>
+      <c r="Z38" s="58"/>
+      <c r="AA38" s="58"/>
+      <c r="AB38" s="59"/>
+      <c r="AC38" s="58"/>
+      <c r="AD38" s="58"/>
+      <c r="AE38" s="58"/>
+      <c r="AF38" s="58"/>
+      <c r="AG38" s="58"/>
+      <c r="AH38" s="58"/>
+      <c r="AI38" s="58"/>
+      <c r="AJ38" s="58"/>
+      <c r="AK38" s="58"/>
+      <c r="AL38" s="58"/>
+      <c r="AM38" s="58"/>
+      <c r="AN38" s="58"/>
+      <c r="AO38" s="58"/>
+      <c r="AP38" s="60"/>
+      <c r="AQ38" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="AR38" s="49"/>
       <c r="AS38" s="49"/>
-      <c r="AT38" s="2"/>
-      <c r="AU38" s="2"/>
-      <c r="AV38" s="2"/>
-      <c r="AW38" s="2"/>
-      <c r="AX38" s="2"/>
-      <c r="AY38"/>
-      <c r="AZ38"/>
-      <c r="BA38"/>
-      <c r="BB38"/>
-      <c r="BC38"/>
-      <c r="BD38"/>
-      <c r="BE38"/>
-      <c r="BF38"/>
-      <c r="BG38"/>
-      <c r="BH38"/>
-      <c r="BI38"/>
-      <c r="BJ38"/>
-      <c r="BK38"/>
-      <c r="BL38"/>
-      <c r="BM38"/>
-      <c r="BN38"/>
-      <c r="BO38"/>
-      <c r="BP38"/>
-      <c r="BQ38"/>
-      <c r="BR38"/>
-      <c r="BS38"/>
-      <c r="BT38"/>
     </row>
     <row r="39" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
-        <v>60</v>
+      <c r="A39" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="B39" s="20">
-        <v>68</v>
-      </c>
-      <c r="C39" s="4">
-        <v>1</v>
-      </c>
-      <c r="D39" s="1">
-        <v>1</v>
-      </c>
-      <c r="E39" s="1">
-        <v>1</v>
-      </c>
-      <c r="F39" s="1">
-        <v>1</v>
-      </c>
-      <c r="G39" s="1">
-        <v>1</v>
-      </c>
-      <c r="H39" s="1">
-        <v>1</v>
-      </c>
-      <c r="I39" s="1">
-        <v>1</v>
-      </c>
-      <c r="J39" s="1">
-        <v>1</v>
-      </c>
-      <c r="K39" s="1">
-        <v>1</v>
-      </c>
-      <c r="L39" s="1">
-        <v>1</v>
-      </c>
-      <c r="M39" s="1">
-        <v>1</v>
-      </c>
-      <c r="N39" s="1">
-        <v>1</v>
-      </c>
-      <c r="O39" s="1">
-        <v>1</v>
-      </c>
-      <c r="P39" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q39" s="1">
-        <v>1</v>
-      </c>
-      <c r="R39" s="1">
-        <v>1</v>
-      </c>
-      <c r="S39" s="1">
-        <v>1</v>
-      </c>
-      <c r="T39" s="1">
-        <v>1</v>
-      </c>
-      <c r="U39" s="39"/>
-      <c r="V39" s="1">
-        <v>1</v>
-      </c>
-      <c r="W39" s="1">
-        <v>1</v>
-      </c>
-      <c r="X39" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y39" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z39" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA39" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB39" s="39"/>
-      <c r="AC39" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD39" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE39" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF39" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG39" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH39" s="1">
-        <v>1</v>
-      </c>
-      <c r="AI39" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ39" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK39" s="1">
-        <v>5</v>
-      </c>
-      <c r="AL39" s="1">
-        <v>7</v>
-      </c>
-      <c r="AM39" s="1">
-        <v>7</v>
-      </c>
-      <c r="AN39" s="1">
-        <v>7</v>
-      </c>
-      <c r="AO39" s="1">
-        <v>7</v>
-      </c>
-      <c r="AP39" s="1">
-        <v>3</v>
-      </c>
-      <c r="AQ39" s="13">
-        <f>SUM(C39:AP39)</f>
-        <v>68</v>
+        <v>8</v>
+      </c>
+      <c r="C39" s="65"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="58"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
+      <c r="I39" s="58"/>
+      <c r="J39" s="58"/>
+      <c r="K39" s="58"/>
+      <c r="L39" s="58"/>
+      <c r="M39" s="58"/>
+      <c r="N39" s="58"/>
+      <c r="O39" s="58"/>
+      <c r="P39" s="58"/>
+      <c r="Q39" s="58"/>
+      <c r="R39" s="58"/>
+      <c r="S39" s="58"/>
+      <c r="T39" s="58"/>
+      <c r="U39" s="59"/>
+      <c r="V39" s="58"/>
+      <c r="W39" s="58"/>
+      <c r="X39" s="58"/>
+      <c r="Y39" s="58"/>
+      <c r="Z39" s="58"/>
+      <c r="AA39" s="58"/>
+      <c r="AB39" s="59"/>
+      <c r="AC39" s="58"/>
+      <c r="AD39" s="58"/>
+      <c r="AE39" s="58"/>
+      <c r="AF39" s="58"/>
+      <c r="AG39" s="58"/>
+      <c r="AH39" s="58"/>
+      <c r="AI39" s="58"/>
+      <c r="AJ39" s="58"/>
+      <c r="AK39" s="58"/>
+      <c r="AL39" s="58"/>
+      <c r="AM39" s="58"/>
+      <c r="AN39" s="58"/>
+      <c r="AO39" s="58"/>
+      <c r="AP39" s="60"/>
+      <c r="AQ39" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="AR39" s="49"/>
       <c r="AS39" s="49"/>
     </row>
     <row r="40" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
-        <v>83</v>
+      <c r="A40" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="B40" s="20">
-        <v>68</v>
-      </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1">
-        <v>4</v>
-      </c>
-      <c r="L40" s="1">
-        <v>4</v>
-      </c>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1">
-        <v>4</v>
-      </c>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
-      <c r="S40" s="1"/>
-      <c r="T40" s="1"/>
-      <c r="U40" s="39"/>
-      <c r="V40" s="1"/>
-      <c r="W40" s="1"/>
-      <c r="X40" s="1"/>
-      <c r="Y40" s="1"/>
-      <c r="Z40" s="1"/>
-      <c r="AA40" s="1"/>
-      <c r="AB40" s="39"/>
-      <c r="AC40" s="1"/>
-      <c r="AD40" s="1"/>
-      <c r="AE40" s="1"/>
-      <c r="AF40" s="1"/>
-      <c r="AG40" s="1"/>
-      <c r="AH40" s="1"/>
-      <c r="AI40" s="1"/>
-      <c r="AJ40" s="1"/>
-      <c r="AK40" s="1"/>
-      <c r="AL40" s="1"/>
-      <c r="AM40" s="1"/>
-      <c r="AN40" s="1"/>
-      <c r="AO40" s="1"/>
-      <c r="AP40" s="1"/>
-      <c r="AQ40" s="13">
-        <f>SUM(C40:AP40)</f>
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="C40" s="65"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="58"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="58"/>
+      <c r="J40" s="58"/>
+      <c r="K40" s="58"/>
+      <c r="L40" s="58"/>
+      <c r="M40" s="58"/>
+      <c r="N40" s="58"/>
+      <c r="O40" s="58"/>
+      <c r="P40" s="58"/>
+      <c r="Q40" s="58"/>
+      <c r="R40" s="58"/>
+      <c r="S40" s="58"/>
+      <c r="T40" s="58"/>
+      <c r="U40" s="59"/>
+      <c r="V40" s="58"/>
+      <c r="W40" s="58"/>
+      <c r="X40" s="58"/>
+      <c r="Y40" s="58"/>
+      <c r="Z40" s="58"/>
+      <c r="AA40" s="58"/>
+      <c r="AB40" s="59"/>
+      <c r="AC40" s="58"/>
+      <c r="AD40" s="58"/>
+      <c r="AE40" s="58"/>
+      <c r="AF40" s="58"/>
+      <c r="AG40" s="58"/>
+      <c r="AH40" s="58"/>
+      <c r="AI40" s="58"/>
+      <c r="AJ40" s="58"/>
+      <c r="AK40" s="58"/>
+      <c r="AL40" s="58"/>
+      <c r="AM40" s="58"/>
+      <c r="AN40" s="58"/>
+      <c r="AO40" s="58"/>
+      <c r="AP40" s="60"/>
+      <c r="AQ40" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="AR40" s="49"/>
       <c r="AS40" s="49"/>
     </row>
     <row r="41" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" s="21">
-        <v>38</v>
-      </c>
-      <c r="C41" s="4">
-        <v>1</v>
-      </c>
-      <c r="D41" s="1">
-        <v>1</v>
-      </c>
-      <c r="E41" s="1">
-        <v>1</v>
-      </c>
-      <c r="F41" s="1">
-        <v>1</v>
-      </c>
-      <c r="G41" s="1">
-        <v>1</v>
-      </c>
-      <c r="H41" s="1">
-        <v>1</v>
-      </c>
-      <c r="I41" s="1">
-        <v>1</v>
-      </c>
-      <c r="J41" s="1">
-        <v>1</v>
-      </c>
-      <c r="K41" s="1">
-        <v>1</v>
-      </c>
-      <c r="L41" s="1">
-        <v>1</v>
-      </c>
-      <c r="M41" s="1">
-        <v>1</v>
-      </c>
-      <c r="N41" s="1">
-        <v>1</v>
-      </c>
-      <c r="O41" s="1">
-        <v>1</v>
-      </c>
-      <c r="P41" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q41" s="1">
-        <v>1</v>
-      </c>
-      <c r="R41" s="1">
-        <v>1</v>
-      </c>
-      <c r="S41" s="1">
-        <v>1</v>
-      </c>
-      <c r="T41" s="1">
-        <v>1</v>
-      </c>
-      <c r="U41" s="39"/>
-      <c r="V41" s="1">
-        <v>1</v>
-      </c>
-      <c r="W41" s="1">
-        <v>1</v>
-      </c>
-      <c r="X41" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y41" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB41" s="39"/>
-      <c r="AC41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AI41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AL41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AM41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AN41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AO41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AP41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ41" s="14">
-        <f>SUM(C41:AP41)</f>
-        <v>38</v>
+      <c r="A41" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="20">
+        <v>10</v>
+      </c>
+      <c r="C41" s="65"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="58"/>
+      <c r="I41" s="58"/>
+      <c r="J41" s="58"/>
+      <c r="K41" s="58"/>
+      <c r="L41" s="58"/>
+      <c r="M41" s="58"/>
+      <c r="N41" s="58"/>
+      <c r="O41" s="58"/>
+      <c r="P41" s="58"/>
+      <c r="Q41" s="58"/>
+      <c r="R41" s="58"/>
+      <c r="S41" s="58"/>
+      <c r="T41" s="58"/>
+      <c r="U41" s="59"/>
+      <c r="V41" s="58"/>
+      <c r="W41" s="58"/>
+      <c r="X41" s="58"/>
+      <c r="Y41" s="58"/>
+      <c r="Z41" s="58"/>
+      <c r="AA41" s="58"/>
+      <c r="AB41" s="59"/>
+      <c r="AC41" s="58"/>
+      <c r="AD41" s="58"/>
+      <c r="AE41" s="58"/>
+      <c r="AF41" s="58"/>
+      <c r="AG41" s="58"/>
+      <c r="AH41" s="58"/>
+      <c r="AI41" s="58"/>
+      <c r="AJ41" s="58"/>
+      <c r="AK41" s="58"/>
+      <c r="AL41" s="58"/>
+      <c r="AM41" s="58"/>
+      <c r="AN41" s="58"/>
+      <c r="AO41" s="58"/>
+      <c r="AP41" s="60"/>
+      <c r="AQ41" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="AR41" s="49"/>
       <c r="AS41" s="49"/>
     </row>
-    <row r="42" spans="1:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="22">
-        <f t="shared" ref="B42:AP42" si="4">SUM(B4:B41)</f>
-        <v>368</v>
-      </c>
-      <c r="C42">
+    <row r="42" spans="1:72" s="40" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="41"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="39"/>
+      <c r="L42" s="39"/>
+      <c r="M42" s="39"/>
+      <c r="N42" s="39"/>
+      <c r="O42" s="39"/>
+      <c r="P42" s="39"/>
+      <c r="Q42" s="39"/>
+      <c r="R42" s="39"/>
+      <c r="S42" s="39"/>
+      <c r="T42" s="39"/>
+      <c r="U42" s="39"/>
+      <c r="V42" s="39"/>
+      <c r="W42" s="39"/>
+      <c r="X42" s="39"/>
+      <c r="Y42" s="39"/>
+      <c r="Z42" s="39"/>
+      <c r="AA42" s="39"/>
+      <c r="AB42" s="39"/>
+      <c r="AC42" s="39"/>
+      <c r="AD42" s="39"/>
+      <c r="AE42" s="39"/>
+      <c r="AF42" s="39"/>
+      <c r="AG42" s="39"/>
+      <c r="AH42" s="39"/>
+      <c r="AI42" s="39"/>
+      <c r="AJ42" s="39"/>
+      <c r="AK42" s="39"/>
+      <c r="AL42" s="39"/>
+      <c r="AM42" s="39"/>
+      <c r="AN42" s="39"/>
+      <c r="AO42" s="39"/>
+      <c r="AP42" s="52"/>
+      <c r="AQ42" s="54"/>
+      <c r="AR42" s="49"/>
+      <c r="AS42" s="49"/>
+      <c r="AT42" s="2"/>
+      <c r="AU42" s="2"/>
+      <c r="AV42" s="2"/>
+      <c r="AW42" s="2"/>
+      <c r="AX42" s="2"/>
+      <c r="AY42"/>
+      <c r="AZ42"/>
+      <c r="BA42"/>
+      <c r="BB42"/>
+      <c r="BC42"/>
+      <c r="BD42"/>
+      <c r="BE42"/>
+      <c r="BF42"/>
+      <c r="BG42"/>
+      <c r="BH42"/>
+      <c r="BI42"/>
+      <c r="BJ42"/>
+      <c r="BK42"/>
+      <c r="BL42"/>
+      <c r="BM42"/>
+      <c r="BN42"/>
+      <c r="BO42"/>
+      <c r="BP42"/>
+      <c r="BQ42"/>
+      <c r="BR42"/>
+      <c r="BS42"/>
+      <c r="BT42"/>
+    </row>
+    <row r="43" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="20">
+        <v>68</v>
+      </c>
+      <c r="C43" s="4">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1</v>
+      </c>
+      <c r="H43" s="1">
+        <v>1</v>
+      </c>
+      <c r="I43" s="1">
+        <v>1</v>
+      </c>
+      <c r="J43" s="1">
+        <v>1</v>
+      </c>
+      <c r="K43" s="1">
+        <v>1</v>
+      </c>
+      <c r="L43" s="1">
+        <v>1</v>
+      </c>
+      <c r="M43" s="1">
+        <v>1</v>
+      </c>
+      <c r="N43" s="1">
+        <v>1</v>
+      </c>
+      <c r="O43" s="1">
+        <v>1</v>
+      </c>
+      <c r="P43" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>1</v>
+      </c>
+      <c r="R43" s="1">
+        <v>3</v>
+      </c>
+      <c r="S43" s="1">
+        <v>1</v>
+      </c>
+      <c r="T43" s="1">
+        <v>1</v>
+      </c>
+      <c r="U43" s="39"/>
+      <c r="V43" s="1">
+        <v>1</v>
+      </c>
+      <c r="W43" s="1">
+        <v>1</v>
+      </c>
+      <c r="X43" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y43" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB43" s="39"/>
+      <c r="AC43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK43" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL43" s="1">
+        <v>7</v>
+      </c>
+      <c r="AM43" s="1">
+        <v>7</v>
+      </c>
+      <c r="AN43" s="1">
+        <v>7</v>
+      </c>
+      <c r="AO43" s="1">
+        <v>7</v>
+      </c>
+      <c r="AP43" s="1">
+        <v>3</v>
+      </c>
+      <c r="AQ43" s="13">
+        <f>SUM(C43:AP43)</f>
+        <v>70</v>
+      </c>
+      <c r="AR43" s="49"/>
+      <c r="AS43" s="49"/>
+    </row>
+    <row r="44" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="20">
+        <v>68</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1">
+        <v>4</v>
+      </c>
+      <c r="L44" s="1">
+        <v>4</v>
+      </c>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1">
+        <v>4</v>
+      </c>
+      <c r="P44" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>2</v>
+      </c>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="39"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+      <c r="Y44" s="1"/>
+      <c r="Z44" s="1"/>
+      <c r="AA44" s="1"/>
+      <c r="AB44" s="39"/>
+      <c r="AC44" s="1"/>
+      <c r="AD44" s="1"/>
+      <c r="AE44" s="1"/>
+      <c r="AF44" s="1"/>
+      <c r="AG44" s="1"/>
+      <c r="AH44" s="1"/>
+      <c r="AI44" s="1"/>
+      <c r="AJ44" s="1"/>
+      <c r="AK44" s="1"/>
+      <c r="AL44" s="1"/>
+      <c r="AM44" s="1"/>
+      <c r="AN44" s="1"/>
+      <c r="AO44" s="1"/>
+      <c r="AP44" s="1"/>
+      <c r="AQ44" s="13">
+        <f>SUM(C44:AP44)</f>
+        <v>18</v>
+      </c>
+      <c r="AR44" s="49"/>
+      <c r="AS44" s="49"/>
+    </row>
+    <row r="45" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="21">
+        <v>38</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+      <c r="G45" s="1">
+        <v>1</v>
+      </c>
+      <c r="H45" s="1">
+        <v>1</v>
+      </c>
+      <c r="I45" s="1">
+        <v>1</v>
+      </c>
+      <c r="J45" s="1">
+        <v>1</v>
+      </c>
+      <c r="K45" s="1">
+        <v>1</v>
+      </c>
+      <c r="L45" s="1">
+        <v>1</v>
+      </c>
+      <c r="M45" s="1">
+        <v>1</v>
+      </c>
+      <c r="N45" s="1">
+        <v>1</v>
+      </c>
+      <c r="O45" s="1">
+        <v>1</v>
+      </c>
+      <c r="P45" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>1</v>
+      </c>
+      <c r="R45" s="1">
+        <v>1</v>
+      </c>
+      <c r="S45" s="1">
+        <v>1</v>
+      </c>
+      <c r="T45" s="1">
+        <v>1</v>
+      </c>
+      <c r="U45" s="39"/>
+      <c r="V45" s="1">
+        <v>1</v>
+      </c>
+      <c r="W45" s="1">
+        <v>1</v>
+      </c>
+      <c r="X45" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y45" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB45" s="39"/>
+      <c r="AC45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ45" s="14">
+        <f>SUM(C45:AP45)</f>
+        <v>38</v>
+      </c>
+      <c r="AR45" s="49"/>
+      <c r="AS45" s="49"/>
+    </row>
+    <row r="46" spans="1:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="22">
+        <f t="shared" ref="B46:AP46" si="4">SUM(B4:B45)</f>
+        <v>380</v>
+      </c>
+      <c r="C46">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="D42" s="22">
+      <c r="D46" s="22">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="E42">
+      <c r="E46">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="F42" s="22">
+      <c r="F46" s="22">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="G42">
+      <c r="G46">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="H42" s="22">
+      <c r="H46" s="22">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="I42" s="22">
+      <c r="I46" s="22">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="J42">
+      <c r="J46">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="K42" s="22">
+      <c r="K46" s="22">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="L42">
+      <c r="L46">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="M42" s="22">
+      <c r="M46" s="22">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="N42">
+      <c r="N46">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="O42" s="22">
+      <c r="O46" s="22">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="P42" s="22">
+      <c r="P46" s="22">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="R46" s="22">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="T46" s="22">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="Q42">
+      <c r="U46">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V46" s="22">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="R42" s="22">
+      <c r="W46" s="22">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="S42">
+      <c r="X46">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="T42" s="22">
+      <c r="Y46" s="22">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="U42">
+      <c r="Z46">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="AA46" s="22">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="AB46">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V42" s="22">
+      <c r="AC46" s="22">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="W42" s="22">
+      <c r="AD46" s="22">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="X42">
+      <c r="AE46">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="Y42" s="22">
+      <c r="AF46" s="22">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="Z42">
+      <c r="AG46">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="AA42" s="22">
+      <c r="AH46" s="22">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="AB42">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AC42" s="22">
+      <c r="AI46">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="AD42" s="22">
+      <c r="AJ46" s="22">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="AE42">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AF42" s="22">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AG42">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AH42" s="22">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AI42">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AJ42" s="22">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AK42" s="22">
+      <c r="AK46" s="22">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="AL42">
+      <c r="AL46">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="AM42" s="22">
+      <c r="AM46" s="22">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="AN42">
+      <c r="AN46">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="AO42" s="22">
+      <c r="AO46" s="22">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="AP42">
+      <c r="AP46">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="AQ42" s="22">
-        <f>SUM(AQ4:AQ41)</f>
-        <v>184</v>
-      </c>
-      <c r="AR42" s="49"/>
-      <c r="AS42" s="49"/>
+      <c r="AQ46" s="22">
+        <f>SUM(AQ4:AQ45)</f>
+        <v>208</v>
+      </c>
+      <c r="AR46" s="49"/>
+      <c r="AS46" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4100,71 +4400,91 @@
     <mergeCell ref="AR6:AR7"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:N8 C10:N10 C12:N12">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="20">
       <formula>LEN(TRIM(C5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:AP8 C16:AP27 C31:AP39 C29:AP29 C10:AP10 C12:AP14 C41:AP41">
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="C5:AP8 C20:AP31 C35:AP43 C33:AP33 C10:AP10 C12:AP13 C45:AP45 C18:AP18">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42">
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
+  <conditionalFormatting sqref="B46">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
       <formula>300</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C42:AP42">
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+  <conditionalFormatting sqref="C46:AP46">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AP42">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+  <conditionalFormatting sqref="AP46">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:AP4">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19:AP19">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34:AP34">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:AP32">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:N9">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="9">
+      <formula>LEN(TRIM(C9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:AP9">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:N11">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="7">
+      <formula>LEN(TRIM(C11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:AP11">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44:AP44">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:AP17">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:AP14">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:AP15">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:AP30">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28:AP28">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:N9">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(C9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:AP9">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:N11">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(C11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:AP11">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40:AP40">
+  <conditionalFormatting sqref="C16:AP16">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
@@ -4176,7 +4496,7 @@
     <oddHeader>&amp;L&amp;F&amp;CDDC'App&amp;RJonathan Borel-Jaquet</oddHeader>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="AQ41 AQ25 AQ13:AQ14" formulaRange="1"/>
+    <ignoredError sqref="AQ45 AQ29 AQ18 AQ13" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Documentation and start of the development of the admin page
</commit_message>
<xml_diff>
--- a/documentation/planning/planning_effectif_travail_de_diplome.xlsx
+++ b/documentation/planning/planning_effectif_travail_de_diplome.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bj-travail-diplome-2021\documentation\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAD3924-31F7-49FA-8FF9-C744BECA2009}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C02D74A-4F3C-44CD-A358-B3B0F968A3BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Onglet agenda</t>
+  </si>
+  <si>
+    <t>Poster</t>
   </si>
 </sst>
 </file>
@@ -1198,10 +1201,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BT46"/>
+  <dimension ref="A1:BT47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3300,7 +3303,9 @@
       <c r="Q32" s="58"/>
       <c r="R32" s="58"/>
       <c r="S32" s="58"/>
-      <c r="T32" s="58"/>
+      <c r="T32" s="58">
+        <v>6</v>
+      </c>
       <c r="U32" s="59"/>
       <c r="V32" s="58"/>
       <c r="W32" s="58"/>
@@ -3325,7 +3330,7 @@
       <c r="AP32" s="60"/>
       <c r="AQ32" s="20">
         <f t="shared" ref="AQ32:AQ41" si="3">SUM(C32:AP32)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AR32" s="49"/>
       <c r="AS32" s="49"/>
@@ -4062,7 +4067,9 @@
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
       <c r="U44" s="39"/>
-      <c r="V44" s="1"/>
+      <c r="V44" s="1">
+        <v>3</v>
+      </c>
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
@@ -4085,12 +4092,12 @@
       <c r="AP44" s="1"/>
       <c r="AQ44" s="13">
         <f>SUM(C44:AP44)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="AR44" s="49"/>
       <c r="AS44" s="49"/>
     </row>
-    <row r="45" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:72" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
         <v>82</v>
       </c>
@@ -4220,177 +4227,233 @@
       <c r="AR45" s="49"/>
       <c r="AS45" s="49"/>
     </row>
-    <row r="46" spans="1:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="22">
-        <f t="shared" ref="B46:AP46" si="4">SUM(B4:B45)</f>
-        <v>380</v>
-      </c>
-      <c r="C46">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="D46" s="22">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="F46" s="22">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="G46">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="H46" s="22">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="I46" s="22">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="K46" s="22">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="L46">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="M46" s="22">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="N46">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="O46" s="22">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="P46" s="22">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="Q46">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="R46" s="22">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="S46">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="T46" s="22">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="U46">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V46" s="22">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="W46" s="22">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="X46">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="Y46" s="22">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="Z46">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AA46" s="22">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AB46">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AC46" s="22">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AD46" s="22">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AE46">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AF46" s="22">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AG46">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AH46" s="22">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AI46">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AJ46" s="22">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="AK46" s="22">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="AL46">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="AM46" s="22">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="AN46">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="AO46" s="22">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="AP46">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="AQ46" s="22">
-        <f>SUM(AQ4:AQ45)</f>
-        <v>208</v>
+    <row r="46" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="20">
+        <v>10</v>
+      </c>
+      <c r="C46" s="65"/>
+      <c r="D46" s="58"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="58"/>
+      <c r="J46" s="58"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
+      <c r="M46" s="58"/>
+      <c r="N46" s="58"/>
+      <c r="O46" s="58"/>
+      <c r="P46" s="58"/>
+      <c r="Q46" s="58"/>
+      <c r="R46" s="58"/>
+      <c r="S46" s="58"/>
+      <c r="T46" s="58"/>
+      <c r="U46" s="59"/>
+      <c r="V46" s="58">
+        <v>3</v>
+      </c>
+      <c r="W46" s="58"/>
+      <c r="X46" s="58"/>
+      <c r="Y46" s="58"/>
+      <c r="Z46" s="58"/>
+      <c r="AA46" s="58"/>
+      <c r="AB46" s="59"/>
+      <c r="AC46" s="58"/>
+      <c r="AD46" s="58"/>
+      <c r="AE46" s="58"/>
+      <c r="AF46" s="58"/>
+      <c r="AG46" s="58"/>
+      <c r="AH46" s="58"/>
+      <c r="AI46" s="58"/>
+      <c r="AJ46" s="58"/>
+      <c r="AK46" s="58"/>
+      <c r="AL46" s="58"/>
+      <c r="AM46" s="58"/>
+      <c r="AN46" s="58"/>
+      <c r="AO46" s="58"/>
+      <c r="AP46" s="60"/>
+      <c r="AQ46" s="20">
+        <f t="shared" ref="AQ46" si="4">SUM(C46:AP46)</f>
+        <v>3</v>
       </c>
       <c r="AR46" s="49"/>
       <c r="AS46" s="49"/>
+    </row>
+    <row r="47" spans="1:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="22">
+        <f t="shared" ref="B47:AP47" si="5">SUM(B4:B45)</f>
+        <v>380</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="D47" s="22">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="F47" s="22">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="H47" s="22">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="I47" s="22">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="K47" s="22">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="M47" s="22">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="O47" s="22">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="P47" s="22">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="R47" s="22">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="T47" s="22">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="U47">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V47" s="22">
+        <f>SUM(V4:V46)</f>
+        <v>8</v>
+      </c>
+      <c r="W47" s="22">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="X47">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Y47" s="22">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Z47">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AA47" s="22">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AB47">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AC47" s="22">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AD47" s="22">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AE47">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AF47" s="22">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AG47">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AH47" s="22">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AI47">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AJ47" s="22">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="AK47" s="22">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="AL47">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="AM47" s="22">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="AN47">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="AO47" s="22">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="AP47">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="AQ47" s="22">
+        <f>SUM(AQ4:AQ45)</f>
+        <v>217</v>
+      </c>
+      <c r="AR47" s="49"/>
+      <c r="AS47" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4400,91 +4463,96 @@
     <mergeCell ref="AR6:AR7"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:N8 C10:N10 C12:N12">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="21">
       <formula>LEN(TRIM(C5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:AP8 C20:AP31 C35:AP43 C33:AP33 C10:AP10 C12:AP13 C45:AP45 C18:AP18">
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+  <conditionalFormatting sqref="B47">
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
       <formula>300</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46:AP46">
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
+  <conditionalFormatting sqref="C47:AP47">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AP46">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+  <conditionalFormatting sqref="AP47">
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:AP4">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:AP19">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:AP34">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:AP32">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:N9">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
       <formula>LEN(TRIM(C9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:AP9">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:N11">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="7">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
       <formula>LEN(TRIM(C11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:AP11">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44:AP44">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:AP17">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:AP14">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:AP15">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:AP16">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46:AP46">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update log_book.md and planning
</commit_message>
<xml_diff>
--- a/documentation/planning/planning_effectif_travail_de_diplome.xlsx
+++ b/documentation/planning/planning_effectif_travail_de_diplome.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bj-travail-diplome-2021\documentation\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C02D74A-4F3C-44CD-A358-B3B0F968A3BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EC353B-2F28-45BE-B2D9-401B3E777677}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -252,9 +252,6 @@
     <t>Onglet contenu séances</t>
   </si>
   <si>
-    <t>Onglet d'affichage de tous les clients</t>
-  </si>
-  <si>
     <t>Onglet des contenus séances d'un client</t>
   </si>
   <si>
@@ -292,6 +289,9 @@
   </si>
   <si>
     <t>Poster</t>
+  </si>
+  <si>
+    <t>Onglet d'affichage de tous les clients (Administration)</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1204,7 @@
   <dimension ref="A1:BT47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+      <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1889,7 +1889,7 @@
     </row>
     <row r="9" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="18">
         <v>6</v>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="10" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="18">
         <v>6</v>
@@ -2013,7 +2013,7 @@
     </row>
     <row r="11" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="18">
         <v>6</v>
@@ -2215,7 +2215,7 @@
     </row>
     <row r="14" spans="1:72" s="40" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" s="41"/>
       <c r="C14" s="64"/>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="15" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" s="20">
         <v>4</v>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="16" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="20">
         <v>4</v>
@@ -2403,7 +2403,7 @@
     </row>
     <row r="17" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B17" s="20">
         <v>4</v>
@@ -2614,7 +2614,9 @@
       <c r="T20" s="58"/>
       <c r="U20" s="59"/>
       <c r="V20" s="58"/>
-      <c r="W20" s="58"/>
+      <c r="W20" s="58">
+        <v>3</v>
+      </c>
       <c r="X20" s="58"/>
       <c r="Y20" s="58"/>
       <c r="Z20" s="58"/>
@@ -2636,7 +2638,7 @@
       <c r="AP20" s="60"/>
       <c r="AQ20" s="20">
         <f>SUM(C20:AP20)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR20" s="49"/>
       <c r="AS20" s="49"/>
@@ -2827,7 +2829,7 @@
     </row>
     <row r="24" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B24" s="20">
         <v>4</v>
@@ -2852,7 +2854,9 @@
       <c r="T24" s="58"/>
       <c r="U24" s="59"/>
       <c r="V24" s="58"/>
-      <c r="W24" s="58"/>
+      <c r="W24" s="58">
+        <v>3</v>
+      </c>
       <c r="X24" s="58"/>
       <c r="Y24" s="58"/>
       <c r="Z24" s="58"/>
@@ -2874,7 +2878,7 @@
       <c r="AP24" s="60"/>
       <c r="AQ24" s="20">
         <f>SUM(C24:AP24)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR24" s="49"/>
       <c r="AS24" s="49"/>
@@ -3097,7 +3101,7 @@
     </row>
     <row r="29" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29" s="20">
         <v>4</v>
@@ -3151,7 +3155,7 @@
     </row>
     <row r="30" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="20">
         <v>4</v>
@@ -3503,7 +3507,7 @@
     </row>
     <row r="36" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="20">
         <v>16</v>
@@ -4033,7 +4037,7 @@
     </row>
     <row r="44" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44" s="20">
         <v>68</v>
@@ -4099,7 +4103,7 @@
     </row>
     <row r="45" spans="1:72" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45" s="21">
         <v>38</v>
@@ -4229,7 +4233,7 @@
     </row>
     <row r="46" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B46" s="20">
         <v>10</v>
@@ -4370,7 +4374,7 @@
       </c>
       <c r="W47" s="22">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="X47">
         <f t="shared" si="5"/>
@@ -4450,7 +4454,7 @@
       </c>
       <c r="AQ47" s="22">
         <f>SUM(AQ4:AQ45)</f>
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="AR47" s="49"/>
       <c r="AS47" s="49"/>

</xml_diff>

<commit_message>
Modification of the documentation images
</commit_message>
<xml_diff>
--- a/documentation/planning/planning_effectif_travail_de_diplome.xlsx
+++ b/documentation/planning/planning_effectif_travail_de_diplome.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bj-travail-diplome-2021\documentation\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EC353B-2F28-45BE-B2D9-401B3E777677}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C18114-CA35-4ED0-BE65-02FEA668CCFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -291,7 +291,13 @@
     <t>Poster</t>
   </si>
   <si>
-    <t>Onglet d'affichage de tous les clients (Administration)</t>
+    <t>Onglet administration</t>
+  </si>
+  <si>
+    <t>Onglet connexion</t>
+  </si>
+  <si>
+    <t>Onglet inscription</t>
   </si>
 </sst>
 </file>
@@ -840,7 +846,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1201,10 +1221,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BT47"/>
+  <dimension ref="A1:BT49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2457,85 +2477,65 @@
       <c r="AR17" s="49"/>
       <c r="AS17" s="49"/>
     </row>
-    <row r="18" spans="1:72" s="40" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="59"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="59"/>
-      <c r="R18" s="59"/>
-      <c r="S18" s="59"/>
-      <c r="T18" s="59"/>
+    <row r="18" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="20">
+        <v>4</v>
+      </c>
+      <c r="C18" s="65"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="58"/>
+      <c r="N18" s="58"/>
+      <c r="O18" s="58"/>
+      <c r="P18" s="58"/>
+      <c r="Q18" s="58"/>
+      <c r="R18" s="58"/>
+      <c r="S18" s="58"/>
+      <c r="T18" s="58"/>
       <c r="U18" s="59"/>
-      <c r="V18" s="59"/>
-      <c r="W18" s="59"/>
-      <c r="X18" s="59"/>
-      <c r="Y18" s="59"/>
-      <c r="Z18" s="59"/>
-      <c r="AA18" s="59"/>
+      <c r="V18" s="58">
+        <v>2</v>
+      </c>
+      <c r="W18" s="58"/>
+      <c r="X18" s="58"/>
+      <c r="Y18" s="58"/>
+      <c r="Z18" s="58"/>
+      <c r="AA18" s="58"/>
       <c r="AB18" s="59"/>
-      <c r="AC18" s="59"/>
-      <c r="AD18" s="59"/>
-      <c r="AE18" s="59"/>
-      <c r="AF18" s="59"/>
-      <c r="AG18" s="59"/>
-      <c r="AH18" s="59"/>
-      <c r="AI18" s="59"/>
-      <c r="AJ18" s="59"/>
-      <c r="AK18" s="59"/>
-      <c r="AL18" s="59"/>
-      <c r="AM18" s="59"/>
-      <c r="AN18" s="59"/>
-      <c r="AO18" s="59"/>
-      <c r="AP18" s="63"/>
-      <c r="AQ18" s="41"/>
+      <c r="AC18" s="58"/>
+      <c r="AD18" s="58"/>
+      <c r="AE18" s="58"/>
+      <c r="AF18" s="58"/>
+      <c r="AG18" s="58"/>
+      <c r="AH18" s="58"/>
+      <c r="AI18" s="58"/>
+      <c r="AJ18" s="58"/>
+      <c r="AK18" s="58"/>
+      <c r="AL18" s="58"/>
+      <c r="AM18" s="58"/>
+      <c r="AN18" s="58"/>
+      <c r="AO18" s="58"/>
+      <c r="AP18" s="60"/>
+      <c r="AQ18" s="20">
+        <f>SUM(C18:AP18)</f>
+        <v>2</v>
+      </c>
       <c r="AR18" s="49"/>
       <c r="AS18" s="49"/>
-      <c r="AT18" s="2"/>
-      <c r="AU18" s="2"/>
-      <c r="AV18" s="2"/>
-      <c r="AW18" s="2"/>
-      <c r="AX18" s="2"/>
-      <c r="AY18"/>
-      <c r="AZ18"/>
-      <c r="BA18"/>
-      <c r="BB18"/>
-      <c r="BC18"/>
-      <c r="BD18"/>
-      <c r="BE18"/>
-      <c r="BF18"/>
-      <c r="BG18"/>
-      <c r="BH18"/>
-      <c r="BI18"/>
-      <c r="BJ18"/>
-      <c r="BK18"/>
-      <c r="BL18"/>
-      <c r="BM18"/>
-      <c r="BN18"/>
-      <c r="BO18"/>
-      <c r="BP18"/>
-      <c r="BQ18"/>
-      <c r="BR18"/>
-      <c r="BS18"/>
-      <c r="BT18"/>
     </row>
     <row r="19" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="B19" s="20">
         <v>4</v>
@@ -2561,8 +2561,12 @@
       <c r="U19" s="59"/>
       <c r="V19" s="58"/>
       <c r="W19" s="58"/>
-      <c r="X19" s="58"/>
-      <c r="Y19" s="58"/>
+      <c r="X19" s="58">
+        <v>3</v>
+      </c>
+      <c r="Y19" s="58">
+        <v>3</v>
+      </c>
       <c r="Z19" s="58"/>
       <c r="AA19" s="58"/>
       <c r="AB19" s="59"/>
@@ -2582,73 +2586,93 @@
       <c r="AP19" s="60"/>
       <c r="AQ19" s="20">
         <f>SUM(C19:AP19)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AR19" s="49"/>
       <c r="AS19" s="49"/>
     </row>
-    <row r="20" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="20">
-        <v>4</v>
-      </c>
-      <c r="C20" s="65"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="58"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="58"/>
-      <c r="O20" s="58"/>
-      <c r="P20" s="58"/>
-      <c r="Q20" s="58"/>
-      <c r="R20" s="58"/>
-      <c r="S20" s="58"/>
-      <c r="T20" s="58"/>
+    <row r="20" spans="1:72" s="40" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="41"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="59"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="59"/>
+      <c r="L20" s="59"/>
+      <c r="M20" s="59"/>
+      <c r="N20" s="59"/>
+      <c r="O20" s="59"/>
+      <c r="P20" s="59"/>
+      <c r="Q20" s="59"/>
+      <c r="R20" s="59"/>
+      <c r="S20" s="59"/>
+      <c r="T20" s="59"/>
       <c r="U20" s="59"/>
-      <c r="V20" s="58"/>
-      <c r="W20" s="58">
-        <v>3</v>
-      </c>
-      <c r="X20" s="58"/>
-      <c r="Y20" s="58"/>
-      <c r="Z20" s="58"/>
-      <c r="AA20" s="58"/>
+      <c r="V20" s="59"/>
+      <c r="W20" s="59"/>
+      <c r="X20" s="59"/>
+      <c r="Y20" s="59"/>
+      <c r="Z20" s="59"/>
+      <c r="AA20" s="59"/>
       <c r="AB20" s="59"/>
-      <c r="AC20" s="58"/>
-      <c r="AD20" s="58"/>
-      <c r="AE20" s="58"/>
-      <c r="AF20" s="58"/>
-      <c r="AG20" s="58"/>
-      <c r="AH20" s="58"/>
-      <c r="AI20" s="58"/>
-      <c r="AJ20" s="58"/>
-      <c r="AK20" s="58"/>
-      <c r="AL20" s="58"/>
-      <c r="AM20" s="58"/>
-      <c r="AN20" s="58"/>
-      <c r="AO20" s="58"/>
-      <c r="AP20" s="60"/>
-      <c r="AQ20" s="20">
-        <f>SUM(C20:AP20)</f>
-        <v>3</v>
-      </c>
+      <c r="AC20" s="59"/>
+      <c r="AD20" s="59"/>
+      <c r="AE20" s="59"/>
+      <c r="AF20" s="59"/>
+      <c r="AG20" s="59"/>
+      <c r="AH20" s="59"/>
+      <c r="AI20" s="59"/>
+      <c r="AJ20" s="59"/>
+      <c r="AK20" s="59"/>
+      <c r="AL20" s="59"/>
+      <c r="AM20" s="59"/>
+      <c r="AN20" s="59"/>
+      <c r="AO20" s="59"/>
+      <c r="AP20" s="63"/>
+      <c r="AQ20" s="41"/>
       <c r="AR20" s="49"/>
       <c r="AS20" s="49"/>
+      <c r="AT20" s="2"/>
+      <c r="AU20" s="2"/>
+      <c r="AV20" s="2"/>
+      <c r="AW20" s="2"/>
+      <c r="AX20" s="2"/>
+      <c r="AY20"/>
+      <c r="AZ20"/>
+      <c r="BA20"/>
+      <c r="BB20"/>
+      <c r="BC20"/>
+      <c r="BD20"/>
+      <c r="BE20"/>
+      <c r="BF20"/>
+      <c r="BG20"/>
+      <c r="BH20"/>
+      <c r="BI20"/>
+      <c r="BJ20"/>
+      <c r="BK20"/>
+      <c r="BL20"/>
+      <c r="BM20"/>
+      <c r="BN20"/>
+      <c r="BO20"/>
+      <c r="BP20"/>
+      <c r="BQ20"/>
+      <c r="BR20"/>
+      <c r="BS20"/>
+      <c r="BT20"/>
     </row>
     <row r="21" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>47</v>
+      <c r="A21" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="B21" s="20">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C21" s="65"/>
       <c r="D21" s="58"/>
@@ -2698,11 +2722,11 @@
       <c r="AS21" s="49"/>
     </row>
     <row r="22" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>74</v>
+      <c r="A22" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="B22" s="20">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C22" s="65"/>
       <c r="D22" s="58"/>
@@ -2724,7 +2748,9 @@
       <c r="T22" s="58"/>
       <c r="U22" s="59"/>
       <c r="V22" s="58"/>
-      <c r="W22" s="58"/>
+      <c r="W22" s="58">
+        <v>3</v>
+      </c>
       <c r="X22" s="58"/>
       <c r="Y22" s="58"/>
       <c r="Z22" s="58"/>
@@ -2746,93 +2772,71 @@
       <c r="AP22" s="60"/>
       <c r="AQ22" s="20">
         <f>SUM(C22:AP22)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR22" s="49"/>
       <c r="AS22" s="49"/>
     </row>
-    <row r="23" spans="1:72" s="40" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59"/>
-      <c r="K23" s="59"/>
-      <c r="L23" s="59"/>
-      <c r="M23" s="59"/>
-      <c r="N23" s="59"/>
-      <c r="O23" s="59"/>
-      <c r="P23" s="59"/>
-      <c r="Q23" s="59"/>
-      <c r="R23" s="59"/>
-      <c r="S23" s="59"/>
-      <c r="T23" s="59"/>
+    <row r="23" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="20">
+        <v>8</v>
+      </c>
+      <c r="C23" s="65"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="58"/>
+      <c r="N23" s="58"/>
+      <c r="O23" s="58"/>
+      <c r="P23" s="58"/>
+      <c r="Q23" s="58"/>
+      <c r="R23" s="58"/>
+      <c r="S23" s="58"/>
+      <c r="T23" s="58"/>
       <c r="U23" s="59"/>
-      <c r="V23" s="59"/>
-      <c r="W23" s="59"/>
-      <c r="X23" s="59"/>
-      <c r="Y23" s="59"/>
-      <c r="Z23" s="59"/>
-      <c r="AA23" s="59"/>
+      <c r="V23" s="58"/>
+      <c r="W23" s="58"/>
+      <c r="X23" s="58"/>
+      <c r="Y23" s="58"/>
+      <c r="Z23" s="58"/>
+      <c r="AA23" s="58"/>
       <c r="AB23" s="59"/>
-      <c r="AC23" s="59"/>
-      <c r="AD23" s="59"/>
-      <c r="AE23" s="59"/>
-      <c r="AF23" s="59"/>
-      <c r="AG23" s="59"/>
-      <c r="AH23" s="59"/>
-      <c r="AI23" s="59"/>
-      <c r="AJ23" s="59"/>
-      <c r="AK23" s="59"/>
-      <c r="AL23" s="59"/>
-      <c r="AM23" s="59"/>
-      <c r="AN23" s="59"/>
-      <c r="AO23" s="59"/>
-      <c r="AP23" s="63"/>
-      <c r="AQ23" s="41"/>
+      <c r="AC23" s="58"/>
+      <c r="AD23" s="58"/>
+      <c r="AE23" s="58"/>
+      <c r="AF23" s="58"/>
+      <c r="AG23" s="58"/>
+      <c r="AH23" s="58"/>
+      <c r="AI23" s="58"/>
+      <c r="AJ23" s="58"/>
+      <c r="AK23" s="58"/>
+      <c r="AL23" s="58"/>
+      <c r="AM23" s="58"/>
+      <c r="AN23" s="58"/>
+      <c r="AO23" s="58"/>
+      <c r="AP23" s="60"/>
+      <c r="AQ23" s="20">
+        <f>SUM(C23:AP23)</f>
+        <v>0</v>
+      </c>
       <c r="AR23" s="49"/>
       <c r="AS23" s="49"/>
-      <c r="AT23" s="2"/>
-      <c r="AU23" s="2"/>
-      <c r="AV23" s="2"/>
-      <c r="AW23" s="2"/>
-      <c r="AX23" s="2"/>
-      <c r="AY23"/>
-      <c r="AZ23"/>
-      <c r="BA23"/>
-      <c r="BB23"/>
-      <c r="BC23"/>
-      <c r="BD23"/>
-      <c r="BE23"/>
-      <c r="BF23"/>
-      <c r="BG23"/>
-      <c r="BH23"/>
-      <c r="BI23"/>
-      <c r="BJ23"/>
-      <c r="BK23"/>
-      <c r="BL23"/>
-      <c r="BM23"/>
-      <c r="BN23"/>
-      <c r="BO23"/>
-      <c r="BP23"/>
-      <c r="BQ23"/>
-      <c r="BR23"/>
-      <c r="BS23"/>
-      <c r="BT23"/>
     </row>
     <row r="24" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>88</v>
+      <c r="A24" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="B24" s="20">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C24" s="65"/>
       <c r="D24" s="58"/>
@@ -2854,9 +2858,7 @@
       <c r="T24" s="58"/>
       <c r="U24" s="59"/>
       <c r="V24" s="58"/>
-      <c r="W24" s="58">
-        <v>3</v>
-      </c>
+      <c r="W24" s="58"/>
       <c r="X24" s="58"/>
       <c r="Y24" s="58"/>
       <c r="Z24" s="58"/>
@@ -2878,68 +2880,90 @@
       <c r="AP24" s="60"/>
       <c r="AQ24" s="20">
         <f>SUM(C24:AP24)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AR24" s="49"/>
       <c r="AS24" s="49"/>
     </row>
-    <row r="25" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="20">
-        <v>4</v>
-      </c>
-      <c r="C25" s="65"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="58"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="58"/>
-      <c r="M25" s="58"/>
-      <c r="N25" s="58"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="58"/>
-      <c r="R25" s="58"/>
-      <c r="S25" s="58"/>
-      <c r="T25" s="58"/>
+    <row r="25" spans="1:72" s="40" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="41"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="59"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="59"/>
+      <c r="T25" s="59"/>
       <c r="U25" s="59"/>
-      <c r="V25" s="58"/>
-      <c r="W25" s="58"/>
-      <c r="X25" s="58"/>
-      <c r="Y25" s="58"/>
-      <c r="Z25" s="58"/>
-      <c r="AA25" s="58"/>
+      <c r="V25" s="59"/>
+      <c r="W25" s="59"/>
+      <c r="X25" s="59"/>
+      <c r="Y25" s="59"/>
+      <c r="Z25" s="59"/>
+      <c r="AA25" s="59"/>
       <c r="AB25" s="59"/>
-      <c r="AC25" s="58"/>
-      <c r="AD25" s="58"/>
-      <c r="AE25" s="58"/>
-      <c r="AF25" s="58"/>
-      <c r="AG25" s="58"/>
-      <c r="AH25" s="58"/>
-      <c r="AI25" s="58"/>
-      <c r="AJ25" s="58"/>
-      <c r="AK25" s="58"/>
-      <c r="AL25" s="58"/>
-      <c r="AM25" s="58"/>
-      <c r="AN25" s="58"/>
-      <c r="AO25" s="58"/>
-      <c r="AP25" s="60"/>
-      <c r="AQ25" s="20">
-        <f>SUM(C25:AP25)</f>
-        <v>0</v>
-      </c>
+      <c r="AC25" s="59"/>
+      <c r="AD25" s="59"/>
+      <c r="AE25" s="59"/>
+      <c r="AF25" s="59"/>
+      <c r="AG25" s="59"/>
+      <c r="AH25" s="59"/>
+      <c r="AI25" s="59"/>
+      <c r="AJ25" s="59"/>
+      <c r="AK25" s="59"/>
+      <c r="AL25" s="59"/>
+      <c r="AM25" s="59"/>
+      <c r="AN25" s="59"/>
+      <c r="AO25" s="59"/>
+      <c r="AP25" s="63"/>
+      <c r="AQ25" s="41"/>
       <c r="AR25" s="49"/>
       <c r="AS25" s="49"/>
+      <c r="AT25" s="2"/>
+      <c r="AU25" s="2"/>
+      <c r="AV25" s="2"/>
+      <c r="AW25" s="2"/>
+      <c r="AX25" s="2"/>
+      <c r="AY25"/>
+      <c r="AZ25"/>
+      <c r="BA25"/>
+      <c r="BB25"/>
+      <c r="BC25"/>
+      <c r="BD25"/>
+      <c r="BE25"/>
+      <c r="BF25"/>
+      <c r="BG25"/>
+      <c r="BH25"/>
+      <c r="BI25"/>
+      <c r="BJ25"/>
+      <c r="BK25"/>
+      <c r="BL25"/>
+      <c r="BM25"/>
+      <c r="BN25"/>
+      <c r="BO25"/>
+      <c r="BP25"/>
+      <c r="BQ25"/>
+      <c r="BR25"/>
+      <c r="BS25"/>
+      <c r="BT25"/>
     </row>
     <row r="26" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="B26" s="20">
         <v>4</v>
@@ -2964,7 +2988,9 @@
       <c r="T26" s="58"/>
       <c r="U26" s="59"/>
       <c r="V26" s="58"/>
-      <c r="W26" s="58"/>
+      <c r="W26" s="58">
+        <v>3</v>
+      </c>
       <c r="X26" s="58"/>
       <c r="Y26" s="58"/>
       <c r="Z26" s="58"/>
@@ -2986,14 +3012,14 @@
       <c r="AP26" s="60"/>
       <c r="AQ26" s="20">
         <f>SUM(C26:AP26)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR26" s="49"/>
       <c r="AS26" s="49"/>
     </row>
     <row r="27" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B27" s="20">
         <v>4</v>
@@ -3047,7 +3073,7 @@
     </row>
     <row r="28" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B28" s="20">
         <v>4</v>
@@ -3101,7 +3127,7 @@
     </row>
     <row r="29" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="B29" s="20">
         <v>4</v>
@@ -3127,10 +3153,18 @@
       <c r="U29" s="59"/>
       <c r="V29" s="58"/>
       <c r="W29" s="58"/>
-      <c r="X29" s="58"/>
-      <c r="Y29" s="58"/>
-      <c r="Z29" s="58"/>
-      <c r="AA29" s="58"/>
+      <c r="X29" s="58">
+        <v>3</v>
+      </c>
+      <c r="Y29" s="58">
+        <v>3</v>
+      </c>
+      <c r="Z29" s="58">
+        <v>6</v>
+      </c>
+      <c r="AA29" s="58">
+        <v>3</v>
+      </c>
       <c r="AB29" s="59"/>
       <c r="AC29" s="58"/>
       <c r="AD29" s="58"/>
@@ -3147,15 +3181,15 @@
       <c r="AO29" s="58"/>
       <c r="AP29" s="60"/>
       <c r="AQ29" s="20">
-        <f t="shared" ref="AQ29" si="2">SUM(C29:AP29)</f>
-        <v>0</v>
+        <f>SUM(C29:AP29)</f>
+        <v>15</v>
       </c>
       <c r="AR29" s="49"/>
       <c r="AS29" s="49"/>
     </row>
-    <row r="30" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>76</v>
+    <row r="30" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="B30" s="20">
         <v>4</v>
@@ -3207,88 +3241,66 @@
       <c r="AR30" s="49"/>
       <c r="AS30" s="49"/>
     </row>
-    <row r="31" spans="1:72" s="40" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="59"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="59"/>
-      <c r="K31" s="59"/>
-      <c r="L31" s="59"/>
-      <c r="M31" s="59"/>
-      <c r="N31" s="59"/>
-      <c r="O31" s="59"/>
-      <c r="P31" s="59"/>
-      <c r="Q31" s="59"/>
-      <c r="R31" s="59"/>
-      <c r="S31" s="59"/>
-      <c r="T31" s="59"/>
+    <row r="31" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="20">
+        <v>4</v>
+      </c>
+      <c r="C31" s="65"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="58"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="58"/>
+      <c r="P31" s="58"/>
+      <c r="Q31" s="58"/>
+      <c r="R31" s="58"/>
+      <c r="S31" s="58"/>
+      <c r="T31" s="58"/>
       <c r="U31" s="59"/>
-      <c r="V31" s="59"/>
-      <c r="W31" s="59"/>
-      <c r="X31" s="59"/>
-      <c r="Y31" s="59"/>
-      <c r="Z31" s="59"/>
-      <c r="AA31" s="59"/>
+      <c r="V31" s="58"/>
+      <c r="W31" s="58"/>
+      <c r="X31" s="58"/>
+      <c r="Y31" s="58"/>
+      <c r="Z31" s="58"/>
+      <c r="AA31" s="58"/>
       <c r="AB31" s="59"/>
-      <c r="AC31" s="59"/>
-      <c r="AD31" s="59"/>
-      <c r="AE31" s="59"/>
-      <c r="AF31" s="59"/>
-      <c r="AG31" s="59"/>
-      <c r="AH31" s="59"/>
-      <c r="AI31" s="59"/>
-      <c r="AJ31" s="59"/>
-      <c r="AK31" s="59"/>
-      <c r="AL31" s="59"/>
-      <c r="AM31" s="59"/>
-      <c r="AN31" s="59"/>
-      <c r="AO31" s="59"/>
-      <c r="AP31" s="63"/>
-      <c r="AQ31" s="41"/>
+      <c r="AC31" s="58"/>
+      <c r="AD31" s="58"/>
+      <c r="AE31" s="58"/>
+      <c r="AF31" s="58"/>
+      <c r="AG31" s="58"/>
+      <c r="AH31" s="58"/>
+      <c r="AI31" s="58"/>
+      <c r="AJ31" s="58"/>
+      <c r="AK31" s="58"/>
+      <c r="AL31" s="58"/>
+      <c r="AM31" s="58"/>
+      <c r="AN31" s="58"/>
+      <c r="AO31" s="58"/>
+      <c r="AP31" s="60"/>
+      <c r="AQ31" s="20">
+        <f t="shared" ref="AQ31" si="2">SUM(C31:AP31)</f>
+        <v>0</v>
+      </c>
       <c r="AR31" s="49"/>
       <c r="AS31" s="49"/>
-      <c r="AT31" s="2"/>
-      <c r="AU31" s="2"/>
-      <c r="AV31" s="2"/>
-      <c r="AW31" s="2"/>
-      <c r="AX31" s="2"/>
-      <c r="AY31"/>
-      <c r="AZ31"/>
-      <c r="BA31"/>
-      <c r="BB31"/>
-      <c r="BC31"/>
-      <c r="BD31"/>
-      <c r="BE31"/>
-      <c r="BF31"/>
-      <c r="BG31"/>
-      <c r="BH31"/>
-      <c r="BI31"/>
-      <c r="BJ31"/>
-      <c r="BK31"/>
-      <c r="BL31"/>
-      <c r="BM31"/>
-      <c r="BN31"/>
-      <c r="BO31"/>
-      <c r="BP31"/>
-      <c r="BQ31"/>
-      <c r="BR31"/>
-      <c r="BS31"/>
-      <c r="BT31"/>
-    </row>
-    <row r="32" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
-        <v>73</v>
+    </row>
+    <row r="32" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="B32" s="20">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C32" s="65"/>
       <c r="D32" s="58"/>
@@ -3307,9 +3319,7 @@
       <c r="Q32" s="58"/>
       <c r="R32" s="58"/>
       <c r="S32" s="58"/>
-      <c r="T32" s="58">
-        <v>6</v>
-      </c>
+      <c r="T32" s="58"/>
       <c r="U32" s="59"/>
       <c r="V32" s="58"/>
       <c r="W32" s="58"/>
@@ -3333,72 +3343,94 @@
       <c r="AO32" s="58"/>
       <c r="AP32" s="60"/>
       <c r="AQ32" s="20">
-        <f t="shared" ref="AQ32:AQ41" si="3">SUM(C32:AP32)</f>
-        <v>6</v>
+        <f>SUM(C32:AP32)</f>
+        <v>0</v>
       </c>
       <c r="AR32" s="49"/>
       <c r="AS32" s="49"/>
     </row>
-    <row r="33" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="20">
-        <v>6</v>
-      </c>
-      <c r="C33" s="65"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="58"/>
-      <c r="Q33" s="58"/>
-      <c r="R33" s="58"/>
-      <c r="S33" s="58"/>
-      <c r="T33" s="58"/>
+    <row r="33" spans="1:72" s="40" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="41"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="59"/>
+      <c r="K33" s="59"/>
+      <c r="L33" s="59"/>
+      <c r="M33" s="59"/>
+      <c r="N33" s="59"/>
+      <c r="O33" s="59"/>
+      <c r="P33" s="59"/>
+      <c r="Q33" s="59"/>
+      <c r="R33" s="59"/>
+      <c r="S33" s="59"/>
+      <c r="T33" s="59"/>
       <c r="U33" s="59"/>
-      <c r="V33" s="58"/>
-      <c r="W33" s="58"/>
-      <c r="X33" s="58"/>
-      <c r="Y33" s="58"/>
-      <c r="Z33" s="58"/>
-      <c r="AA33" s="58"/>
+      <c r="V33" s="59"/>
+      <c r="W33" s="59"/>
+      <c r="X33" s="59"/>
+      <c r="Y33" s="59"/>
+      <c r="Z33" s="59"/>
+      <c r="AA33" s="59"/>
       <c r="AB33" s="59"/>
-      <c r="AC33" s="58"/>
-      <c r="AD33" s="58"/>
-      <c r="AE33" s="58"/>
-      <c r="AF33" s="58"/>
-      <c r="AG33" s="58"/>
-      <c r="AH33" s="58"/>
-      <c r="AI33" s="58"/>
-      <c r="AJ33" s="58"/>
-      <c r="AK33" s="58"/>
-      <c r="AL33" s="58"/>
-      <c r="AM33" s="58"/>
-      <c r="AN33" s="58"/>
-      <c r="AO33" s="58"/>
-      <c r="AP33" s="60"/>
-      <c r="AQ33" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="AC33" s="59"/>
+      <c r="AD33" s="59"/>
+      <c r="AE33" s="59"/>
+      <c r="AF33" s="59"/>
+      <c r="AG33" s="59"/>
+      <c r="AH33" s="59"/>
+      <c r="AI33" s="59"/>
+      <c r="AJ33" s="59"/>
+      <c r="AK33" s="59"/>
+      <c r="AL33" s="59"/>
+      <c r="AM33" s="59"/>
+      <c r="AN33" s="59"/>
+      <c r="AO33" s="59"/>
+      <c r="AP33" s="63"/>
+      <c r="AQ33" s="41"/>
       <c r="AR33" s="49"/>
       <c r="AS33" s="49"/>
+      <c r="AT33" s="2"/>
+      <c r="AU33" s="2"/>
+      <c r="AV33" s="2"/>
+      <c r="AW33" s="2"/>
+      <c r="AX33" s="2"/>
+      <c r="AY33"/>
+      <c r="AZ33"/>
+      <c r="BA33"/>
+      <c r="BB33"/>
+      <c r="BC33"/>
+      <c r="BD33"/>
+      <c r="BE33"/>
+      <c r="BF33"/>
+      <c r="BG33"/>
+      <c r="BH33"/>
+      <c r="BI33"/>
+      <c r="BJ33"/>
+      <c r="BK33"/>
+      <c r="BL33"/>
+      <c r="BM33"/>
+      <c r="BN33"/>
+      <c r="BO33"/>
+      <c r="BP33"/>
+      <c r="BQ33"/>
+      <c r="BR33"/>
+      <c r="BS33"/>
+      <c r="BT33"/>
     </row>
     <row r="34" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B34" s="20">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C34" s="65"/>
       <c r="D34" s="58"/>
@@ -3417,7 +3449,9 @@
       <c r="Q34" s="58"/>
       <c r="R34" s="58"/>
       <c r="S34" s="58"/>
-      <c r="T34" s="58"/>
+      <c r="T34" s="58">
+        <v>6</v>
+      </c>
       <c r="U34" s="59"/>
       <c r="V34" s="58"/>
       <c r="W34" s="58"/>
@@ -3441,18 +3475,18 @@
       <c r="AO34" s="58"/>
       <c r="AP34" s="60"/>
       <c r="AQ34" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="AQ34:AQ43" si="3">SUM(C34:AP34)</f>
+        <v>6</v>
       </c>
       <c r="AR34" s="49"/>
       <c r="AS34" s="49"/>
     </row>
     <row r="35" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35" s="20">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C35" s="65"/>
       <c r="D35" s="58"/>
@@ -3467,12 +3501,8 @@
       <c r="M35" s="58"/>
       <c r="N35" s="58"/>
       <c r="O35" s="58"/>
-      <c r="P35" s="58">
-        <v>2</v>
-      </c>
-      <c r="Q35" s="58">
-        <v>4</v>
-      </c>
+      <c r="P35" s="58"/>
+      <c r="Q35" s="58"/>
       <c r="R35" s="58"/>
       <c r="S35" s="58"/>
       <c r="T35" s="58"/>
@@ -3500,17 +3530,17 @@
       <c r="AP35" s="60"/>
       <c r="AQ35" s="20">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AR35" s="49"/>
       <c r="AS35" s="49"/>
     </row>
     <row r="36" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B36" s="20">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C36" s="65"/>
       <c r="D36" s="58"/>
@@ -3561,7 +3591,7 @@
     </row>
     <row r="37" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B37" s="20">
         <v>8</v>
@@ -3579,8 +3609,12 @@
       <c r="M37" s="58"/>
       <c r="N37" s="58"/>
       <c r="O37" s="58"/>
-      <c r="P37" s="58"/>
-      <c r="Q37" s="58"/>
+      <c r="P37" s="58">
+        <v>2</v>
+      </c>
+      <c r="Q37" s="58">
+        <v>4</v>
+      </c>
       <c r="R37" s="58"/>
       <c r="S37" s="58"/>
       <c r="T37" s="58"/>
@@ -3608,17 +3642,17 @@
       <c r="AP37" s="60"/>
       <c r="AQ37" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AR37" s="49"/>
       <c r="AS37" s="49"/>
     </row>
     <row r="38" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="B38" s="20">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C38" s="65"/>
       <c r="D38" s="58"/>
@@ -3668,8 +3702,8 @@
       <c r="AS38" s="49"/>
     </row>
     <row r="39" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
-        <v>59</v>
+      <c r="A39" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="B39" s="20">
         <v>8</v>
@@ -3723,10 +3757,10 @@
     </row>
     <row r="40" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B40" s="20">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C40" s="65"/>
       <c r="D40" s="58"/>
@@ -3775,12 +3809,12 @@
       <c r="AR40" s="49"/>
       <c r="AS40" s="49"/>
     </row>
-    <row r="41" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>58</v>
+    <row r="41" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="B41" s="20">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C41" s="65"/>
       <c r="D41" s="58"/>
@@ -3829,284 +3863,196 @@
       <c r="AR41" s="49"/>
       <c r="AS41" s="49"/>
     </row>
-    <row r="42" spans="1:72" s="40" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" s="41"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="39"/>
-      <c r="L42" s="39"/>
-      <c r="M42" s="39"/>
-      <c r="N42" s="39"/>
-      <c r="O42" s="39"/>
-      <c r="P42" s="39"/>
-      <c r="Q42" s="39"/>
-      <c r="R42" s="39"/>
-      <c r="S42" s="39"/>
-      <c r="T42" s="39"/>
-      <c r="U42" s="39"/>
-      <c r="V42" s="39"/>
-      <c r="W42" s="39"/>
-      <c r="X42" s="39"/>
-      <c r="Y42" s="39"/>
-      <c r="Z42" s="39"/>
-      <c r="AA42" s="39"/>
-      <c r="AB42" s="39"/>
-      <c r="AC42" s="39"/>
-      <c r="AD42" s="39"/>
-      <c r="AE42" s="39"/>
-      <c r="AF42" s="39"/>
-      <c r="AG42" s="39"/>
-      <c r="AH42" s="39"/>
-      <c r="AI42" s="39"/>
-      <c r="AJ42" s="39"/>
-      <c r="AK42" s="39"/>
-      <c r="AL42" s="39"/>
-      <c r="AM42" s="39"/>
-      <c r="AN42" s="39"/>
-      <c r="AO42" s="39"/>
-      <c r="AP42" s="52"/>
-      <c r="AQ42" s="54"/>
+    <row r="42" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" s="20">
+        <v>16</v>
+      </c>
+      <c r="C42" s="65"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="58"/>
+      <c r="J42" s="58"/>
+      <c r="K42" s="58"/>
+      <c r="L42" s="58"/>
+      <c r="M42" s="58"/>
+      <c r="N42" s="58"/>
+      <c r="O42" s="58"/>
+      <c r="P42" s="58"/>
+      <c r="Q42" s="58"/>
+      <c r="R42" s="58"/>
+      <c r="S42" s="58"/>
+      <c r="T42" s="58"/>
+      <c r="U42" s="59"/>
+      <c r="V42" s="58"/>
+      <c r="W42" s="58"/>
+      <c r="X42" s="58"/>
+      <c r="Y42" s="58"/>
+      <c r="Z42" s="58"/>
+      <c r="AA42" s="58"/>
+      <c r="AB42" s="59"/>
+      <c r="AC42" s="58"/>
+      <c r="AD42" s="58"/>
+      <c r="AE42" s="58"/>
+      <c r="AF42" s="58"/>
+      <c r="AG42" s="58"/>
+      <c r="AH42" s="58"/>
+      <c r="AI42" s="58"/>
+      <c r="AJ42" s="58"/>
+      <c r="AK42" s="58"/>
+      <c r="AL42" s="58"/>
+      <c r="AM42" s="58"/>
+      <c r="AN42" s="58"/>
+      <c r="AO42" s="58"/>
+      <c r="AP42" s="60"/>
+      <c r="AQ42" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="AR42" s="49"/>
       <c r="AS42" s="49"/>
-      <c r="AT42" s="2"/>
-      <c r="AU42" s="2"/>
-      <c r="AV42" s="2"/>
-      <c r="AW42" s="2"/>
-      <c r="AX42" s="2"/>
-      <c r="AY42"/>
-      <c r="AZ42"/>
-      <c r="BA42"/>
-      <c r="BB42"/>
-      <c r="BC42"/>
-      <c r="BD42"/>
-      <c r="BE42"/>
-      <c r="BF42"/>
-      <c r="BG42"/>
-      <c r="BH42"/>
-      <c r="BI42"/>
-      <c r="BJ42"/>
-      <c r="BK42"/>
-      <c r="BL42"/>
-      <c r="BM42"/>
-      <c r="BN42"/>
-      <c r="BO42"/>
-      <c r="BP42"/>
-      <c r="BQ42"/>
-      <c r="BR42"/>
-      <c r="BS42"/>
-      <c r="BT42"/>
-    </row>
-    <row r="43" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
-        <v>60</v>
+    </row>
+    <row r="43" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="B43" s="20">
-        <v>68</v>
-      </c>
-      <c r="C43" s="4">
-        <v>1</v>
-      </c>
-      <c r="D43" s="1">
-        <v>1</v>
-      </c>
-      <c r="E43" s="1">
-        <v>1</v>
-      </c>
-      <c r="F43" s="1">
-        <v>1</v>
-      </c>
-      <c r="G43" s="1">
-        <v>1</v>
-      </c>
-      <c r="H43" s="1">
-        <v>1</v>
-      </c>
-      <c r="I43" s="1">
-        <v>1</v>
-      </c>
-      <c r="J43" s="1">
-        <v>1</v>
-      </c>
-      <c r="K43" s="1">
-        <v>1</v>
-      </c>
-      <c r="L43" s="1">
-        <v>1</v>
-      </c>
-      <c r="M43" s="1">
-        <v>1</v>
-      </c>
-      <c r="N43" s="1">
-        <v>1</v>
-      </c>
-      <c r="O43" s="1">
-        <v>1</v>
-      </c>
-      <c r="P43" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q43" s="1">
-        <v>1</v>
-      </c>
-      <c r="R43" s="1">
-        <v>3</v>
-      </c>
-      <c r="S43" s="1">
-        <v>1</v>
-      </c>
-      <c r="T43" s="1">
-        <v>1</v>
-      </c>
-      <c r="U43" s="39"/>
-      <c r="V43" s="1">
-        <v>1</v>
-      </c>
-      <c r="W43" s="1">
-        <v>1</v>
-      </c>
-      <c r="X43" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y43" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB43" s="39"/>
-      <c r="AC43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AI43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK43" s="1">
-        <v>5</v>
-      </c>
-      <c r="AL43" s="1">
-        <v>7</v>
-      </c>
-      <c r="AM43" s="1">
-        <v>7</v>
-      </c>
-      <c r="AN43" s="1">
-        <v>7</v>
-      </c>
-      <c r="AO43" s="1">
-        <v>7</v>
-      </c>
-      <c r="AP43" s="1">
-        <v>3</v>
-      </c>
-      <c r="AQ43" s="13">
-        <f>SUM(C43:AP43)</f>
-        <v>70</v>
+        <v>10</v>
+      </c>
+      <c r="C43" s="65"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="58"/>
+      <c r="K43" s="58"/>
+      <c r="L43" s="58"/>
+      <c r="M43" s="58"/>
+      <c r="N43" s="58"/>
+      <c r="O43" s="58"/>
+      <c r="P43" s="58"/>
+      <c r="Q43" s="58"/>
+      <c r="R43" s="58"/>
+      <c r="S43" s="58"/>
+      <c r="T43" s="58"/>
+      <c r="U43" s="59"/>
+      <c r="V43" s="58"/>
+      <c r="W43" s="58"/>
+      <c r="X43" s="58"/>
+      <c r="Y43" s="58"/>
+      <c r="Z43" s="58"/>
+      <c r="AA43" s="58"/>
+      <c r="AB43" s="59"/>
+      <c r="AC43" s="58"/>
+      <c r="AD43" s="58"/>
+      <c r="AE43" s="58"/>
+      <c r="AF43" s="58"/>
+      <c r="AG43" s="58"/>
+      <c r="AH43" s="58"/>
+      <c r="AI43" s="58"/>
+      <c r="AJ43" s="58"/>
+      <c r="AK43" s="58"/>
+      <c r="AL43" s="58"/>
+      <c r="AM43" s="58"/>
+      <c r="AN43" s="58"/>
+      <c r="AO43" s="58"/>
+      <c r="AP43" s="60"/>
+      <c r="AQ43" s="20">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="AR43" s="49"/>
       <c r="AS43" s="49"/>
     </row>
-    <row r="44" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" s="20">
-        <v>68</v>
-      </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1">
-        <v>4</v>
-      </c>
-      <c r="L44" s="1">
-        <v>4</v>
-      </c>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1">
-        <v>4</v>
-      </c>
-      <c r="P44" s="1">
-        <v>4</v>
-      </c>
-      <c r="Q44" s="1">
-        <v>2</v>
-      </c>
-      <c r="R44" s="1"/>
-      <c r="S44" s="1"/>
-      <c r="T44" s="1"/>
+    <row r="44" spans="1:72" s="40" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="41"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="39"/>
+      <c r="M44" s="39"/>
+      <c r="N44" s="39"/>
+      <c r="O44" s="39"/>
+      <c r="P44" s="39"/>
+      <c r="Q44" s="39"/>
+      <c r="R44" s="39"/>
+      <c r="S44" s="39"/>
+      <c r="T44" s="39"/>
       <c r="U44" s="39"/>
-      <c r="V44" s="1">
-        <v>3</v>
-      </c>
-      <c r="W44" s="1"/>
-      <c r="X44" s="1"/>
-      <c r="Y44" s="1"/>
-      <c r="Z44" s="1"/>
-      <c r="AA44" s="1"/>
+      <c r="V44" s="39"/>
+      <c r="W44" s="39"/>
+      <c r="X44" s="39"/>
+      <c r="Y44" s="39"/>
+      <c r="Z44" s="39"/>
+      <c r="AA44" s="39"/>
       <c r="AB44" s="39"/>
-      <c r="AC44" s="1"/>
-      <c r="AD44" s="1"/>
-      <c r="AE44" s="1"/>
-      <c r="AF44" s="1"/>
-      <c r="AG44" s="1"/>
-      <c r="AH44" s="1"/>
-      <c r="AI44" s="1"/>
-      <c r="AJ44" s="1"/>
-      <c r="AK44" s="1"/>
-      <c r="AL44" s="1"/>
-      <c r="AM44" s="1"/>
-      <c r="AN44" s="1"/>
-      <c r="AO44" s="1"/>
-      <c r="AP44" s="1"/>
-      <c r="AQ44" s="13">
-        <f>SUM(C44:AP44)</f>
-        <v>21</v>
-      </c>
+      <c r="AC44" s="39"/>
+      <c r="AD44" s="39"/>
+      <c r="AE44" s="39"/>
+      <c r="AF44" s="39"/>
+      <c r="AG44" s="39"/>
+      <c r="AH44" s="39"/>
+      <c r="AI44" s="39"/>
+      <c r="AJ44" s="39"/>
+      <c r="AK44" s="39"/>
+      <c r="AL44" s="39"/>
+      <c r="AM44" s="39"/>
+      <c r="AN44" s="39"/>
+      <c r="AO44" s="39"/>
+      <c r="AP44" s="52"/>
+      <c r="AQ44" s="54"/>
       <c r="AR44" s="49"/>
       <c r="AS44" s="49"/>
-    </row>
-    <row r="45" spans="1:72" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B45" s="21">
-        <v>38</v>
+      <c r="AT44" s="2"/>
+      <c r="AU44" s="2"/>
+      <c r="AV44" s="2"/>
+      <c r="AW44" s="2"/>
+      <c r="AX44" s="2"/>
+      <c r="AY44"/>
+      <c r="AZ44"/>
+      <c r="BA44"/>
+      <c r="BB44"/>
+      <c r="BC44"/>
+      <c r="BD44"/>
+      <c r="BE44"/>
+      <c r="BF44"/>
+      <c r="BG44"/>
+      <c r="BH44"/>
+      <c r="BI44"/>
+      <c r="BJ44"/>
+      <c r="BK44"/>
+      <c r="BL44"/>
+      <c r="BM44"/>
+      <c r="BN44"/>
+      <c r="BO44"/>
+      <c r="BP44"/>
+      <c r="BQ44"/>
+      <c r="BR44"/>
+      <c r="BS44"/>
+      <c r="BT44"/>
+    </row>
+    <row r="45" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" s="20">
+        <v>68</v>
       </c>
       <c r="C45" s="4">
         <v>1</v>
@@ -4154,7 +4100,7 @@
         <v>1</v>
       </c>
       <c r="R45" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S45" s="1">
         <v>1</v>
@@ -4207,257 +4153,455 @@
         <v>1</v>
       </c>
       <c r="AK45" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AL45" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AM45" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AN45" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AO45" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AP45" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ45" s="14">
+        <v>3</v>
+      </c>
+      <c r="AQ45" s="13">
         <f>SUM(C45:AP45)</f>
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="AR45" s="49"/>
       <c r="AS45" s="49"/>
     </row>
     <row r="46" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
-        <v>87</v>
+      <c r="A46" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="B46" s="20">
-        <v>10</v>
-      </c>
-      <c r="C46" s="65"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="58"/>
-      <c r="J46" s="58"/>
-      <c r="K46" s="58"/>
-      <c r="L46" s="58"/>
-      <c r="M46" s="58"/>
-      <c r="N46" s="58"/>
-      <c r="O46" s="58"/>
-      <c r="P46" s="58"/>
-      <c r="Q46" s="58"/>
-      <c r="R46" s="58"/>
-      <c r="S46" s="58"/>
-      <c r="T46" s="58"/>
-      <c r="U46" s="59"/>
-      <c r="V46" s="58">
+        <v>68</v>
+      </c>
+      <c r="C46" s="4"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1">
+        <v>4</v>
+      </c>
+      <c r="L46" s="1">
+        <v>4</v>
+      </c>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1">
+        <v>4</v>
+      </c>
+      <c r="P46" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>2</v>
+      </c>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="39"/>
+      <c r="V46" s="1">
+        <v>2</v>
+      </c>
+      <c r="W46" s="1"/>
+      <c r="X46" s="1"/>
+      <c r="Y46" s="1"/>
+      <c r="Z46" s="1"/>
+      <c r="AA46" s="1">
         <v>3</v>
       </c>
-      <c r="W46" s="58"/>
-      <c r="X46" s="58"/>
-      <c r="Y46" s="58"/>
-      <c r="Z46" s="58"/>
-      <c r="AA46" s="58"/>
-      <c r="AB46" s="59"/>
-      <c r="AC46" s="58"/>
-      <c r="AD46" s="58"/>
-      <c r="AE46" s="58"/>
-      <c r="AF46" s="58"/>
-      <c r="AG46" s="58"/>
-      <c r="AH46" s="58"/>
-      <c r="AI46" s="58"/>
-      <c r="AJ46" s="58"/>
-      <c r="AK46" s="58"/>
-      <c r="AL46" s="58"/>
-      <c r="AM46" s="58"/>
-      <c r="AN46" s="58"/>
-      <c r="AO46" s="58"/>
-      <c r="AP46" s="60"/>
-      <c r="AQ46" s="20">
-        <f t="shared" ref="AQ46" si="4">SUM(C46:AP46)</f>
-        <v>3</v>
+      <c r="AB46" s="39"/>
+      <c r="AC46" s="1"/>
+      <c r="AD46" s="1"/>
+      <c r="AE46" s="1"/>
+      <c r="AF46" s="1"/>
+      <c r="AG46" s="1"/>
+      <c r="AH46" s="1"/>
+      <c r="AI46" s="1"/>
+      <c r="AJ46" s="1"/>
+      <c r="AK46" s="1"/>
+      <c r="AL46" s="1"/>
+      <c r="AM46" s="1"/>
+      <c r="AN46" s="1"/>
+      <c r="AO46" s="1"/>
+      <c r="AP46" s="1"/>
+      <c r="AQ46" s="13">
+        <f>SUM(C46:AP46)</f>
+        <v>23</v>
       </c>
       <c r="AR46" s="49"/>
       <c r="AS46" s="49"/>
     </row>
-    <row r="47" spans="1:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="22">
-        <f t="shared" ref="B47:AP47" si="5">SUM(B4:B45)</f>
-        <v>380</v>
-      </c>
-      <c r="C47">
+    <row r="47" spans="1:72" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" s="21">
+        <v>38</v>
+      </c>
+      <c r="C47" s="4">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1</v>
+      </c>
+      <c r="G47" s="1">
+        <v>1</v>
+      </c>
+      <c r="H47" s="1">
+        <v>1</v>
+      </c>
+      <c r="I47" s="1">
+        <v>1</v>
+      </c>
+      <c r="J47" s="1">
+        <v>1</v>
+      </c>
+      <c r="K47" s="1">
+        <v>1</v>
+      </c>
+      <c r="L47" s="1">
+        <v>1</v>
+      </c>
+      <c r="M47" s="1">
+        <v>1</v>
+      </c>
+      <c r="N47" s="1">
+        <v>1</v>
+      </c>
+      <c r="O47" s="1">
+        <v>1</v>
+      </c>
+      <c r="P47" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>1</v>
+      </c>
+      <c r="R47" s="1">
+        <v>1</v>
+      </c>
+      <c r="S47" s="1">
+        <v>1</v>
+      </c>
+      <c r="T47" s="1">
+        <v>1</v>
+      </c>
+      <c r="U47" s="39"/>
+      <c r="V47" s="1">
+        <v>1</v>
+      </c>
+      <c r="W47" s="1">
+        <v>1</v>
+      </c>
+      <c r="X47" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y47" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB47" s="39"/>
+      <c r="AC47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ47" s="14">
+        <f>SUM(C47:AP47)</f>
+        <v>38</v>
+      </c>
+      <c r="AR47" s="49"/>
+      <c r="AS47" s="49"/>
+    </row>
+    <row r="48" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="20">
+        <v>10</v>
+      </c>
+      <c r="C48" s="65"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="58"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
+      <c r="I48" s="58"/>
+      <c r="J48" s="58"/>
+      <c r="K48" s="58"/>
+      <c r="L48" s="58"/>
+      <c r="M48" s="58"/>
+      <c r="N48" s="58"/>
+      <c r="O48" s="58"/>
+      <c r="P48" s="58"/>
+      <c r="Q48" s="58"/>
+      <c r="R48" s="58"/>
+      <c r="S48" s="58"/>
+      <c r="T48" s="58"/>
+      <c r="U48" s="59"/>
+      <c r="V48" s="58">
+        <v>2</v>
+      </c>
+      <c r="W48" s="58"/>
+      <c r="X48" s="58"/>
+      <c r="Y48" s="58"/>
+      <c r="Z48" s="58"/>
+      <c r="AA48" s="58"/>
+      <c r="AB48" s="59"/>
+      <c r="AC48" s="58"/>
+      <c r="AD48" s="58"/>
+      <c r="AE48" s="58"/>
+      <c r="AF48" s="58"/>
+      <c r="AG48" s="58"/>
+      <c r="AH48" s="58"/>
+      <c r="AI48" s="58"/>
+      <c r="AJ48" s="58"/>
+      <c r="AK48" s="58"/>
+      <c r="AL48" s="58"/>
+      <c r="AM48" s="58"/>
+      <c r="AN48" s="58"/>
+      <c r="AO48" s="58"/>
+      <c r="AP48" s="60"/>
+      <c r="AQ48" s="20">
+        <f t="shared" ref="AQ48" si="4">SUM(C48:AP48)</f>
+        <v>2</v>
+      </c>
+      <c r="AR48" s="49"/>
+      <c r="AS48" s="49"/>
+    </row>
+    <row r="49" spans="2:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="22">
+        <f t="shared" ref="B49:AP49" si="5">SUM(B4:B47)</f>
+        <v>388</v>
+      </c>
+      <c r="C49">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="D47" s="22">
+      <c r="D49" s="22">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="E47">
+      <c r="E49">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="F47" s="22">
+      <c r="F49" s="22">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="G47">
+      <c r="G49">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="H47" s="22">
+      <c r="H49" s="22">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="I47" s="22">
+      <c r="I49" s="22">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="J47">
+      <c r="J49">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="K47" s="22">
+      <c r="K49" s="22">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="L47">
+      <c r="L49">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="M47" s="22">
+      <c r="M49" s="22">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="N47">
+      <c r="N49">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="O47" s="22">
+      <c r="O49" s="22">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="P47" s="22">
+      <c r="P49" s="22">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="Q47">
+      <c r="Q49">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="R47" s="22">
+      <c r="R49" s="22">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="S47">
+      <c r="S49">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="T47" s="22">
+      <c r="T49" s="22">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="U47">
+      <c r="U49">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V47" s="22">
-        <f>SUM(V4:V46)</f>
+      <c r="V49" s="22">
+        <f>SUM(V4:V48)</f>
         <v>8</v>
       </c>
-      <c r="W47" s="22">
+      <c r="W49" s="22">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="X47">
+      <c r="X49">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="Y49" s="22">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="Z49">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="AA49" s="22">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="AB49">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AC49" s="22">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="Y47" s="22">
+      <c r="AD49" s="22">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="Z47">
+      <c r="AE49">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="AA47" s="22">
+      <c r="AF49" s="22">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="AB47">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AC47" s="22">
+      <c r="AG49">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="AD47" s="22">
+      <c r="AH49" s="22">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="AE47">
+      <c r="AI49">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="AF47" s="22">
+      <c r="AJ49" s="22">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="AG47">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AH47" s="22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AI47">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AJ47" s="22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AK47" s="22">
+      <c r="AK49" s="22">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="AL47">
+      <c r="AL49">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="AM47" s="22">
+      <c r="AM49" s="22">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="AN47">
+      <c r="AN49">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="AO47" s="22">
+      <c r="AO49" s="22">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="AP47">
+      <c r="AP49">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="AQ47" s="22">
-        <f>SUM(AQ4:AQ45)</f>
-        <v>223</v>
-      </c>
-      <c r="AR47" s="49"/>
-      <c r="AS47" s="49"/>
+      <c r="AQ49" s="22">
+        <f>SUM(AQ4:AQ47)</f>
+        <v>248</v>
+      </c>
+      <c r="AR49" s="49"/>
+      <c r="AS49" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4467,96 +4611,106 @@
     <mergeCell ref="AR6:AR7"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:N8 C10:N10 C12:N12">
-    <cfRule type="notContainsBlanks" dxfId="18" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="23">
       <formula>LEN(TRIM(C5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:AP8 C20:AP31 C35:AP43 C33:AP33 C10:AP10 C12:AP13 C45:AP45 C18:AP18">
-    <cfRule type="cellIs" dxfId="17" priority="20" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="C5:AP8 C22:AP33 C37:AP45 C35:AP35 C10:AP10 C12:AP13 C47:AP47 C20:AP20">
+    <cfRule type="cellIs" dxfId="19" priority="22" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47">
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
+  <conditionalFormatting sqref="B49">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
       <formula>300</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47:AP47">
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+  <conditionalFormatting sqref="C49:AP49">
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AP47">
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+  <conditionalFormatting sqref="AP49">
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:AP4">
-    <cfRule type="cellIs" dxfId="13" priority="16" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21:AP21">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36:AP36">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34:AP34">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:N9">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
+      <formula>LEN(TRIM(C9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:AP9">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:N11">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
+      <formula>LEN(TRIM(C11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:AP11">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46:AP46">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:AP19">
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:AP34">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32:AP32">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:N9">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
-      <formula>LEN(TRIM(C9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:AP9">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:N11">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
-      <formula>LEN(TRIM(C11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:AP11">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C44:AP44">
+  <conditionalFormatting sqref="C14:AP14">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17:AP17">
+  <conditionalFormatting sqref="C15:AP15">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:AP14">
+  <conditionalFormatting sqref="C16:AP16">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:AP15">
+  <conditionalFormatting sqref="C48:AP48">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16:AP16">
+  <conditionalFormatting sqref="C17:AP17">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46:AP46">
+  <conditionalFormatting sqref="C18:AP18">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
@@ -4568,7 +4722,7 @@
     <oddHeader>&amp;L&amp;F&amp;CDDC'App&amp;RJonathan Borel-Jaquet</oddHeader>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="AQ45 AQ29 AQ18 AQ13" formulaRange="1"/>
+    <ignoredError sqref="AQ47 AQ31 AQ20 AQ13" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Development of the educator appoitment page
</commit_message>
<xml_diff>
--- a/documentation/planning/planning_effectif_travail_de_diplome.xlsx
+++ b/documentation/planning/planning_effectif_travail_de_diplome.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bj-travail-diplome-2021\documentation\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C18114-CA35-4ED0-BE65-02FEA668CCFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EC7E8D-6441-4537-ADBF-90D0286A14A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -179,9 +179,6 @@
   </si>
   <si>
     <t>Fonctionnalités</t>
-  </si>
-  <si>
-    <t>Inscription</t>
   </si>
   <si>
     <t>Affichage calendrier avec rendez-vous</t>
@@ -243,9 +240,6 @@
     <t>Onglet rendez-vous autonome</t>
   </si>
   <si>
-    <t>Connexion</t>
-  </si>
-  <si>
     <t>Progressive web app</t>
   </si>
   <si>
@@ -298,6 +292,9 @@
   </si>
   <si>
     <t>Onglet inscription</t>
+  </si>
+  <si>
+    <t>Envoie d'e-mail</t>
   </si>
 </sst>
 </file>
@@ -846,7 +843,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1221,10 +1225,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BT49"/>
+  <dimension ref="A1:BT48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AD35" sqref="AD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1434,7 +1438,7 @@
         <v>23</v>
       </c>
       <c r="U2" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="V2" s="24" t="s">
         <v>35</v>
@@ -1455,7 +1459,7 @@
         <v>27</v>
       </c>
       <c r="AB2" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC2" s="23" t="s">
         <v>28</v>
@@ -1500,10 +1504,10 @@
         <v>43</v>
       </c>
       <c r="AQ2" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR2" s="66" t="s">
         <v>64</v>
-      </c>
-      <c r="AR2" s="66" t="s">
-        <v>65</v>
       </c>
       <c r="AS2" s="17">
         <v>8</v>
@@ -1517,7 +1521,7 @@
     </row>
     <row r="3" spans="1:72" s="16" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="37"/>
@@ -1573,7 +1577,7 @@
     </row>
     <row r="4" spans="1:72" s="40" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="41"/>
       <c r="C4" s="64"/>
@@ -1618,7 +1622,7 @@
       <c r="AP4" s="63"/>
       <c r="AQ4" s="41"/>
       <c r="AR4" s="72" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AS4" s="68">
         <v>3.125E-2</v>
@@ -1775,7 +1779,7 @@
         <v>12</v>
       </c>
       <c r="AR6" s="74" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS6" s="70">
         <v>300</v>
@@ -1847,7 +1851,7 @@
     </row>
     <row r="8" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="18">
         <v>8</v>
@@ -1909,7 +1913,7 @@
     </row>
     <row r="9" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9" s="18">
         <v>6</v>
@@ -1971,7 +1975,7 @@
     </row>
     <row r="10" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10" s="18">
         <v>6</v>
@@ -2033,7 +2037,7 @@
     </row>
     <row r="11" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11" s="18">
         <v>6</v>
@@ -2097,7 +2101,7 @@
     </row>
     <row r="12" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="18">
         <v>6</v>
@@ -2235,7 +2239,7 @@
     </row>
     <row r="14" spans="1:72" s="40" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="45" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B14" s="41"/>
       <c r="C14" s="64"/>
@@ -2311,7 +2315,7 @@
     </row>
     <row r="15" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B15" s="20">
         <v>4</v>
@@ -2367,7 +2371,7 @@
     </row>
     <row r="16" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B16" s="20">
         <v>4</v>
@@ -2423,7 +2427,7 @@
     </row>
     <row r="17" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B17" s="20">
         <v>4</v>
@@ -2479,7 +2483,7 @@
     </row>
     <row r="18" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B18" s="20">
         <v>4</v>
@@ -2535,7 +2539,7 @@
     </row>
     <row r="19" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B19" s="20">
         <v>4</v>
@@ -2669,7 +2673,7 @@
     </row>
     <row r="21" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="20">
         <v>4</v>
@@ -2757,7 +2761,9 @@
       <c r="AA22" s="58"/>
       <c r="AB22" s="59"/>
       <c r="AC22" s="58"/>
-      <c r="AD22" s="58"/>
+      <c r="AD22" s="58">
+        <v>2</v>
+      </c>
       <c r="AE22" s="58"/>
       <c r="AF22" s="58"/>
       <c r="AG22" s="58"/>
@@ -2772,7 +2778,7 @@
       <c r="AP22" s="60"/>
       <c r="AQ22" s="20">
         <f>SUM(C22:AP22)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AR22" s="49"/>
       <c r="AS22" s="49"/>
@@ -2833,7 +2839,7 @@
     </row>
     <row r="24" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B24" s="20">
         <v>8</v>
@@ -2864,7 +2870,9 @@
       <c r="Z24" s="58"/>
       <c r="AA24" s="58"/>
       <c r="AB24" s="59"/>
-      <c r="AC24" s="58"/>
+      <c r="AC24" s="58">
+        <v>2</v>
+      </c>
       <c r="AD24" s="58"/>
       <c r="AE24" s="58"/>
       <c r="AF24" s="58"/>
@@ -2880,7 +2888,7 @@
       <c r="AP24" s="60"/>
       <c r="AQ24" s="20">
         <f>SUM(C24:AP24)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR24" s="49"/>
       <c r="AS24" s="49"/>
@@ -2963,7 +2971,7 @@
     </row>
     <row r="26" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B26" s="20">
         <v>4</v>
@@ -2997,7 +3005,9 @@
       <c r="AA26" s="58"/>
       <c r="AB26" s="59"/>
       <c r="AC26" s="58"/>
-      <c r="AD26" s="58"/>
+      <c r="AD26" s="58">
+        <v>2</v>
+      </c>
       <c r="AE26" s="58"/>
       <c r="AF26" s="58"/>
       <c r="AG26" s="58"/>
@@ -3012,7 +3022,7 @@
       <c r="AP26" s="60"/>
       <c r="AQ26" s="20">
         <f>SUM(C26:AP26)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AR26" s="49"/>
       <c r="AS26" s="49"/>
@@ -3154,13 +3164,13 @@
       <c r="V29" s="58"/>
       <c r="W29" s="58"/>
       <c r="X29" s="58">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y29" s="58">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Z29" s="58">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA29" s="58">
         <v>3</v>
@@ -3182,7 +3192,7 @@
       <c r="AP29" s="60"/>
       <c r="AQ29" s="20">
         <f>SUM(C29:AP29)</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AR29" s="49"/>
       <c r="AS29" s="49"/>
@@ -3243,7 +3253,7 @@
     </row>
     <row r="31" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B31" s="20">
         <v>4</v>
@@ -3274,7 +3284,9 @@
       <c r="Z31" s="58"/>
       <c r="AA31" s="58"/>
       <c r="AB31" s="59"/>
-      <c r="AC31" s="58"/>
+      <c r="AC31" s="58">
+        <v>2</v>
+      </c>
       <c r="AD31" s="58"/>
       <c r="AE31" s="58"/>
       <c r="AF31" s="58"/>
@@ -3290,14 +3302,14 @@
       <c r="AP31" s="60"/>
       <c r="AQ31" s="20">
         <f t="shared" ref="AQ31" si="2">SUM(C31:AP31)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR31" s="49"/>
       <c r="AS31" s="49"/>
     </row>
     <row r="32" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B32" s="20">
         <v>4</v>
@@ -3427,7 +3439,7 @@
     </row>
     <row r="34" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B34" s="20">
         <v>8</v>
@@ -3475,7 +3487,7 @@
       <c r="AO34" s="58"/>
       <c r="AP34" s="60"/>
       <c r="AQ34" s="20">
-        <f t="shared" ref="AQ34:AQ43" si="3">SUM(C34:AP34)</f>
+        <f t="shared" ref="AQ34:AQ42" si="3">SUM(C34:AP34)</f>
         <v>6</v>
       </c>
       <c r="AR34" s="49"/>
@@ -3486,7 +3498,7 @@
         <v>53</v>
       </c>
       <c r="B35" s="20">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C35" s="65"/>
       <c r="D35" s="58"/>
@@ -3501,8 +3513,12 @@
       <c r="M35" s="58"/>
       <c r="N35" s="58"/>
       <c r="O35" s="58"/>
-      <c r="P35" s="58"/>
-      <c r="Q35" s="58"/>
+      <c r="P35" s="58">
+        <v>2</v>
+      </c>
+      <c r="Q35" s="58">
+        <v>4</v>
+      </c>
       <c r="R35" s="58"/>
       <c r="S35" s="58"/>
       <c r="T35" s="58"/>
@@ -3530,17 +3546,17 @@
       <c r="AP35" s="60"/>
       <c r="AQ35" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AR35" s="49"/>
       <c r="AS35" s="49"/>
     </row>
     <row r="36" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B36" s="20">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C36" s="65"/>
       <c r="D36" s="58"/>
@@ -3563,7 +3579,9 @@
       <c r="U36" s="59"/>
       <c r="V36" s="58"/>
       <c r="W36" s="58"/>
-      <c r="X36" s="58"/>
+      <c r="X36" s="58">
+        <v>1</v>
+      </c>
       <c r="Y36" s="58"/>
       <c r="Z36" s="58"/>
       <c r="AA36" s="58"/>
@@ -3583,18 +3601,18 @@
       <c r="AO36" s="58"/>
       <c r="AP36" s="60"/>
       <c r="AQ36" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="AQ36" si="4">SUM(C36:AP36)</f>
+        <v>1</v>
       </c>
       <c r="AR36" s="49"/>
       <c r="AS36" s="49"/>
     </row>
     <row r="37" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="B37" s="20">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C37" s="65"/>
       <c r="D37" s="58"/>
@@ -3609,12 +3627,8 @@
       <c r="M37" s="58"/>
       <c r="N37" s="58"/>
       <c r="O37" s="58"/>
-      <c r="P37" s="58">
-        <v>2</v>
-      </c>
-      <c r="Q37" s="58">
-        <v>4</v>
-      </c>
+      <c r="P37" s="58"/>
+      <c r="Q37" s="58"/>
       <c r="R37" s="58"/>
       <c r="S37" s="58"/>
       <c r="T37" s="58"/>
@@ -3642,17 +3656,17 @@
       <c r="AP37" s="60"/>
       <c r="AQ37" s="20">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AR37" s="49"/>
       <c r="AS37" s="49"/>
     </row>
     <row r="38" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="B38" s="20">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C38" s="65"/>
       <c r="D38" s="58"/>
@@ -3675,13 +3689,17 @@
       <c r="U38" s="59"/>
       <c r="V38" s="58"/>
       <c r="W38" s="58"/>
-      <c r="X38" s="58"/>
+      <c r="X38" s="58">
+        <v>1</v>
+      </c>
       <c r="Y38" s="58"/>
       <c r="Z38" s="58"/>
       <c r="AA38" s="58"/>
       <c r="AB38" s="59"/>
       <c r="AC38" s="58"/>
-      <c r="AD38" s="58"/>
+      <c r="AD38" s="58">
+        <v>2</v>
+      </c>
       <c r="AE38" s="58"/>
       <c r="AF38" s="58"/>
       <c r="AG38" s="58"/>
@@ -3696,7 +3714,7 @@
       <c r="AP38" s="60"/>
       <c r="AQ38" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR38" s="49"/>
       <c r="AS38" s="49"/>
@@ -3730,11 +3748,15 @@
       <c r="V39" s="58"/>
       <c r="W39" s="58"/>
       <c r="X39" s="58"/>
-      <c r="Y39" s="58"/>
+      <c r="Y39" s="58">
+        <v>1</v>
+      </c>
       <c r="Z39" s="58"/>
       <c r="AA39" s="58"/>
       <c r="AB39" s="59"/>
-      <c r="AC39" s="58"/>
+      <c r="AC39" s="58">
+        <v>2</v>
+      </c>
       <c r="AD39" s="58"/>
       <c r="AE39" s="58"/>
       <c r="AF39" s="58"/>
@@ -3750,14 +3772,14 @@
       <c r="AP39" s="60"/>
       <c r="AQ39" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR39" s="49"/>
       <c r="AS39" s="49"/>
     </row>
     <row r="40" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
-        <v>56</v>
+      <c r="A40" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="B40" s="20">
         <v>8</v>
@@ -3810,11 +3832,11 @@
       <c r="AS40" s="49"/>
     </row>
     <row r="41" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="10" t="s">
-        <v>59</v>
+      <c r="A41" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="B41" s="20">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C41" s="65"/>
       <c r="D41" s="58"/>
@@ -3839,7 +3861,9 @@
       <c r="W41" s="58"/>
       <c r="X41" s="58"/>
       <c r="Y41" s="58"/>
-      <c r="Z41" s="58"/>
+      <c r="Z41" s="58">
+        <v>1</v>
+      </c>
       <c r="AA41" s="58"/>
       <c r="AB41" s="59"/>
       <c r="AC41" s="58"/>
@@ -3858,17 +3882,17 @@
       <c r="AP41" s="60"/>
       <c r="AQ41" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR41" s="49"/>
       <c r="AS41" s="49"/>
     </row>
-    <row r="42" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B42" s="20">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C42" s="65"/>
       <c r="D42" s="58"/>
@@ -3917,691 +3941,637 @@
       <c r="AR42" s="49"/>
       <c r="AS42" s="49"/>
     </row>
-    <row r="43" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B43" s="20">
-        <v>10</v>
-      </c>
-      <c r="C43" s="65"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
-      <c r="K43" s="58"/>
-      <c r="L43" s="58"/>
-      <c r="M43" s="58"/>
-      <c r="N43" s="58"/>
-      <c r="O43" s="58"/>
-      <c r="P43" s="58"/>
-      <c r="Q43" s="58"/>
-      <c r="R43" s="58"/>
-      <c r="S43" s="58"/>
-      <c r="T43" s="58"/>
-      <c r="U43" s="59"/>
-      <c r="V43" s="58"/>
-      <c r="W43" s="58"/>
-      <c r="X43" s="58"/>
-      <c r="Y43" s="58"/>
-      <c r="Z43" s="58"/>
-      <c r="AA43" s="58"/>
-      <c r="AB43" s="59"/>
-      <c r="AC43" s="58"/>
-      <c r="AD43" s="58"/>
-      <c r="AE43" s="58"/>
-      <c r="AF43" s="58"/>
-      <c r="AG43" s="58"/>
-      <c r="AH43" s="58"/>
-      <c r="AI43" s="58"/>
-      <c r="AJ43" s="58"/>
-      <c r="AK43" s="58"/>
-      <c r="AL43" s="58"/>
-      <c r="AM43" s="58"/>
-      <c r="AN43" s="58"/>
-      <c r="AO43" s="58"/>
-      <c r="AP43" s="60"/>
-      <c r="AQ43" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+    <row r="43" spans="1:72" s="40" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="41"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
+      <c r="K43" s="39"/>
+      <c r="L43" s="39"/>
+      <c r="M43" s="39"/>
+      <c r="N43" s="39"/>
+      <c r="O43" s="39"/>
+      <c r="P43" s="39"/>
+      <c r="Q43" s="39"/>
+      <c r="R43" s="39"/>
+      <c r="S43" s="39"/>
+      <c r="T43" s="39"/>
+      <c r="U43" s="39"/>
+      <c r="V43" s="39"/>
+      <c r="W43" s="39"/>
+      <c r="X43" s="39"/>
+      <c r="Y43" s="39"/>
+      <c r="Z43" s="39"/>
+      <c r="AA43" s="39"/>
+      <c r="AB43" s="39"/>
+      <c r="AC43" s="39"/>
+      <c r="AD43" s="39"/>
+      <c r="AE43" s="39"/>
+      <c r="AF43" s="39"/>
+      <c r="AG43" s="39"/>
+      <c r="AH43" s="39"/>
+      <c r="AI43" s="39"/>
+      <c r="AJ43" s="39"/>
+      <c r="AK43" s="39"/>
+      <c r="AL43" s="39"/>
+      <c r="AM43" s="39"/>
+      <c r="AN43" s="39"/>
+      <c r="AO43" s="39"/>
+      <c r="AP43" s="52"/>
+      <c r="AQ43" s="54"/>
       <c r="AR43" s="49"/>
       <c r="AS43" s="49"/>
-    </row>
-    <row r="44" spans="1:72" s="40" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="41"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
-      <c r="M44" s="39"/>
-      <c r="N44" s="39"/>
-      <c r="O44" s="39"/>
-      <c r="P44" s="39"/>
-      <c r="Q44" s="39"/>
-      <c r="R44" s="39"/>
-      <c r="S44" s="39"/>
-      <c r="T44" s="39"/>
+      <c r="AT43" s="2"/>
+      <c r="AU43" s="2"/>
+      <c r="AV43" s="2"/>
+      <c r="AW43" s="2"/>
+      <c r="AX43" s="2"/>
+      <c r="AY43"/>
+      <c r="AZ43"/>
+      <c r="BA43"/>
+      <c r="BB43"/>
+      <c r="BC43"/>
+      <c r="BD43"/>
+      <c r="BE43"/>
+      <c r="BF43"/>
+      <c r="BG43"/>
+      <c r="BH43"/>
+      <c r="BI43"/>
+      <c r="BJ43"/>
+      <c r="BK43"/>
+      <c r="BL43"/>
+      <c r="BM43"/>
+      <c r="BN43"/>
+      <c r="BO43"/>
+      <c r="BP43"/>
+      <c r="BQ43"/>
+      <c r="BR43"/>
+      <c r="BS43"/>
+      <c r="BT43"/>
+    </row>
+    <row r="44" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="20">
+        <v>68</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1">
+        <v>1</v>
+      </c>
+      <c r="I44" s="1">
+        <v>1</v>
+      </c>
+      <c r="J44" s="1">
+        <v>1</v>
+      </c>
+      <c r="K44" s="1">
+        <v>1</v>
+      </c>
+      <c r="L44" s="1">
+        <v>1</v>
+      </c>
+      <c r="M44" s="1">
+        <v>1</v>
+      </c>
+      <c r="N44" s="1">
+        <v>1</v>
+      </c>
+      <c r="O44" s="1">
+        <v>1</v>
+      </c>
+      <c r="P44" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>1</v>
+      </c>
+      <c r="R44" s="1">
+        <v>3</v>
+      </c>
+      <c r="S44" s="1">
+        <v>1</v>
+      </c>
+      <c r="T44" s="1">
+        <v>1</v>
+      </c>
       <c r="U44" s="39"/>
-      <c r="V44" s="39"/>
-      <c r="W44" s="39"/>
-      <c r="X44" s="39"/>
-      <c r="Y44" s="39"/>
-      <c r="Z44" s="39"/>
-      <c r="AA44" s="39"/>
+      <c r="V44" s="1">
+        <v>1</v>
+      </c>
+      <c r="W44" s="1">
+        <v>1</v>
+      </c>
+      <c r="X44" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y44" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z44" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA44" s="1">
+        <v>1</v>
+      </c>
       <c r="AB44" s="39"/>
-      <c r="AC44" s="39"/>
-      <c r="AD44" s="39"/>
-      <c r="AE44" s="39"/>
-      <c r="AF44" s="39"/>
-      <c r="AG44" s="39"/>
-      <c r="AH44" s="39"/>
-      <c r="AI44" s="39"/>
-      <c r="AJ44" s="39"/>
-      <c r="AK44" s="39"/>
-      <c r="AL44" s="39"/>
-      <c r="AM44" s="39"/>
-      <c r="AN44" s="39"/>
-      <c r="AO44" s="39"/>
-      <c r="AP44" s="52"/>
-      <c r="AQ44" s="54"/>
+      <c r="AC44" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD44" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE44" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF44" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG44" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH44" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI44" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ44" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK44" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL44" s="1">
+        <v>7</v>
+      </c>
+      <c r="AM44" s="1">
+        <v>7</v>
+      </c>
+      <c r="AN44" s="1">
+        <v>7</v>
+      </c>
+      <c r="AO44" s="1">
+        <v>7</v>
+      </c>
+      <c r="AP44" s="1">
+        <v>3</v>
+      </c>
+      <c r="AQ44" s="13">
+        <f>SUM(C44:AP44)</f>
+        <v>70</v>
+      </c>
       <c r="AR44" s="49"/>
       <c r="AS44" s="49"/>
-      <c r="AT44" s="2"/>
-      <c r="AU44" s="2"/>
-      <c r="AV44" s="2"/>
-      <c r="AW44" s="2"/>
-      <c r="AX44" s="2"/>
-      <c r="AY44"/>
-      <c r="AZ44"/>
-      <c r="BA44"/>
-      <c r="BB44"/>
-      <c r="BC44"/>
-      <c r="BD44"/>
-      <c r="BE44"/>
-      <c r="BF44"/>
-      <c r="BG44"/>
-      <c r="BH44"/>
-      <c r="BI44"/>
-      <c r="BJ44"/>
-      <c r="BK44"/>
-      <c r="BL44"/>
-      <c r="BM44"/>
-      <c r="BN44"/>
-      <c r="BO44"/>
-      <c r="BP44"/>
-      <c r="BQ44"/>
-      <c r="BR44"/>
-      <c r="BS44"/>
-      <c r="BT44"/>
     </row>
     <row r="45" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B45" s="20">
         <v>68</v>
       </c>
-      <c r="C45" s="4">
-        <v>1</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1</v>
-      </c>
-      <c r="E45" s="1">
-        <v>1</v>
-      </c>
-      <c r="F45" s="1">
-        <v>1</v>
-      </c>
-      <c r="G45" s="1">
-        <v>1</v>
-      </c>
-      <c r="H45" s="1">
-        <v>1</v>
-      </c>
-      <c r="I45" s="1">
-        <v>1</v>
-      </c>
-      <c r="J45" s="1">
-        <v>1</v>
-      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
       <c r="K45" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L45" s="1">
-        <v>1</v>
-      </c>
-      <c r="M45" s="1">
-        <v>1</v>
-      </c>
-      <c r="N45" s="1">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
       <c r="O45" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P45" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q45" s="1">
-        <v>1</v>
-      </c>
-      <c r="R45" s="1">
-        <v>3</v>
-      </c>
-      <c r="S45" s="1">
-        <v>1</v>
-      </c>
-      <c r="T45" s="1">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
       <c r="U45" s="39"/>
       <c r="V45" s="1">
-        <v>1</v>
-      </c>
-      <c r="W45" s="1">
-        <v>1</v>
-      </c>
-      <c r="X45" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y45" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z45" s="1">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1"/>
+      <c r="Y45" s="1"/>
+      <c r="Z45" s="1"/>
       <c r="AA45" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AB45" s="39"/>
-      <c r="AC45" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD45" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE45" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF45" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG45" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH45" s="1">
-        <v>1</v>
-      </c>
-      <c r="AI45" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ45" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK45" s="1">
-        <v>5</v>
-      </c>
-      <c r="AL45" s="1">
-        <v>7</v>
-      </c>
-      <c r="AM45" s="1">
-        <v>7</v>
-      </c>
-      <c r="AN45" s="1">
-        <v>7</v>
-      </c>
-      <c r="AO45" s="1">
-        <v>7</v>
-      </c>
-      <c r="AP45" s="1">
-        <v>3</v>
-      </c>
+      <c r="AC45" s="1"/>
+      <c r="AD45" s="1"/>
+      <c r="AE45" s="1"/>
+      <c r="AF45" s="1"/>
+      <c r="AG45" s="1"/>
+      <c r="AH45" s="1"/>
+      <c r="AI45" s="1"/>
+      <c r="AJ45" s="1"/>
+      <c r="AK45" s="1"/>
+      <c r="AL45" s="1"/>
+      <c r="AM45" s="1"/>
+      <c r="AN45" s="1"/>
+      <c r="AO45" s="1"/>
+      <c r="AP45" s="1"/>
       <c r="AQ45" s="13">
         <f>SUM(C45:AP45)</f>
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="AR45" s="49"/>
       <c r="AS45" s="49"/>
     </row>
-    <row r="46" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B46" s="20">
-        <v>68</v>
-      </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
+    <row r="46" spans="1:72" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="21">
+        <v>38</v>
+      </c>
+      <c r="C46" s="4">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1</v>
+      </c>
+      <c r="G46" s="1">
+        <v>1</v>
+      </c>
+      <c r="H46" s="1">
+        <v>1</v>
+      </c>
+      <c r="I46" s="1">
+        <v>1</v>
+      </c>
+      <c r="J46" s="1">
+        <v>1</v>
+      </c>
       <c r="K46" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L46" s="1">
-        <v>4</v>
-      </c>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="M46" s="1">
+        <v>1</v>
+      </c>
+      <c r="N46" s="1">
+        <v>1</v>
+      </c>
       <c r="O46" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P46" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q46" s="1">
-        <v>2</v>
-      </c>
-      <c r="R46" s="1"/>
-      <c r="S46" s="1"/>
-      <c r="T46" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="R46" s="1">
+        <v>1</v>
+      </c>
+      <c r="S46" s="1">
+        <v>1</v>
+      </c>
+      <c r="T46" s="1">
+        <v>1</v>
+      </c>
       <c r="U46" s="39"/>
       <c r="V46" s="1">
-        <v>2</v>
-      </c>
-      <c r="W46" s="1"/>
-      <c r="X46" s="1"/>
-      <c r="Y46" s="1"/>
-      <c r="Z46" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="W46" s="1">
+        <v>1</v>
+      </c>
+      <c r="X46" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y46" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z46" s="1">
+        <v>1</v>
+      </c>
       <c r="AA46" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB46" s="39"/>
-      <c r="AC46" s="1"/>
-      <c r="AD46" s="1"/>
-      <c r="AE46" s="1"/>
-      <c r="AF46" s="1"/>
-      <c r="AG46" s="1"/>
-      <c r="AH46" s="1"/>
-      <c r="AI46" s="1"/>
-      <c r="AJ46" s="1"/>
-      <c r="AK46" s="1"/>
-      <c r="AL46" s="1"/>
-      <c r="AM46" s="1"/>
-      <c r="AN46" s="1"/>
-      <c r="AO46" s="1"/>
-      <c r="AP46" s="1"/>
-      <c r="AQ46" s="13">
+      <c r="AC46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ46" s="14">
         <f>SUM(C46:AP46)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="AR46" s="49"/>
       <c r="AS46" s="49"/>
     </row>
-    <row r="47" spans="1:72" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B47" s="21">
-        <v>38</v>
-      </c>
-      <c r="C47" s="4">
-        <v>1</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
-      <c r="E47" s="1">
-        <v>1</v>
-      </c>
-      <c r="F47" s="1">
-        <v>1</v>
-      </c>
-      <c r="G47" s="1">
-        <v>1</v>
-      </c>
-      <c r="H47" s="1">
-        <v>1</v>
-      </c>
-      <c r="I47" s="1">
-        <v>1</v>
-      </c>
-      <c r="J47" s="1">
-        <v>1</v>
-      </c>
-      <c r="K47" s="1">
-        <v>1</v>
-      </c>
-      <c r="L47" s="1">
-        <v>1</v>
-      </c>
-      <c r="M47" s="1">
-        <v>1</v>
-      </c>
-      <c r="N47" s="1">
-        <v>1</v>
-      </c>
-      <c r="O47" s="1">
-        <v>1</v>
-      </c>
-      <c r="P47" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q47" s="1">
-        <v>1</v>
-      </c>
-      <c r="R47" s="1">
-        <v>1</v>
-      </c>
-      <c r="S47" s="1">
-        <v>1</v>
-      </c>
-      <c r="T47" s="1">
-        <v>1</v>
-      </c>
-      <c r="U47" s="39"/>
-      <c r="V47" s="1">
-        <v>1</v>
-      </c>
-      <c r="W47" s="1">
-        <v>1</v>
-      </c>
-      <c r="X47" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y47" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB47" s="39"/>
-      <c r="AC47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AI47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AL47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AM47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AN47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AO47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AP47" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ47" s="14">
-        <f>SUM(C47:AP47)</f>
-        <v>38</v>
+    <row r="47" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="20">
+        <v>10</v>
+      </c>
+      <c r="C47" s="65"/>
+      <c r="D47" s="58"/>
+      <c r="E47" s="58"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="58"/>
+      <c r="I47" s="58"/>
+      <c r="J47" s="58"/>
+      <c r="K47" s="58"/>
+      <c r="L47" s="58"/>
+      <c r="M47" s="58"/>
+      <c r="N47" s="58"/>
+      <c r="O47" s="58"/>
+      <c r="P47" s="58"/>
+      <c r="Q47" s="58"/>
+      <c r="R47" s="58"/>
+      <c r="S47" s="58"/>
+      <c r="T47" s="58"/>
+      <c r="U47" s="59"/>
+      <c r="V47" s="58">
+        <v>2</v>
+      </c>
+      <c r="W47" s="58"/>
+      <c r="X47" s="58"/>
+      <c r="Y47" s="58"/>
+      <c r="Z47" s="58"/>
+      <c r="AA47" s="58"/>
+      <c r="AB47" s="59"/>
+      <c r="AC47" s="58"/>
+      <c r="AD47" s="58"/>
+      <c r="AE47" s="58"/>
+      <c r="AF47" s="58"/>
+      <c r="AG47" s="58"/>
+      <c r="AH47" s="58"/>
+      <c r="AI47" s="58"/>
+      <c r="AJ47" s="58"/>
+      <c r="AK47" s="58"/>
+      <c r="AL47" s="58"/>
+      <c r="AM47" s="58"/>
+      <c r="AN47" s="58"/>
+      <c r="AO47" s="58"/>
+      <c r="AP47" s="60"/>
+      <c r="AQ47" s="20">
+        <f t="shared" ref="AQ47" si="5">SUM(C47:AP47)</f>
+        <v>2</v>
       </c>
       <c r="AR47" s="49"/>
       <c r="AS47" s="49"/>
     </row>
-    <row r="48" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B48" s="20">
-        <v>10</v>
-      </c>
-      <c r="C48" s="65"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="58"/>
-      <c r="J48" s="58"/>
-      <c r="K48" s="58"/>
-      <c r="L48" s="58"/>
-      <c r="M48" s="58"/>
-      <c r="N48" s="58"/>
-      <c r="O48" s="58"/>
-      <c r="P48" s="58"/>
-      <c r="Q48" s="58"/>
-      <c r="R48" s="58"/>
-      <c r="S48" s="58"/>
-      <c r="T48" s="58"/>
-      <c r="U48" s="59"/>
-      <c r="V48" s="58">
+    <row r="48" spans="1:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="22">
+        <f t="shared" ref="B48:AP48" si="6">SUM(B4:B46)</f>
+        <v>384</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="D48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="F48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="H48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="I48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="K48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="M48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="O48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="R48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="T48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="U48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V48" s="22">
+        <f>SUM(V4:V47)</f>
+        <v>8</v>
+      </c>
+      <c r="W48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="X48">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="Y48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="Z48">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="AA48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="AB48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="AD48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="AE48">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="W48" s="58"/>
-      <c r="X48" s="58"/>
-      <c r="Y48" s="58"/>
-      <c r="Z48" s="58"/>
-      <c r="AA48" s="58"/>
-      <c r="AB48" s="59"/>
-      <c r="AC48" s="58"/>
-      <c r="AD48" s="58"/>
-      <c r="AE48" s="58"/>
-      <c r="AF48" s="58"/>
-      <c r="AG48" s="58"/>
-      <c r="AH48" s="58"/>
-      <c r="AI48" s="58"/>
-      <c r="AJ48" s="58"/>
-      <c r="AK48" s="58"/>
-      <c r="AL48" s="58"/>
-      <c r="AM48" s="58"/>
-      <c r="AN48" s="58"/>
-      <c r="AO48" s="58"/>
-      <c r="AP48" s="60"/>
-      <c r="AQ48" s="20">
-        <f t="shared" ref="AQ48" si="4">SUM(C48:AP48)</f>
+      <c r="AF48" s="22">
+        <f t="shared" si="6"/>
         <v>2</v>
+      </c>
+      <c r="AG48">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="AH48" s="22">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="AI48">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="AJ48" s="22">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="AK48" s="22">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AL48">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="AM48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="AN48">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="AO48" s="22">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="AP48">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AQ48" s="22">
+        <f>SUM(AQ4:AQ46)</f>
+        <v>261</v>
       </c>
       <c r="AR48" s="49"/>
       <c r="AS48" s="49"/>
-    </row>
-    <row r="49" spans="2:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="22">
-        <f t="shared" ref="B49:AP49" si="5">SUM(B4:B47)</f>
-        <v>388</v>
-      </c>
-      <c r="C49">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="D49" s="22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E49">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="F49" s="22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="G49">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="H49" s="22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="I49" s="22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="J49">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="K49" s="22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="L49">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="M49" s="22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="N49">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="O49" s="22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="P49" s="22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="Q49">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="R49" s="22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="S49">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="T49" s="22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="U49">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V49" s="22">
-        <f>SUM(V4:V48)</f>
-        <v>8</v>
-      </c>
-      <c r="W49" s="22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="X49">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="Y49" s="22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="Z49">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="AA49" s="22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="AB49">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AC49" s="22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AD49" s="22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AE49">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AF49" s="22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AG49">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AH49" s="22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AI49">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AJ49" s="22">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="AK49" s="22">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="AL49">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="AM49" s="22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="AN49">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="AO49" s="22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="AP49">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="AQ49" s="22">
-        <f>SUM(AQ4:AQ47)</f>
-        <v>248</v>
-      </c>
-      <c r="AR49" s="49"/>
-      <c r="AS49" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4611,106 +4581,106 @@
     <mergeCell ref="AR6:AR7"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:N8 C10:N10 C12:N12">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="23">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="24">
       <formula>LEN(TRIM(C5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:AP8 C22:AP33 C37:AP45 C35:AP35 C10:AP10 C12:AP13 C47:AP47 C20:AP20">
-    <cfRule type="cellIs" dxfId="19" priority="22" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="C5:AP8 C22:AP33 C35:AP35 C10:AP10 C12:AP13 C46:AP46 C20:AP20 C37:AP44">
+    <cfRule type="cellIs" dxfId="20" priority="23" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49">
-    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+  <conditionalFormatting sqref="B48">
+    <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
       <formula>300</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:AP49">
-    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
+  <conditionalFormatting sqref="C48:AP48">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AP49">
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
+  <conditionalFormatting sqref="AP48">
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:AP4">
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:AP21">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34:AP34">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:N9">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
+      <formula>LEN(TRIM(C9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:AP9">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:N11">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+      <formula>LEN(TRIM(C11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:AP11">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45:AP45">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19:AP19">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:AP14">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:AP15">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:AP16">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47:AP47">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:AP17">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:AP18">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:AP36">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:AP34">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:N9">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
-      <formula>LEN(TRIM(C9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:AP9">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:N11">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
-      <formula>LEN(TRIM(C11))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:AP11">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C46:AP46">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19:AP19">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14:AP14">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15:AP15">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16:AP16">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48:AP48">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17:AP17">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18:AP18">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
@@ -4722,7 +4692,7 @@
     <oddHeader>&amp;L&amp;F&amp;CDDC'App&amp;RJonathan Borel-Jaquet</oddHeader>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="AQ47 AQ31 AQ20 AQ13" formulaRange="1"/>
+    <ignoredError sqref="AQ46 AQ31 AQ20 AQ13" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Documentation and reCAPTCHA feature
</commit_message>
<xml_diff>
--- a/documentation/planning/planning_effectif_travail_de_diplome.xlsx
+++ b/documentation/planning/planning_effectif_travail_de_diplome.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bj-travail-diplome-2021\documentation\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84199E21-6FC4-468F-929E-09458E1A7A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C9554B-0848-4DBE-938D-48810898F50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -229,9 +229,6 @@
   </si>
   <si>
     <t>Absence</t>
-  </si>
-  <si>
-    <t>Onglet rendez-vous autonome</t>
   </si>
   <si>
     <t>Progressive web app</t>
@@ -834,7 +831,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="21">
     <dxf>
       <fill>
         <patternFill>
@@ -932,13 +929,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1216,10 +1206,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BT46"/>
+  <dimension ref="A1:BT44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1729,7 +1719,7 @@
         <v>3</v>
       </c>
       <c r="J6" s="55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K6" s="55"/>
       <c r="L6" s="55">
@@ -1767,7 +1757,7 @@
       <c r="AP6" s="59"/>
       <c r="AQ6" s="19">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AR6" s="73" t="s">
         <v>60</v>
@@ -1797,7 +1787,7 @@
         <v>3</v>
       </c>
       <c r="J7" s="55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K7" s="55">
         <v>2</v>
@@ -1835,7 +1825,7 @@
       <c r="AP7" s="59"/>
       <c r="AQ7" s="19">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AR7" s="72"/>
       <c r="AS7" s="70"/>
@@ -1904,7 +1894,7 @@
     </row>
     <row r="9" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="17">
         <v>6</v>
@@ -1966,7 +1956,7 @@
     </row>
     <row r="10" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="17">
         <v>6</v>
@@ -2028,7 +2018,7 @@
     </row>
     <row r="11" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="17">
         <v>6</v>
@@ -2230,7 +2220,7 @@
     </row>
     <row r="14" spans="1:72" s="39" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="40"/>
       <c r="C14" s="63"/>
@@ -2306,7 +2296,7 @@
     </row>
     <row r="15" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="19">
         <v>4</v>
@@ -2362,7 +2352,7 @@
     </row>
     <row r="16" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" s="19">
         <v>4</v>
@@ -2418,7 +2408,7 @@
     </row>
     <row r="17" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B17" s="19">
         <v>4</v>
@@ -2474,7 +2464,7 @@
     </row>
     <row r="18" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="19">
         <v>4</v>
@@ -2530,7 +2520,7 @@
     </row>
     <row r="19" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" s="19">
         <v>4</v>
@@ -2569,7 +2559,9 @@
       <c r="AD19" s="57"/>
       <c r="AE19" s="57"/>
       <c r="AF19" s="57"/>
-      <c r="AG19" s="57"/>
+      <c r="AG19" s="57">
+        <v>3</v>
+      </c>
       <c r="AH19" s="57"/>
       <c r="AI19" s="57"/>
       <c r="AJ19" s="57"/>
@@ -2581,7 +2573,7 @@
       <c r="AP19" s="59"/>
       <c r="AQ19" s="19">
         <f>SUM(C19:AP19)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AR19" s="48"/>
       <c r="AS19" s="48"/>
@@ -2664,7 +2656,7 @@
     </row>
     <row r="21" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B21" s="19">
         <v>4</v>
@@ -2689,14 +2681,18 @@
       <c r="T21" s="57"/>
       <c r="U21" s="58"/>
       <c r="V21" s="57"/>
-      <c r="W21" s="57"/>
+      <c r="W21" s="57">
+        <v>3</v>
+      </c>
       <c r="X21" s="57"/>
       <c r="Y21" s="57"/>
       <c r="Z21" s="57"/>
       <c r="AA21" s="57"/>
       <c r="AB21" s="58"/>
       <c r="AC21" s="57"/>
-      <c r="AD21" s="57"/>
+      <c r="AD21" s="57">
+        <v>2</v>
+      </c>
       <c r="AE21" s="57"/>
       <c r="AF21" s="57"/>
       <c r="AG21" s="57"/>
@@ -2711,17 +2707,17 @@
       <c r="AP21" s="59"/>
       <c r="AQ21" s="19">
         <f>SUM(C21:AP21)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AR21" s="48"/>
       <c r="AS21" s="48"/>
     </row>
     <row r="22" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>46</v>
+      <c r="A22" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="B22" s="19">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C22" s="64"/>
       <c r="D22" s="57"/>
@@ -2743,18 +2739,16 @@
       <c r="T22" s="57"/>
       <c r="U22" s="58"/>
       <c r="V22" s="57"/>
-      <c r="W22" s="57">
-        <v>3</v>
-      </c>
+      <c r="W22" s="57"/>
       <c r="X22" s="57"/>
       <c r="Y22" s="57"/>
       <c r="Z22" s="57"/>
       <c r="AA22" s="57"/>
       <c r="AB22" s="58"/>
-      <c r="AC22" s="57"/>
-      <c r="AD22" s="57">
+      <c r="AC22" s="57">
         <v>2</v>
       </c>
+      <c r="AD22" s="57"/>
       <c r="AE22" s="57"/>
       <c r="AF22" s="57"/>
       <c r="AG22" s="57"/>
@@ -2769,71 +2763,93 @@
       <c r="AP22" s="59"/>
       <c r="AQ22" s="19">
         <f>SUM(C22:AP22)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AR22" s="48"/>
       <c r="AS22" s="48"/>
     </row>
-    <row r="23" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="19">
-        <v>8</v>
-      </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="57"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="57"/>
-      <c r="O23" s="57"/>
-      <c r="P23" s="57"/>
-      <c r="Q23" s="57"/>
-      <c r="R23" s="57"/>
-      <c r="S23" s="57"/>
-      <c r="T23" s="57"/>
+    <row r="23" spans="1:72" s="39" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="40"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="58"/>
+      <c r="N23" s="58"/>
+      <c r="O23" s="58"/>
+      <c r="P23" s="58"/>
+      <c r="Q23" s="58"/>
+      <c r="R23" s="58"/>
+      <c r="S23" s="58"/>
+      <c r="T23" s="58"/>
       <c r="U23" s="58"/>
-      <c r="V23" s="57"/>
-      <c r="W23" s="57"/>
-      <c r="X23" s="57"/>
-      <c r="Y23" s="57"/>
-      <c r="Z23" s="57"/>
-      <c r="AA23" s="57"/>
+      <c r="V23" s="58"/>
+      <c r="W23" s="58"/>
+      <c r="X23" s="58"/>
+      <c r="Y23" s="58"/>
+      <c r="Z23" s="58"/>
+      <c r="AA23" s="58"/>
       <c r="AB23" s="58"/>
-      <c r="AC23" s="57"/>
-      <c r="AD23" s="57"/>
-      <c r="AE23" s="57"/>
-      <c r="AF23" s="57"/>
-      <c r="AG23" s="57"/>
-      <c r="AH23" s="57"/>
-      <c r="AI23" s="57"/>
-      <c r="AJ23" s="57"/>
-      <c r="AK23" s="57"/>
-      <c r="AL23" s="57"/>
-      <c r="AM23" s="57"/>
-      <c r="AN23" s="57"/>
-      <c r="AO23" s="57"/>
-      <c r="AP23" s="59"/>
-      <c r="AQ23" s="19">
-        <f>SUM(C23:AP23)</f>
-        <v>0</v>
-      </c>
+      <c r="AC23" s="58"/>
+      <c r="AD23" s="58"/>
+      <c r="AE23" s="58"/>
+      <c r="AF23" s="58"/>
+      <c r="AG23" s="58"/>
+      <c r="AH23" s="58"/>
+      <c r="AI23" s="58"/>
+      <c r="AJ23" s="58"/>
+      <c r="AK23" s="58"/>
+      <c r="AL23" s="58"/>
+      <c r="AM23" s="58"/>
+      <c r="AN23" s="58"/>
+      <c r="AO23" s="58"/>
+      <c r="AP23" s="62"/>
+      <c r="AQ23" s="40"/>
       <c r="AR23" s="48"/>
       <c r="AS23" s="48"/>
+      <c r="AT23" s="2"/>
+      <c r="AU23" s="2"/>
+      <c r="AV23" s="2"/>
+      <c r="AW23" s="2"/>
+      <c r="AX23" s="2"/>
+      <c r="AY23"/>
+      <c r="AZ23"/>
+      <c r="BA23"/>
+      <c r="BB23"/>
+      <c r="BC23"/>
+      <c r="BD23"/>
+      <c r="BE23"/>
+      <c r="BF23"/>
+      <c r="BG23"/>
+      <c r="BH23"/>
+      <c r="BI23"/>
+      <c r="BJ23"/>
+      <c r="BK23"/>
+      <c r="BL23"/>
+      <c r="BM23"/>
+      <c r="BN23"/>
+      <c r="BO23"/>
+      <c r="BP23"/>
+      <c r="BQ23"/>
+      <c r="BR23"/>
+      <c r="BS23"/>
+      <c r="BT23"/>
     </row>
     <row r="24" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>70</v>
+      <c r="A24" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="B24" s="19">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C24" s="64"/>
       <c r="D24" s="57"/>
@@ -2855,16 +2871,18 @@
       <c r="T24" s="57"/>
       <c r="U24" s="58"/>
       <c r="V24" s="57"/>
-      <c r="W24" s="57"/>
+      <c r="W24" s="57">
+        <v>3</v>
+      </c>
       <c r="X24" s="57"/>
       <c r="Y24" s="57"/>
       <c r="Z24" s="57"/>
       <c r="AA24" s="57"/>
       <c r="AB24" s="58"/>
-      <c r="AC24" s="57">
+      <c r="AC24" s="57"/>
+      <c r="AD24" s="57">
         <v>2</v>
       </c>
-      <c r="AD24" s="57"/>
       <c r="AE24" s="57"/>
       <c r="AF24" s="57"/>
       <c r="AG24" s="57"/>
@@ -2879,90 +2897,72 @@
       <c r="AP24" s="59"/>
       <c r="AQ24" s="19">
         <f>SUM(C24:AP24)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AR24" s="48"/>
       <c r="AS24" s="48"/>
     </row>
-    <row r="25" spans="1:72" s="39" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="58"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="58"/>
-      <c r="M25" s="58"/>
-      <c r="N25" s="58"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="58"/>
-      <c r="R25" s="58"/>
-      <c r="S25" s="58"/>
-      <c r="T25" s="58"/>
+    <row r="25" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="19">
+        <v>4</v>
+      </c>
+      <c r="C25" s="64"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="57"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="57"/>
+      <c r="P25" s="57"/>
+      <c r="Q25" s="57"/>
+      <c r="R25" s="57"/>
+      <c r="S25" s="57"/>
+      <c r="T25" s="57"/>
       <c r="U25" s="58"/>
-      <c r="V25" s="58"/>
-      <c r="W25" s="58"/>
-      <c r="X25" s="58"/>
-      <c r="Y25" s="58"/>
-      <c r="Z25" s="58"/>
-      <c r="AA25" s="58"/>
+      <c r="V25" s="57"/>
+      <c r="W25" s="57"/>
+      <c r="X25" s="57"/>
+      <c r="Y25" s="57"/>
+      <c r="Z25" s="57"/>
+      <c r="AA25" s="57"/>
       <c r="AB25" s="58"/>
-      <c r="AC25" s="58"/>
-      <c r="AD25" s="58"/>
-      <c r="AE25" s="58"/>
-      <c r="AF25" s="58"/>
-      <c r="AG25" s="58"/>
-      <c r="AH25" s="58"/>
-      <c r="AI25" s="58"/>
-      <c r="AJ25" s="58"/>
-      <c r="AK25" s="58"/>
-      <c r="AL25" s="58"/>
-      <c r="AM25" s="58"/>
-      <c r="AN25" s="58"/>
-      <c r="AO25" s="58"/>
-      <c r="AP25" s="62"/>
-      <c r="AQ25" s="40"/>
+      <c r="AC25" s="57"/>
+      <c r="AD25" s="57"/>
+      <c r="AE25" s="57">
+        <v>3</v>
+      </c>
+      <c r="AF25" s="57">
+        <v>2</v>
+      </c>
+      <c r="AG25" s="57"/>
+      <c r="AH25" s="57"/>
+      <c r="AI25" s="57"/>
+      <c r="AJ25" s="57"/>
+      <c r="AK25" s="57"/>
+      <c r="AL25" s="57"/>
+      <c r="AM25" s="57"/>
+      <c r="AN25" s="57"/>
+      <c r="AO25" s="57"/>
+      <c r="AP25" s="59"/>
+      <c r="AQ25" s="19">
+        <f>SUM(C25:AP25)</f>
+        <v>5</v>
+      </c>
       <c r="AR25" s="48"/>
       <c r="AS25" s="48"/>
-      <c r="AT25" s="2"/>
-      <c r="AU25" s="2"/>
-      <c r="AV25" s="2"/>
-      <c r="AW25" s="2"/>
-      <c r="AX25" s="2"/>
-      <c r="AY25"/>
-      <c r="AZ25"/>
-      <c r="BA25"/>
-      <c r="BB25"/>
-      <c r="BC25"/>
-      <c r="BD25"/>
-      <c r="BE25"/>
-      <c r="BF25"/>
-      <c r="BG25"/>
-      <c r="BH25"/>
-      <c r="BI25"/>
-      <c r="BJ25"/>
-      <c r="BK25"/>
-      <c r="BL25"/>
-      <c r="BM25"/>
-      <c r="BN25"/>
-      <c r="BO25"/>
-      <c r="BP25"/>
-      <c r="BQ25"/>
-      <c r="BR25"/>
-      <c r="BS25"/>
-      <c r="BT25"/>
     </row>
     <row r="26" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="B26" s="19">
         <v>4</v>
@@ -2987,18 +2987,22 @@
       <c r="T26" s="57"/>
       <c r="U26" s="58"/>
       <c r="V26" s="57"/>
-      <c r="W26" s="57">
+      <c r="W26" s="57"/>
+      <c r="X26" s="57">
+        <v>2</v>
+      </c>
+      <c r="Y26" s="57">
+        <v>2</v>
+      </c>
+      <c r="Z26" s="57">
+        <v>5</v>
+      </c>
+      <c r="AA26" s="57">
         <v>3</v>
       </c>
-      <c r="X26" s="57"/>
-      <c r="Y26" s="57"/>
-      <c r="Z26" s="57"/>
-      <c r="AA26" s="57"/>
       <c r="AB26" s="58"/>
       <c r="AC26" s="57"/>
-      <c r="AD26" s="57">
-        <v>2</v>
-      </c>
+      <c r="AD26" s="57"/>
       <c r="AE26" s="57"/>
       <c r="AF26" s="57"/>
       <c r="AG26" s="57"/>
@@ -3013,14 +3017,14 @@
       <c r="AP26" s="59"/>
       <c r="AQ26" s="19">
         <f>SUM(C26:AP26)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AR26" s="48"/>
       <c r="AS26" s="48"/>
     </row>
     <row r="27" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="B27" s="19">
         <v>4</v>
@@ -3053,10 +3057,10 @@
       <c r="AB27" s="58"/>
       <c r="AC27" s="57"/>
       <c r="AD27" s="57"/>
-      <c r="AE27" s="57">
-        <v>3</v>
-      </c>
-      <c r="AF27" s="57"/>
+      <c r="AE27" s="57"/>
+      <c r="AF27" s="57">
+        <v>4</v>
+      </c>
       <c r="AG27" s="57"/>
       <c r="AH27" s="57"/>
       <c r="AI27" s="57"/>
@@ -3068,15 +3072,15 @@
       <c r="AO27" s="57"/>
       <c r="AP27" s="59"/>
       <c r="AQ27" s="19">
-        <f>SUM(C27:AP27)</f>
-        <v>3</v>
+        <f t="shared" ref="AQ27" si="2">SUM(C27:AP27)</f>
+        <v>4</v>
       </c>
       <c r="AR27" s="48"/>
       <c r="AS27" s="48"/>
     </row>
-    <row r="28" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="B28" s="19">
         <v>4</v>
@@ -3102,22 +3106,18 @@
       <c r="U28" s="58"/>
       <c r="V28" s="57"/>
       <c r="W28" s="57"/>
-      <c r="X28" s="57">
+      <c r="X28" s="57"/>
+      <c r="Y28" s="57"/>
+      <c r="Z28" s="57"/>
+      <c r="AA28" s="57"/>
+      <c r="AB28" s="58"/>
+      <c r="AC28" s="57">
         <v>2</v>
       </c>
-      <c r="Y28" s="57">
-        <v>2</v>
-      </c>
-      <c r="Z28" s="57">
-        <v>5</v>
-      </c>
-      <c r="AA28" s="57">
+      <c r="AD28" s="57"/>
+      <c r="AE28" s="57">
         <v>3</v>
       </c>
-      <c r="AB28" s="58"/>
-      <c r="AC28" s="57"/>
-      <c r="AD28" s="57"/>
-      <c r="AE28" s="57"/>
       <c r="AF28" s="57"/>
       <c r="AG28" s="57"/>
       <c r="AH28" s="57"/>
@@ -3130,74 +3130,94 @@
       <c r="AO28" s="57"/>
       <c r="AP28" s="59"/>
       <c r="AQ28" s="19">
-        <f>SUM(C28:AP28)</f>
-        <v>12</v>
+        <f t="shared" ref="AQ28" si="3">SUM(C28:AP28)</f>
+        <v>5</v>
       </c>
       <c r="AR28" s="48"/>
       <c r="AS28" s="48"/>
     </row>
-    <row r="29" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="19">
-        <v>4</v>
-      </c>
-      <c r="C29" s="64"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="57"/>
-      <c r="K29" s="57"/>
-      <c r="L29" s="57"/>
-      <c r="M29" s="57"/>
-      <c r="N29" s="57"/>
-      <c r="O29" s="57"/>
-      <c r="P29" s="57"/>
-      <c r="Q29" s="57"/>
-      <c r="R29" s="57"/>
-      <c r="S29" s="57"/>
-      <c r="T29" s="57"/>
+    <row r="29" spans="1:72" s="39" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="40"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="58"/>
+      <c r="N29" s="58"/>
+      <c r="O29" s="58"/>
+      <c r="P29" s="58"/>
+      <c r="Q29" s="58"/>
+      <c r="R29" s="58"/>
+      <c r="S29" s="58"/>
+      <c r="T29" s="58"/>
       <c r="U29" s="58"/>
-      <c r="V29" s="57"/>
-      <c r="W29" s="57"/>
-      <c r="X29" s="57"/>
-      <c r="Y29" s="57"/>
-      <c r="Z29" s="57"/>
-      <c r="AA29" s="57"/>
+      <c r="V29" s="58"/>
+      <c r="W29" s="58"/>
+      <c r="X29" s="58"/>
+      <c r="Y29" s="58"/>
+      <c r="Z29" s="58"/>
+      <c r="AA29" s="58"/>
       <c r="AB29" s="58"/>
-      <c r="AC29" s="57">
-        <v>2</v>
-      </c>
-      <c r="AD29" s="57"/>
-      <c r="AE29" s="57"/>
-      <c r="AF29" s="57"/>
-      <c r="AG29" s="57"/>
-      <c r="AH29" s="57"/>
-      <c r="AI29" s="57"/>
-      <c r="AJ29" s="57"/>
-      <c r="AK29" s="57"/>
-      <c r="AL29" s="57"/>
-      <c r="AM29" s="57"/>
-      <c r="AN29" s="57"/>
-      <c r="AO29" s="57"/>
-      <c r="AP29" s="59"/>
-      <c r="AQ29" s="19">
-        <f t="shared" ref="AQ29" si="2">SUM(C29:AP29)</f>
-        <v>2</v>
-      </c>
+      <c r="AC29" s="58"/>
+      <c r="AD29" s="58"/>
+      <c r="AE29" s="58"/>
+      <c r="AF29" s="58"/>
+      <c r="AG29" s="58"/>
+      <c r="AH29" s="58"/>
+      <c r="AI29" s="58"/>
+      <c r="AJ29" s="58"/>
+      <c r="AK29" s="58"/>
+      <c r="AL29" s="58"/>
+      <c r="AM29" s="58"/>
+      <c r="AN29" s="58"/>
+      <c r="AO29" s="58"/>
+      <c r="AP29" s="62"/>
+      <c r="AQ29" s="40"/>
       <c r="AR29" s="48"/>
       <c r="AS29" s="48"/>
+      <c r="AT29" s="2"/>
+      <c r="AU29" s="2"/>
+      <c r="AV29" s="2"/>
+      <c r="AW29" s="2"/>
+      <c r="AX29" s="2"/>
+      <c r="AY29"/>
+      <c r="AZ29"/>
+      <c r="BA29"/>
+      <c r="BB29"/>
+      <c r="BC29"/>
+      <c r="BD29"/>
+      <c r="BE29"/>
+      <c r="BF29"/>
+      <c r="BG29"/>
+      <c r="BH29"/>
+      <c r="BI29"/>
+      <c r="BJ29"/>
+      <c r="BK29"/>
+      <c r="BL29"/>
+      <c r="BM29"/>
+      <c r="BN29"/>
+      <c r="BO29"/>
+      <c r="BP29"/>
+      <c r="BQ29"/>
+      <c r="BR29"/>
+      <c r="BS29"/>
+      <c r="BT29"/>
     </row>
-    <row r="30" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="B30" s="19">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C30" s="64"/>
       <c r="D30" s="57"/>
@@ -3216,7 +3236,9 @@
       <c r="Q30" s="57"/>
       <c r="R30" s="57"/>
       <c r="S30" s="57"/>
-      <c r="T30" s="57"/>
+      <c r="T30" s="57">
+        <v>6</v>
+      </c>
       <c r="U30" s="58"/>
       <c r="V30" s="57"/>
       <c r="W30" s="57"/>
@@ -3225,13 +3247,9 @@
       <c r="Z30" s="57"/>
       <c r="AA30" s="57"/>
       <c r="AB30" s="58"/>
-      <c r="AC30" s="57">
-        <v>2</v>
-      </c>
+      <c r="AC30" s="57"/>
       <c r="AD30" s="57"/>
-      <c r="AE30" s="57">
-        <v>3</v>
-      </c>
+      <c r="AE30" s="57"/>
       <c r="AF30" s="57"/>
       <c r="AG30" s="57"/>
       <c r="AH30" s="57"/>
@@ -3244,91 +3262,73 @@
       <c r="AO30" s="57"/>
       <c r="AP30" s="59"/>
       <c r="AQ30" s="19">
-        <f t="shared" ref="AQ30" si="3">SUM(C30:AP30)</f>
-        <v>5</v>
+        <f t="shared" ref="AQ30:AQ38" si="4">SUM(C30:AP30)</f>
+        <v>6</v>
       </c>
       <c r="AR30" s="48"/>
       <c r="AS30" s="48"/>
     </row>
-    <row r="31" spans="1:72" s="39" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
-      <c r="K31" s="58"/>
-      <c r="L31" s="58"/>
-      <c r="M31" s="58"/>
-      <c r="N31" s="58"/>
-      <c r="O31" s="58"/>
-      <c r="P31" s="58"/>
-      <c r="Q31" s="58"/>
-      <c r="R31" s="58"/>
-      <c r="S31" s="58"/>
-      <c r="T31" s="58"/>
+    <row r="31" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="19">
+        <v>8</v>
+      </c>
+      <c r="C31" s="64"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="57"/>
+      <c r="O31" s="57"/>
+      <c r="P31" s="57">
+        <v>2</v>
+      </c>
+      <c r="Q31" s="57">
+        <v>4</v>
+      </c>
+      <c r="R31" s="57"/>
+      <c r="S31" s="57"/>
+      <c r="T31" s="57"/>
       <c r="U31" s="58"/>
-      <c r="V31" s="58"/>
-      <c r="W31" s="58"/>
-      <c r="X31" s="58"/>
-      <c r="Y31" s="58"/>
-      <c r="Z31" s="58"/>
-      <c r="AA31" s="58"/>
+      <c r="V31" s="57"/>
+      <c r="W31" s="57"/>
+      <c r="X31" s="57"/>
+      <c r="Y31" s="57"/>
+      <c r="Z31" s="57"/>
+      <c r="AA31" s="57"/>
       <c r="AB31" s="58"/>
-      <c r="AC31" s="58"/>
-      <c r="AD31" s="58"/>
-      <c r="AE31" s="58"/>
-      <c r="AF31" s="58"/>
-      <c r="AG31" s="58"/>
-      <c r="AH31" s="58"/>
-      <c r="AI31" s="58"/>
-      <c r="AJ31" s="58"/>
-      <c r="AK31" s="58"/>
-      <c r="AL31" s="58"/>
-      <c r="AM31" s="58"/>
-      <c r="AN31" s="58"/>
-      <c r="AO31" s="58"/>
-      <c r="AP31" s="62"/>
-      <c r="AQ31" s="40"/>
+      <c r="AC31" s="57"/>
+      <c r="AD31" s="57"/>
+      <c r="AE31" s="57"/>
+      <c r="AF31" s="57"/>
+      <c r="AG31" s="57"/>
+      <c r="AH31" s="57"/>
+      <c r="AI31" s="57"/>
+      <c r="AJ31" s="57"/>
+      <c r="AK31" s="57"/>
+      <c r="AL31" s="57"/>
+      <c r="AM31" s="57"/>
+      <c r="AN31" s="57"/>
+      <c r="AO31" s="57"/>
+      <c r="AP31" s="59"/>
+      <c r="AQ31" s="19">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
       <c r="AR31" s="48"/>
       <c r="AS31" s="48"/>
-      <c r="AT31" s="2"/>
-      <c r="AU31" s="2"/>
-      <c r="AV31" s="2"/>
-      <c r="AW31" s="2"/>
-      <c r="AX31" s="2"/>
-      <c r="AY31"/>
-      <c r="AZ31"/>
-      <c r="BA31"/>
-      <c r="BB31"/>
-      <c r="BC31"/>
-      <c r="BD31"/>
-      <c r="BE31"/>
-      <c r="BF31"/>
-      <c r="BG31"/>
-      <c r="BH31"/>
-      <c r="BI31"/>
-      <c r="BJ31"/>
-      <c r="BK31"/>
-      <c r="BL31"/>
-      <c r="BM31"/>
-      <c r="BN31"/>
-      <c r="BO31"/>
-      <c r="BP31"/>
-      <c r="BQ31"/>
-      <c r="BR31"/>
-      <c r="BS31"/>
-      <c r="BT31"/>
     </row>
     <row r="32" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B32" s="19">
         <v>8</v>
@@ -3350,13 +3350,13 @@
       <c r="Q32" s="57"/>
       <c r="R32" s="57"/>
       <c r="S32" s="57"/>
-      <c r="T32" s="57">
-        <v>6</v>
-      </c>
+      <c r="T32" s="57"/>
       <c r="U32" s="58"/>
       <c r="V32" s="57"/>
       <c r="W32" s="57"/>
-      <c r="X32" s="57"/>
+      <c r="X32" s="57">
+        <v>1</v>
+      </c>
       <c r="Y32" s="57"/>
       <c r="Z32" s="57"/>
       <c r="AA32" s="57"/>
@@ -3376,18 +3376,18 @@
       <c r="AO32" s="57"/>
       <c r="AP32" s="59"/>
       <c r="AQ32" s="19">
-        <f t="shared" ref="AQ32:AQ40" si="4">SUM(C32:AP32)</f>
-        <v>6</v>
+        <f t="shared" ref="AQ32" si="5">SUM(C32:AP32)</f>
+        <v>1</v>
       </c>
       <c r="AR32" s="48"/>
       <c r="AS32" s="48"/>
     </row>
     <row r="33" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B33" s="19">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C33" s="64"/>
       <c r="D33" s="57"/>
@@ -3402,12 +3402,8 @@
       <c r="M33" s="57"/>
       <c r="N33" s="57"/>
       <c r="O33" s="57"/>
-      <c r="P33" s="57">
-        <v>2</v>
-      </c>
-      <c r="Q33" s="57">
-        <v>4</v>
-      </c>
+      <c r="P33" s="57"/>
+      <c r="Q33" s="57"/>
       <c r="R33" s="57"/>
       <c r="S33" s="57"/>
       <c r="T33" s="57"/>
@@ -3435,14 +3431,14 @@
       <c r="AP33" s="59"/>
       <c r="AQ33" s="19">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AR33" s="48"/>
       <c r="AS33" s="48"/>
     </row>
     <row r="34" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="B34" s="19">
         <v>8</v>
@@ -3476,7 +3472,9 @@
       <c r="AA34" s="57"/>
       <c r="AB34" s="58"/>
       <c r="AC34" s="57"/>
-      <c r="AD34" s="57"/>
+      <c r="AD34" s="57">
+        <v>2</v>
+      </c>
       <c r="AE34" s="57"/>
       <c r="AF34" s="57"/>
       <c r="AG34" s="57"/>
@@ -3490,18 +3488,18 @@
       <c r="AO34" s="57"/>
       <c r="AP34" s="59"/>
       <c r="AQ34" s="19">
-        <f t="shared" ref="AQ34" si="5">SUM(C34:AP34)</f>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
       <c r="AR34" s="48"/>
       <c r="AS34" s="48"/>
     </row>
     <row r="35" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="B35" s="19">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C35" s="64"/>
       <c r="D35" s="57"/>
@@ -3525,11 +3523,15 @@
       <c r="V35" s="57"/>
       <c r="W35" s="57"/>
       <c r="X35" s="57"/>
-      <c r="Y35" s="57"/>
+      <c r="Y35" s="57">
+        <v>1</v>
+      </c>
       <c r="Z35" s="57"/>
       <c r="AA35" s="57"/>
       <c r="AB35" s="58"/>
-      <c r="AC35" s="57"/>
+      <c r="AC35" s="57">
+        <v>2</v>
+      </c>
       <c r="AD35" s="57"/>
       <c r="AE35" s="57"/>
       <c r="AF35" s="57"/>
@@ -3545,14 +3547,14 @@
       <c r="AP35" s="59"/>
       <c r="AQ35" s="19">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR35" s="48"/>
       <c r="AS35" s="48"/>
     </row>
     <row r="36" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
-        <v>86</v>
+      <c r="A36" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="B36" s="19">
         <v>8</v>
@@ -3564,7 +3566,9 @@
       <c r="G36" s="57"/>
       <c r="H36" s="57"/>
       <c r="I36" s="57"/>
-      <c r="J36" s="57"/>
+      <c r="J36" s="57">
+        <v>2</v>
+      </c>
       <c r="K36" s="57"/>
       <c r="L36" s="57"/>
       <c r="M36" s="57"/>
@@ -3578,17 +3582,13 @@
       <c r="U36" s="58"/>
       <c r="V36" s="57"/>
       <c r="W36" s="57"/>
-      <c r="X36" s="57">
-        <v>1</v>
-      </c>
+      <c r="X36" s="57"/>
       <c r="Y36" s="57"/>
       <c r="Z36" s="57"/>
       <c r="AA36" s="57"/>
       <c r="AB36" s="58"/>
       <c r="AC36" s="57"/>
-      <c r="AD36" s="57">
-        <v>2</v>
-      </c>
+      <c r="AD36" s="57"/>
       <c r="AE36" s="57"/>
       <c r="AF36" s="57"/>
       <c r="AG36" s="57"/>
@@ -3603,17 +3603,17 @@
       <c r="AP36" s="59"/>
       <c r="AQ36" s="19">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AR36" s="48"/>
       <c r="AS36" s="48"/>
     </row>
     <row r="37" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B37" s="19">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C37" s="64"/>
       <c r="D37" s="57"/>
@@ -3637,15 +3637,13 @@
       <c r="V37" s="57"/>
       <c r="W37" s="57"/>
       <c r="X37" s="57"/>
-      <c r="Y37" s="57">
-        <v>1</v>
-      </c>
-      <c r="Z37" s="57"/>
+      <c r="Y37" s="57"/>
+      <c r="Z37" s="57">
+        <v>1</v>
+      </c>
       <c r="AA37" s="57"/>
       <c r="AB37" s="58"/>
-      <c r="AC37" s="57">
-        <v>2</v>
-      </c>
+      <c r="AC37" s="57"/>
       <c r="AD37" s="57"/>
       <c r="AE37" s="57"/>
       <c r="AF37" s="57"/>
@@ -3661,17 +3659,17 @@
       <c r="AP37" s="59"/>
       <c r="AQ37" s="19">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AR37" s="48"/>
       <c r="AS37" s="48"/>
     </row>
-    <row r="38" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
-        <v>56</v>
+    <row r="38" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="B38" s="19">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C38" s="64"/>
       <c r="D38" s="57"/>
@@ -3720,198 +3718,286 @@
       <c r="AR38" s="48"/>
       <c r="AS38" s="48"/>
     </row>
-    <row r="39" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="19">
-        <v>16</v>
-      </c>
-      <c r="C39" s="64"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="57"/>
-      <c r="G39" s="57"/>
-      <c r="H39" s="57"/>
-      <c r="I39" s="57"/>
-      <c r="J39" s="57"/>
-      <c r="K39" s="57"/>
-      <c r="L39" s="57"/>
-      <c r="M39" s="57"/>
-      <c r="N39" s="57"/>
-      <c r="O39" s="57"/>
-      <c r="P39" s="57"/>
-      <c r="Q39" s="57"/>
-      <c r="R39" s="57"/>
-      <c r="S39" s="57"/>
-      <c r="T39" s="57"/>
-      <c r="U39" s="58"/>
-      <c r="V39" s="57"/>
-      <c r="W39" s="57"/>
-      <c r="X39" s="57"/>
-      <c r="Y39" s="57"/>
-      <c r="Z39" s="57">
-        <v>1</v>
-      </c>
-      <c r="AA39" s="57"/>
-      <c r="AB39" s="58"/>
-      <c r="AC39" s="57"/>
-      <c r="AD39" s="57"/>
-      <c r="AE39" s="57"/>
-      <c r="AF39" s="57"/>
-      <c r="AG39" s="57"/>
-      <c r="AH39" s="57"/>
-      <c r="AI39" s="57"/>
-      <c r="AJ39" s="57"/>
-      <c r="AK39" s="57"/>
-      <c r="AL39" s="57"/>
-      <c r="AM39" s="57"/>
-      <c r="AN39" s="57"/>
-      <c r="AO39" s="57"/>
-      <c r="AP39" s="59"/>
-      <c r="AQ39" s="19">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
+    <row r="39" spans="1:72" s="39" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="40"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
+      <c r="K39" s="38"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="38"/>
+      <c r="N39" s="38"/>
+      <c r="O39" s="38"/>
+      <c r="P39" s="38"/>
+      <c r="Q39" s="38"/>
+      <c r="R39" s="38"/>
+      <c r="S39" s="38"/>
+      <c r="T39" s="38"/>
+      <c r="U39" s="38"/>
+      <c r="V39" s="38"/>
+      <c r="W39" s="38"/>
+      <c r="X39" s="38"/>
+      <c r="Y39" s="38"/>
+      <c r="Z39" s="38"/>
+      <c r="AA39" s="38"/>
+      <c r="AB39" s="38"/>
+      <c r="AC39" s="38"/>
+      <c r="AD39" s="38"/>
+      <c r="AE39" s="38"/>
+      <c r="AF39" s="38"/>
+      <c r="AG39" s="38"/>
+      <c r="AH39" s="38"/>
+      <c r="AI39" s="38"/>
+      <c r="AJ39" s="38"/>
+      <c r="AK39" s="38"/>
+      <c r="AL39" s="38"/>
+      <c r="AM39" s="38"/>
+      <c r="AN39" s="38"/>
+      <c r="AO39" s="38"/>
+      <c r="AP39" s="51"/>
+      <c r="AQ39" s="53"/>
       <c r="AR39" s="48"/>
       <c r="AS39" s="48"/>
+      <c r="AT39" s="2"/>
+      <c r="AU39" s="2"/>
+      <c r="AV39" s="2"/>
+      <c r="AW39" s="2"/>
+      <c r="AX39" s="2"/>
+      <c r="AY39"/>
+      <c r="AZ39"/>
+      <c r="BA39"/>
+      <c r="BB39"/>
+      <c r="BC39"/>
+      <c r="BD39"/>
+      <c r="BE39"/>
+      <c r="BF39"/>
+      <c r="BG39"/>
+      <c r="BH39"/>
+      <c r="BI39"/>
+      <c r="BJ39"/>
+      <c r="BK39"/>
+      <c r="BL39"/>
+      <c r="BM39"/>
+      <c r="BN39"/>
+      <c r="BO39"/>
+      <c r="BP39"/>
+      <c r="BQ39"/>
+      <c r="BR39"/>
+      <c r="BS39"/>
+      <c r="BT39"/>
     </row>
-    <row r="40" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>55</v>
+    <row r="40" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="B40" s="19">
-        <v>10</v>
-      </c>
-      <c r="C40" s="64"/>
-      <c r="D40" s="57"/>
-      <c r="E40" s="57"/>
-      <c r="F40" s="57"/>
-      <c r="G40" s="57"/>
-      <c r="H40" s="57"/>
-      <c r="I40" s="57"/>
-      <c r="J40" s="57"/>
-      <c r="K40" s="57"/>
-      <c r="L40" s="57"/>
-      <c r="M40" s="57"/>
-      <c r="N40" s="57"/>
-      <c r="O40" s="57"/>
-      <c r="P40" s="57"/>
-      <c r="Q40" s="57"/>
-      <c r="R40" s="57"/>
-      <c r="S40" s="57"/>
-      <c r="T40" s="57"/>
-      <c r="U40" s="58"/>
-      <c r="V40" s="57"/>
-      <c r="W40" s="57"/>
-      <c r="X40" s="57"/>
-      <c r="Y40" s="57"/>
-      <c r="Z40" s="57"/>
-      <c r="AA40" s="57"/>
-      <c r="AB40" s="58"/>
-      <c r="AC40" s="57"/>
-      <c r="AD40" s="57"/>
-      <c r="AE40" s="57"/>
-      <c r="AF40" s="57"/>
-      <c r="AG40" s="57"/>
-      <c r="AH40" s="57"/>
-      <c r="AI40" s="57"/>
-      <c r="AJ40" s="57"/>
-      <c r="AK40" s="57"/>
-      <c r="AL40" s="57"/>
-      <c r="AM40" s="57"/>
-      <c r="AN40" s="57"/>
-      <c r="AO40" s="57"/>
-      <c r="AP40" s="59"/>
-      <c r="AQ40" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <v>68</v>
+      </c>
+      <c r="C40" s="4">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1</v>
+      </c>
+      <c r="H40" s="1">
+        <v>1</v>
+      </c>
+      <c r="I40" s="1">
+        <v>1</v>
+      </c>
+      <c r="J40" s="1">
+        <v>1</v>
+      </c>
+      <c r="K40" s="1">
+        <v>1</v>
+      </c>
+      <c r="L40" s="1">
+        <v>1</v>
+      </c>
+      <c r="M40" s="1">
+        <v>1</v>
+      </c>
+      <c r="N40" s="1">
+        <v>1</v>
+      </c>
+      <c r="O40" s="1">
+        <v>1</v>
+      </c>
+      <c r="P40" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>1</v>
+      </c>
+      <c r="R40" s="1">
+        <v>3</v>
+      </c>
+      <c r="S40" s="1">
+        <v>1</v>
+      </c>
+      <c r="T40" s="1">
+        <v>1</v>
+      </c>
+      <c r="U40" s="38"/>
+      <c r="V40" s="1">
+        <v>1</v>
+      </c>
+      <c r="W40" s="1">
+        <v>1</v>
+      </c>
+      <c r="X40" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y40" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB40" s="38"/>
+      <c r="AC40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG40" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK40" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL40" s="1">
+        <v>7</v>
+      </c>
+      <c r="AM40" s="1">
+        <v>7</v>
+      </c>
+      <c r="AN40" s="1">
+        <v>7</v>
+      </c>
+      <c r="AO40" s="1">
+        <v>7</v>
+      </c>
+      <c r="AP40" s="1">
+        <v>3</v>
+      </c>
+      <c r="AQ40" s="12">
+        <f>SUM(C40:AP40)</f>
+        <v>73</v>
       </c>
       <c r="AR40" s="48"/>
       <c r="AS40" s="48"/>
     </row>
-    <row r="41" spans="1:72" s="39" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="38"/>
-      <c r="J41" s="38"/>
-      <c r="K41" s="38"/>
-      <c r="L41" s="38"/>
-      <c r="M41" s="38"/>
-      <c r="N41" s="38"/>
-      <c r="O41" s="38"/>
-      <c r="P41" s="38"/>
-      <c r="Q41" s="38"/>
-      <c r="R41" s="38"/>
-      <c r="S41" s="38"/>
-      <c r="T41" s="38"/>
+    <row r="41" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="19">
+        <v>68</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1">
+        <v>4</v>
+      </c>
+      <c r="L41" s="1">
+        <v>4</v>
+      </c>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1">
+        <v>4</v>
+      </c>
+      <c r="P41" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>2</v>
+      </c>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
       <c r="U41" s="38"/>
-      <c r="V41" s="38"/>
-      <c r="W41" s="38"/>
-      <c r="X41" s="38"/>
-      <c r="Y41" s="38"/>
-      <c r="Z41" s="38"/>
-      <c r="AA41" s="38"/>
+      <c r="V41" s="1">
+        <v>2</v>
+      </c>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+      <c r="Y41" s="1"/>
+      <c r="Z41" s="1"/>
+      <c r="AA41" s="1">
+        <v>3</v>
+      </c>
       <c r="AB41" s="38"/>
-      <c r="AC41" s="38"/>
-      <c r="AD41" s="38"/>
-      <c r="AE41" s="38"/>
-      <c r="AF41" s="38"/>
-      <c r="AG41" s="38"/>
-      <c r="AH41" s="38"/>
-      <c r="AI41" s="38"/>
-      <c r="AJ41" s="38"/>
-      <c r="AK41" s="38"/>
-      <c r="AL41" s="38"/>
-      <c r="AM41" s="38"/>
-      <c r="AN41" s="38"/>
-      <c r="AO41" s="38"/>
-      <c r="AP41" s="51"/>
-      <c r="AQ41" s="53"/>
+      <c r="AC41" s="1"/>
+      <c r="AD41" s="1"/>
+      <c r="AE41" s="1"/>
+      <c r="AF41" s="1"/>
+      <c r="AG41" s="1"/>
+      <c r="AH41" s="1"/>
+      <c r="AI41" s="1"/>
+      <c r="AJ41" s="1"/>
+      <c r="AK41" s="1"/>
+      <c r="AL41" s="1"/>
+      <c r="AM41" s="1"/>
+      <c r="AN41" s="1"/>
+      <c r="AO41" s="1"/>
+      <c r="AP41" s="1"/>
+      <c r="AQ41" s="12">
+        <f>SUM(C41:AP41)</f>
+        <v>23</v>
+      </c>
       <c r="AR41" s="48"/>
       <c r="AS41" s="48"/>
-      <c r="AT41" s="2"/>
-      <c r="AU41" s="2"/>
-      <c r="AV41" s="2"/>
-      <c r="AW41" s="2"/>
-      <c r="AX41" s="2"/>
-      <c r="AY41"/>
-      <c r="AZ41"/>
-      <c r="BA41"/>
-      <c r="BB41"/>
-      <c r="BC41"/>
-      <c r="BD41"/>
-      <c r="BE41"/>
-      <c r="BF41"/>
-      <c r="BG41"/>
-      <c r="BH41"/>
-      <c r="BI41"/>
-      <c r="BJ41"/>
-      <c r="BK41"/>
-      <c r="BL41"/>
-      <c r="BM41"/>
-      <c r="BN41"/>
-      <c r="BO41"/>
-      <c r="BP41"/>
-      <c r="BQ41"/>
-      <c r="BR41"/>
-      <c r="BS41"/>
-      <c r="BT41"/>
     </row>
-    <row r="42" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B42" s="19">
-        <v>68</v>
+    <row r="42" spans="1:72" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" s="20">
+        <v>38</v>
       </c>
       <c r="C42" s="4">
         <v>1</v>
@@ -3959,7 +4045,7 @@
         <v>1</v>
       </c>
       <c r="R42" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S42" s="1">
         <v>1</v>
@@ -4012,455 +4098,257 @@
         <v>1</v>
       </c>
       <c r="AK42" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AL42" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AM42" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AN42" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AO42" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AP42" s="1">
-        <v>3</v>
-      </c>
-      <c r="AQ42" s="12">
+        <v>1</v>
+      </c>
+      <c r="AQ42" s="13">
         <f>SUM(C42:AP42)</f>
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="AR42" s="48"/>
       <c r="AS42" s="48"/>
     </row>
     <row r="43" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
-        <v>77</v>
+      <c r="A43" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="B43" s="19">
-        <v>68</v>
-      </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1">
-        <v>4</v>
-      </c>
-      <c r="L43" s="1">
-        <v>4</v>
-      </c>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1">
-        <v>4</v>
-      </c>
-      <c r="P43" s="1">
-        <v>4</v>
-      </c>
-      <c r="Q43" s="1">
+        <v>10</v>
+      </c>
+      <c r="C43" s="64"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="57"/>
+      <c r="J43" s="57"/>
+      <c r="K43" s="57"/>
+      <c r="L43" s="57"/>
+      <c r="M43" s="57"/>
+      <c r="N43" s="57"/>
+      <c r="O43" s="57"/>
+      <c r="P43" s="57"/>
+      <c r="Q43" s="57"/>
+      <c r="R43" s="57"/>
+      <c r="S43" s="57"/>
+      <c r="T43" s="57"/>
+      <c r="U43" s="58"/>
+      <c r="V43" s="57">
         <v>2</v>
       </c>
-      <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
-      <c r="T43" s="1"/>
-      <c r="U43" s="38"/>
-      <c r="V43" s="1">
+      <c r="W43" s="57"/>
+      <c r="X43" s="57"/>
+      <c r="Y43" s="57"/>
+      <c r="Z43" s="57"/>
+      <c r="AA43" s="57"/>
+      <c r="AB43" s="58"/>
+      <c r="AC43" s="57"/>
+      <c r="AD43" s="57"/>
+      <c r="AE43" s="57"/>
+      <c r="AF43" s="57"/>
+      <c r="AG43" s="57"/>
+      <c r="AH43" s="57"/>
+      <c r="AI43" s="57"/>
+      <c r="AJ43" s="57"/>
+      <c r="AK43" s="57"/>
+      <c r="AL43" s="57"/>
+      <c r="AM43" s="57"/>
+      <c r="AN43" s="57"/>
+      <c r="AO43" s="57"/>
+      <c r="AP43" s="59"/>
+      <c r="AQ43" s="19">
+        <f t="shared" ref="AQ43" si="6">SUM(C43:AP43)</f>
         <v>2</v>
-      </c>
-      <c r="W43" s="1"/>
-      <c r="X43" s="1"/>
-      <c r="Y43" s="1"/>
-      <c r="Z43" s="1"/>
-      <c r="AA43" s="1">
-        <v>3</v>
-      </c>
-      <c r="AB43" s="38"/>
-      <c r="AC43" s="1"/>
-      <c r="AD43" s="1"/>
-      <c r="AE43" s="1"/>
-      <c r="AF43" s="1"/>
-      <c r="AG43" s="1"/>
-      <c r="AH43" s="1"/>
-      <c r="AI43" s="1"/>
-      <c r="AJ43" s="1"/>
-      <c r="AK43" s="1"/>
-      <c r="AL43" s="1"/>
-      <c r="AM43" s="1"/>
-      <c r="AN43" s="1"/>
-      <c r="AO43" s="1"/>
-      <c r="AP43" s="1"/>
-      <c r="AQ43" s="12">
-        <f>SUM(C43:AP43)</f>
-        <v>23</v>
       </c>
       <c r="AR43" s="48"/>
       <c r="AS43" s="48"/>
     </row>
-    <row r="44" spans="1:72" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B44" s="20">
-        <v>38</v>
-      </c>
-      <c r="C44" s="4">
-        <v>1</v>
-      </c>
-      <c r="D44" s="1">
-        <v>1</v>
-      </c>
-      <c r="E44" s="1">
-        <v>1</v>
-      </c>
-      <c r="F44" s="1">
-        <v>1</v>
-      </c>
-      <c r="G44" s="1">
-        <v>1</v>
-      </c>
-      <c r="H44" s="1">
-        <v>1</v>
-      </c>
-      <c r="I44" s="1">
-        <v>1</v>
-      </c>
-      <c r="J44" s="1">
-        <v>1</v>
-      </c>
-      <c r="K44" s="1">
-        <v>1</v>
-      </c>
-      <c r="L44" s="1">
-        <v>1</v>
-      </c>
-      <c r="M44" s="1">
-        <v>1</v>
-      </c>
-      <c r="N44" s="1">
-        <v>1</v>
-      </c>
-      <c r="O44" s="1">
-        <v>1</v>
-      </c>
-      <c r="P44" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q44" s="1">
-        <v>1</v>
-      </c>
-      <c r="R44" s="1">
-        <v>1</v>
-      </c>
-      <c r="S44" s="1">
-        <v>1</v>
-      </c>
-      <c r="T44" s="1">
-        <v>1</v>
-      </c>
-      <c r="U44" s="38"/>
-      <c r="V44" s="1">
-        <v>1</v>
-      </c>
-      <c r="W44" s="1">
-        <v>1</v>
-      </c>
-      <c r="X44" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y44" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB44" s="38"/>
-      <c r="AC44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AI44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AL44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AM44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AN44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AO44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AP44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ44" s="13">
-        <f>SUM(C44:AP44)</f>
-        <v>38</v>
+    <row r="44" spans="1:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="21">
+        <f t="shared" ref="B44:AP44" si="7">SUM(B4:B42)</f>
+        <v>364</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="D44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="F44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="H44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="I44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="K44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="M44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="O44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="P44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="R44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="T44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="U44">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V44" s="21">
+        <f>SUM(V4:V43)</f>
+        <v>8</v>
+      </c>
+      <c r="W44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="X44">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="Y44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="Z44">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AA44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AB44">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AD44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AE44">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AF44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AG44">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AH44" s="21">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="AI44">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="AJ44" s="21">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="AK44" s="21">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="AL44">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AM44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AN44">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AO44" s="21">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AP44">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="AQ44" s="21">
+        <f>SUM(AQ4:AQ42)</f>
+        <v>278</v>
       </c>
       <c r="AR44" s="48"/>
       <c r="AS44" s="48"/>
-    </row>
-    <row r="45" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45" s="19">
-        <v>10</v>
-      </c>
-      <c r="C45" s="64"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="57"/>
-      <c r="G45" s="57"/>
-      <c r="H45" s="57"/>
-      <c r="I45" s="57"/>
-      <c r="J45" s="57"/>
-      <c r="K45" s="57"/>
-      <c r="L45" s="57"/>
-      <c r="M45" s="57"/>
-      <c r="N45" s="57"/>
-      <c r="O45" s="57"/>
-      <c r="P45" s="57"/>
-      <c r="Q45" s="57"/>
-      <c r="R45" s="57"/>
-      <c r="S45" s="57"/>
-      <c r="T45" s="57"/>
-      <c r="U45" s="58"/>
-      <c r="V45" s="57">
-        <v>2</v>
-      </c>
-      <c r="W45" s="57"/>
-      <c r="X45" s="57"/>
-      <c r="Y45" s="57"/>
-      <c r="Z45" s="57"/>
-      <c r="AA45" s="57"/>
-      <c r="AB45" s="58"/>
-      <c r="AC45" s="57"/>
-      <c r="AD45" s="57"/>
-      <c r="AE45" s="57"/>
-      <c r="AF45" s="57"/>
-      <c r="AG45" s="57"/>
-      <c r="AH45" s="57"/>
-      <c r="AI45" s="57"/>
-      <c r="AJ45" s="57"/>
-      <c r="AK45" s="57"/>
-      <c r="AL45" s="57"/>
-      <c r="AM45" s="57"/>
-      <c r="AN45" s="57"/>
-      <c r="AO45" s="57"/>
-      <c r="AP45" s="59"/>
-      <c r="AQ45" s="19">
-        <f t="shared" ref="AQ45" si="6">SUM(C45:AP45)</f>
-        <v>2</v>
-      </c>
-      <c r="AR45" s="48"/>
-      <c r="AS45" s="48"/>
-    </row>
-    <row r="46" spans="1:72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="21">
-        <f t="shared" ref="B46:AP46" si="7">SUM(B4:B44)</f>
-        <v>376</v>
-      </c>
-      <c r="C46">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="D46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="F46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="G46">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="H46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="I46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="K46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="L46">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="M46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="N46">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="O46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="P46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="Q46">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="R46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="S46">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="T46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="U46">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="V46" s="21">
-        <f>SUM(V4:V45)</f>
-        <v>8</v>
-      </c>
-      <c r="W46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="X46">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="Y46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="Z46">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="AA46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="AB46">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AC46" s="21">
-        <f t="shared" si="7"/>
-        <v>10</v>
-      </c>
-      <c r="AD46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="AE46">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="AF46" s="21">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="AG46">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="AH46" s="21">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="AI46">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="AJ46" s="21">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="AK46" s="21">
-        <f t="shared" si="7"/>
-        <v>6</v>
-      </c>
-      <c r="AL46">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="AM46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="AN46">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="AO46" s="21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="AP46">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="AQ46" s="21">
-        <f>SUM(AQ4:AQ44)</f>
-        <v>268</v>
-      </c>
-      <c r="AR46" s="48"/>
-      <c r="AS46" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4470,41 +4358,36 @@
     <mergeCell ref="AR6:AR7"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:N8 C10:N10 C12:N12">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="25">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="25">
       <formula>LEN(TRIM(C5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:AP8 C33:AP33 C10:AP10 C12:AP13 C44:AP44 C20:AP20 C35:AP42 C22:AP28 C30:AP31">
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="C5:AP8 C31:AP31 C10:AP10 C12:AP13 C42:AP42 C33:AP40 C28:AP29 C20:AP26">
+    <cfRule type="cellIs" dxfId="19" priority="24" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+  <conditionalFormatting sqref="B44">
+    <cfRule type="cellIs" dxfId="18" priority="23" operator="equal">
       <formula>300</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46:AP46">
-    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
+  <conditionalFormatting sqref="C44:AP44">
+    <cfRule type="cellIs" dxfId="17" priority="22" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AP46">
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+  <conditionalFormatting sqref="AP44">
+    <cfRule type="cellIs" dxfId="16" priority="21" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:AP4">
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="20" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:AP21">
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThanOrEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32:AP32">
+  <conditionalFormatting sqref="C30:AP30">
     <cfRule type="cellIs" dxfId="14" priority="15" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
@@ -4529,7 +4412,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43:AP43">
+  <conditionalFormatting sqref="C41:AP41">
     <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
@@ -4554,7 +4437,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C45:AP45">
+  <conditionalFormatting sqref="C43:AP43">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
@@ -4569,12 +4452,12 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34:AP34">
+  <conditionalFormatting sqref="C32:AP32">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:AP29">
+  <conditionalFormatting sqref="C27:AP27">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
@@ -4586,7 +4469,7 @@
     <oddHeader>&amp;L&amp;F&amp;CDDC'App&amp;RJonathan Borel-Jaquet</oddHeader>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="AQ44 AQ30 AQ20 AQ13" formulaRange="1"/>
+    <ignoredError sqref="AQ42 AQ28 AQ20 AQ13" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Generate and send ICS file for appointment
</commit_message>
<xml_diff>
--- a/documentation/planning/planning_effectif_travail_de_diplome.xlsx
+++ b/documentation/planning/planning_effectif_travail_de_diplome.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bj-travail-diplome-2021\documentation\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C9554B-0848-4DBE-938D-48810898F50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -291,7 +290,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\.m"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -1201,15 +1200,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BT44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF35" sqref="AF35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2446,7 +2445,9 @@
       <c r="AE17" s="57"/>
       <c r="AF17" s="57"/>
       <c r="AG17" s="57"/>
-      <c r="AH17" s="57"/>
+      <c r="AH17" s="57">
+        <v>2</v>
+      </c>
       <c r="AI17" s="57"/>
       <c r="AJ17" s="57"/>
       <c r="AK17" s="57"/>
@@ -2457,7 +2458,7 @@
       <c r="AP17" s="59"/>
       <c r="AQ17" s="19">
         <f>SUM(C17:AP17)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AR17" s="48"/>
       <c r="AS17" s="48"/>
@@ -3062,7 +3063,9 @@
         <v>4</v>
       </c>
       <c r="AG27" s="57"/>
-      <c r="AH27" s="57"/>
+      <c r="AH27" s="57">
+        <v>2</v>
+      </c>
       <c r="AI27" s="57"/>
       <c r="AJ27" s="57"/>
       <c r="AK27" s="57"/>
@@ -3073,7 +3076,7 @@
       <c r="AP27" s="59"/>
       <c r="AQ27" s="19">
         <f t="shared" ref="AQ27" si="2">SUM(C27:AP27)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AR27" s="48"/>
       <c r="AS27" s="48"/>
@@ -3702,7 +3705,9 @@
       <c r="AE38" s="57"/>
       <c r="AF38" s="57"/>
       <c r="AG38" s="57"/>
-      <c r="AH38" s="57"/>
+      <c r="AH38" s="57">
+        <v>2</v>
+      </c>
       <c r="AI38" s="57"/>
       <c r="AJ38" s="57"/>
       <c r="AK38" s="57"/>
@@ -3713,7 +3718,7 @@
       <c r="AP38" s="59"/>
       <c r="AQ38" s="19">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR38" s="48"/>
       <c r="AS38" s="48"/>
@@ -4309,7 +4314,7 @@
       </c>
       <c r="AH44" s="21">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AI44">
         <f t="shared" si="7"/>
@@ -4345,7 +4350,7 @@
       </c>
       <c r="AQ44" s="21">
         <f>SUM(AQ4:AQ42)</f>
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="AR44" s="48"/>
       <c r="AS44" s="48"/>

</xml_diff>